<commit_message>
Fixed subnet deploy logic
</commit_message>
<xml_diff>
--- a/PowerShell/ParametersFileBuilder_3-Spoke.xlsx
+++ b/PowerShell/ParametersFileBuilder_3-Spoke.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mark.bakunas\Documents\GitHub\Azure-HubSpoke\PowerShell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978C28EA-4A59-47C2-B41C-9AF37265FA78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3D7725-3B28-4271-8F53-20F728B505B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="1080" windowWidth="21600" windowHeight="13650" xr2:uid="{74A5C2AD-3876-4989-8818-24030CBF60E7}"/>
+    <workbookView xWindow="-25545" yWindow="1065" windowWidth="21600" windowHeight="13650" activeTab="2" xr2:uid="{74A5C2AD-3876-4989-8818-24030CBF60E7}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="4" r:id="rId1"/>
@@ -33,28 +33,28 @@
     <definedName name="calcHubSubnetJumpHostsAddressSpace">ParametersFile!$B$12</definedName>
     <definedName name="dcAdminsAadGroupObjectId">General!$B$10</definedName>
     <definedName name="deployOptions_List">Lists!$E$2:$E$3</definedName>
-    <definedName name="hubSubnet1AddressSpace">Hub!$C$8</definedName>
-    <definedName name="hubSubnet1Deploy">Hub!$D$8</definedName>
-    <definedName name="hubSubnet1Name">Hub!$B$8</definedName>
-    <definedName name="hubSubnet2AddressSpace">Hub!$C$9</definedName>
-    <definedName name="hubSubnet2Deploy">Hub!$D$9</definedName>
-    <definedName name="hubSubnet2Name">Hub!$B$9</definedName>
-    <definedName name="hubSubnet3AddressSpace">Hub!$C$10</definedName>
-    <definedName name="hubSubnet3Deploy">Hub!$D$10</definedName>
-    <definedName name="hubSubnet3Name">Hub!$B$10</definedName>
-    <definedName name="hubSubnet4AddressSpace">Hub!$C$11</definedName>
-    <definedName name="hubSubnet4Deploy">Hub!$D$11</definedName>
-    <definedName name="hubSubnet4Name">Hub!$B$11</definedName>
-    <definedName name="hubSubnetBastionAddressSpace">Hub!$C$5</definedName>
-    <definedName name="hubSubnetBastionDeploy">Hub!$D$5</definedName>
-    <definedName name="hubSubnetDcAddressSpace">Hub!$C$6</definedName>
-    <definedName name="hubSubnetDcName">Hub!$B$6</definedName>
-    <definedName name="hubSubnetFirewallAddressSpace">Hub!$C$4</definedName>
-    <definedName name="hubSubnetFirewallDeploy">Hub!$D$4</definedName>
-    <definedName name="hubSubnetGatewayAddressSpace">Hub!$C$3</definedName>
-    <definedName name="hubSubnetJumpHostsAddressSpace">Hub!$C$7</definedName>
-    <definedName name="hubSubnetJumpHostsDeploy">Hub!$D$7</definedName>
-    <definedName name="hubSubnetJumpHostsName">Hub!$B$7</definedName>
+    <definedName name="hubSubnet1AddressSpace">Hub!$C$9</definedName>
+    <definedName name="hubSubnet1Deploy">Hub!$D$9</definedName>
+    <definedName name="hubSubnet1Name">Hub!$B$9</definedName>
+    <definedName name="hubSubnet2AddressSpace">Hub!$C$10</definedName>
+    <definedName name="hubSubnet2Deploy">Hub!$D$10</definedName>
+    <definedName name="hubSubnet2Name">Hub!$B$10</definedName>
+    <definedName name="hubSubnet3AddressSpace">Hub!$C$11</definedName>
+    <definedName name="hubSubnet3Deploy">Hub!$D$11</definedName>
+    <definedName name="hubSubnet3Name">Hub!$B$11</definedName>
+    <definedName name="hubSubnet4AddressSpace">Hub!$C$12</definedName>
+    <definedName name="hubSubnet4Deploy">Hub!$D$12</definedName>
+    <definedName name="hubSubnet4Name">Hub!$B$12</definedName>
+    <definedName name="hubSubnetBastionAddressSpace">Hub!$C$6</definedName>
+    <definedName name="hubSubnetBastionDeploy">Hub!$D$6</definedName>
+    <definedName name="hubSubnetDcAddressSpace">Hub!$C$7</definedName>
+    <definedName name="hubSubnetDcName">Hub!$B$7</definedName>
+    <definedName name="hubSubnetFirewallAddressSpace">Hub!$C$5</definedName>
+    <definedName name="hubSubnetFirewallDeploy">Hub!$D$5</definedName>
+    <definedName name="hubSubnetGatewayAddressSpace">Hub!$C$4</definedName>
+    <definedName name="hubSubnetJumpHostsAddressSpace">Hub!$C$8</definedName>
+    <definedName name="hubSubnetJumpHostsDeploy">Hub!$D$8</definedName>
+    <definedName name="hubSubnetJumpHostsName">Hub!$B$8</definedName>
     <definedName name="hubVnetAddressSpace">Hub!$C$2</definedName>
     <definedName name="hubVnetName">Hub!$B$2</definedName>
     <definedName name="routeTableName">General!$B$7</definedName>
@@ -70,6 +70,7 @@
     <definedName name="spokeSubnetAppGwName">ParametersFile!$B$24</definedName>
     <definedName name="spokeSubnetBastionAddressSpace">ParametersFile!$B$23</definedName>
     <definedName name="spokeSubnetUniqueness_List">Lists!$G$2:$G$3</definedName>
+    <definedName name="spokeVmContributorsRoleAssignmentID">ParametersFile!$B$32</definedName>
     <definedName name="spokeVnetAddressSpace">ParametersFile!$B$21</definedName>
     <definedName name="spokeVnetName">ParametersFile!$B$20</definedName>
     <definedName name="vnetDdosProtectionLevel">General!$B$4</definedName>
@@ -96,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="135">
   <si>
     <t>Name</t>
   </si>
@@ -455,9 +456,6 @@
     <t>High</t>
   </si>
   <si>
-    <t>Azure AD goup object ID</t>
-  </si>
-  <si>
     <t>Deploy</t>
   </si>
   <si>
@@ -498,6 +496,12 @@
   </si>
   <si>
     <t>Common</t>
+  </si>
+  <si>
+    <t>spokeVmContributorsRoleAssignmentID</t>
+  </si>
+  <si>
+    <t>Azure AD group object ID</t>
   </si>
 </sst>
 </file>
@@ -560,7 +564,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
@@ -569,6 +573,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -892,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27806494-5F45-4C9A-ADBE-3476E1448E75}">
   <dimension ref="A2:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,7 +954,7 @@
         <v>102</v>
       </c>
       <c r="B9" t="s">
-        <v>119</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -994,7 +1000,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC352499-16C6-4142-B6A7-FED4572A9C0C}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -1027,143 +1033,133 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
+    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>120</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>120</v>
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>120</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" t="s">
-        <v>120</v>
+        <v>20</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" t="s">
-        <v>120</v>
+        <v>25</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" t="s">
-        <v>120</v>
+        <v>26</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D11" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" t="s">
-        <v>50</v>
+      <c r="D12" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
+      </c>
+      <c r="D14" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1171,27 +1167,27 @@
         <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>2</v>
+        <v>59</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1202,10 +1198,10 @@
         <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1216,10 +1212,10 @@
         <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1230,10 +1226,10 @@
         <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1244,10 +1240,10 @@
         <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1255,19 +1251,33 @@
         <v>45</v>
       </c>
       <c r="B21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" t="s">
         <v>60</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>103</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D5 D7:D11" xr:uid="{D9354EF7-27D1-4C1F-B57B-07A789DEC96E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D6 D8:D12" xr:uid="{D9354EF7-27D1-4C1F-B57B-07A789DEC96E}">
       <formula1>deployOptions_List</formula1>
     </dataValidation>
   </dataValidations>
@@ -1278,7 +1288,203 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4D3422A-C2D2-42AC-9F3F-3909382DD971}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="5" width="37.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" t="str">
+        <f>IF(B2 &lt;&gt; "", _xlfn.CONCAT(CHAR(34), B2, "/", C2, CHAR(34)), _xlfn.CONCAT("""", """"))</f>
+        <v>""</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D8 D10:D11" xr:uid="{0CD32938-FC7D-4A2D-89DA-FA2CAD0BA150}">
+      <formula1>deployOptions_List</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E11" xr:uid="{EBB888DC-D06B-428F-9A6F-3A30046B1109}">
+      <formula1>spokeSubnetUniqueness_List</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A2061D0-44C8-4698-9DEF-5B9D4440337D}">
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -1307,11 +1513,15 @@
       <c r="A2" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="D2" t="str">
         <f>IF(B2 &lt;&gt; "", _xlfn.CONCAT(CHAR(34), B2, "/", C2, CHAR(34)), _xlfn.CONCAT("""", """"))</f>
-        <v>""</v>
+        <v>"c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02"</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1327,122 +1537,117 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>133</v>
-      </c>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>36</v>
+        <v>80</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>133</v>
+        <v>119</v>
+      </c>
+      <c r="E7" t="str">
+        <f>Spoke1!E7</f>
+        <v>Common</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>133</v>
+        <v>81</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E8" t="str">
+        <f>Spoke1!E8</f>
+        <v>Common</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>133</v>
+        <v>82</v>
+      </c>
+      <c r="E9" t="str">
+        <f>Spoke1!E9</f>
+        <v>Common</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E10" t="str">
+        <f>Spoke1!E10</f>
+        <v>Common</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" t="s">
-        <v>50</v>
+      <c r="C11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E11" t="str">
+        <f>Spoke1!E11</f>
+        <v>Common</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
+      </c>
+      <c r="D13" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
         <v>48</v>
@@ -1451,16 +1656,27 @@
         <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>52</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D7 D9:D10" xr:uid="{0CD32938-FC7D-4A2D-89DA-FA2CAD0BA150}">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D8 D10:D11" xr:uid="{01786FD6-A133-4CF7-BD55-62BA227952C7}">
       <formula1>deployOptions_List</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E10" xr:uid="{EBB888DC-D06B-428F-9A6F-3A30046B1109}">
-      <formula1>spokeSubnetUniqueness_List</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1468,9 +1684,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A2061D0-44C8-4698-9DEF-5B9D4440337D}">
-  <dimension ref="A1:E14"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91E1F8B8-C0E8-4047-B16B-8927D4C4193D}">
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -1500,14 +1716,14 @@
         <v>41</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="D2" t="str">
         <f>IF(B2 &lt;&gt; "", _xlfn.CONCAT(CHAR(34), B2, "/", C2, CHAR(34)), _xlfn.CONCAT("""", """"))</f>
-        <v>"c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02"</v>
+        <v>"16936380-29b0-4326-8f6b-db86da154736/HubSpoke-03"</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1523,39 +1739,25 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E6" t="str">
-        <f>Spoke1!E6</f>
-        <v>Common</v>
-      </c>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E7" t="str">
         <f>Spoke1!E7</f>
@@ -1564,13 +1766,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>82</v>
+        <v>111</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>119</v>
       </c>
       <c r="E8" t="str">
         <f>Spoke1!E8</f>
@@ -1579,16 +1784,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="E9" t="str">
         <f>Spoke1!E9</f>
@@ -1597,53 +1799,57 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>84</v>
+        <v>113</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E10" t="str">
         <f>Spoke1!E10</f>
         <v>Common</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" t="s">
-        <v>50</v>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E11" t="str">
+        <f>Spoke1!E11</f>
+        <v>Common</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>85</v>
+        <v>58</v>
+      </c>
+      <c r="D13" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
         <v>48</v>
@@ -1652,210 +1858,26 @@
         <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>86</v>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D7 D9:D10" xr:uid="{01786FD6-A133-4CF7-BD55-62BA227952C7}">
-      <formula1>deployOptions_List</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91E1F8B8-C0E8-4047-B16B-8927D4C4193D}">
-  <dimension ref="A1:E14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="5" width="37.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D2" t="str">
-        <f>IF(B2 &lt;&gt; "", _xlfn.CONCAT(CHAR(34), B2, "/", C2, CHAR(34)), _xlfn.CONCAT("""", """"))</f>
-        <v>"16936380-29b0-4326-8f6b-db86da154736/HubSpoke-03"</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E6" t="str">
-        <f>Spoke1!E6</f>
-        <v>Common</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E7" t="str">
-        <f>Spoke1!E7</f>
-        <v>Common</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E8" t="str">
-        <f>Spoke1!E8</f>
-        <v>Common</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E9" t="str">
-        <f>Spoke1!E9</f>
-        <v>Common</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E10" t="str">
-        <f>Spoke1!E10</f>
-        <v>Common</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D7 D9:D10" xr:uid="{18BEFA5C-BFE0-444D-A090-ECC81E547311}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D8 D10:D11" xr:uid="{18BEFA5C-BFE0-444D-A090-ECC81E547311}">
       <formula1>deployOptions_List</formula1>
     </dataValidation>
   </dataValidations>
@@ -1866,10 +1888,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E5F0421-4CC3-4847-AE8E-9E8CD1C6E8C6}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1884,7 +1906,7 @@
       </c>
       <c r="B1" s="4" t="str">
         <f>_xlfn.CONCAT(B3, ",", B4, ",", B5,  B6)</f>
-        <v>{"$schema":"https://schema.management.azure.com/schemas/2019-04-01/deploymentParameters.json#","contentVersion":"1.0.0.0","parameters":{"assetLocationURI": {"value":"https://raw.githubusercontent.com/mbakunas/Azure-HubSpoke/master/"},"vnetDdosProtectionLevel": {"value":"Basic"},"vnetDdosProtectionPlanName": {"value":"DDOS-Plan-01"},"vnetNsgSecurityLevel": {"value":"Medium"},"routeTableName": {"value":"RouteTable-01"},"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"10.0.0.64/26"},"hubSubnetBastionAddressSpace": {"value":"10.0.0.128/26"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},"dcVmContributorsAadGroupId": {"value":"17ba8236-a5e8-4173-8ce9-c69b17743ac2"},"dcVmContributorsRoleAssignmentID": {"value":["184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"]},"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01","Spoke-Dev-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16","10.3.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["","c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02","16936380-29b0-4326-8f6b-db86da154736/HubSpoke-03"]},"spokeSubnetBastionAddressSpace": {"value":["0.0.0.0/0","0.0.0.0/0","0.0.0.0/0"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25","10.3.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24","10.3.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24","10.3.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24","10.3.3.0/24"]}}}</v>
+        <v>{"$schema":"https://schema.management.azure.com/schemas/2019-04-01/deploymentParameters.json#","contentVersion":"1.0.0.0","parameters":{"assetLocationURI": {"value":"https://raw.githubusercontent.com/mbakunas/Azure-HubSpoke/master/"},"vnetDdosProtectionLevel": {"value":"Basic"},"vnetDdosProtectionPlanName": {"value":"DDOS-Plan-01"},"vnetNsgSecurityLevel": {"value":"Medium"},"routeTableName": {"value":"RouteTable-01"},"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetBastionAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},"dcVmContributorsAadGroupId": {"value":"17ba8236-a5e8-4173-8ce9-c69b17743ac2"},"dcVmContributorsRoleAssignmentID": {"value":["184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"]},"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01","Spoke-Dev-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16","10.3.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["","c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02","16936380-29b0-4326-8f6b-db86da154736/HubSpoke-03"]},"spokeSubnetBastionAddressSpace": {"value":["0.0.0.0/0"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25","10.3.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24","10.3.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24","10.3.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24","10.3.3.0/24"]},"spokeVmContributorsAadGroupId": {"value":["c2ecad99-6ed7-4e11-8acc-0fa0262a2c69"]},"spokeVmContributorsRoleAssignmentID": {"value":["5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6","b2b76710-60c9-4826-b864-272c7c115806"]}}}</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1929,9 +1951,9 @@
 CHAR(34), "hubSubnet4Name", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), hubSubnet4Name, CHAR(34), "},",
 CHAR(34), "hubSubnet4AddressSpace", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), calcHubSubnet4AddressSpace, CHAR(34), "},",
 CHAR(34), "dcVmContributorsAadGroupId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), dcAdminsAadGroupObjectId, CHAR(34), "},",
-CHAR(34), "dcVmContributorsRoleAssignmentID", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", CHAR(34), Hub!D14, CHAR(34), ",", CHAR(34),Hub!D15, CHAR(34), "]}",
+CHAR(34), "dcVmContributorsRoleAssignmentID", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", CHAR(34), Hub!D15, CHAR(34), ",", CHAR(34),Hub!D16, CHAR(34), "]}",
 )</f>
-        <v>"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"10.0.0.64/26"},"hubSubnetBastionAddressSpace": {"value":"10.0.0.128/26"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},"dcVmContributorsAadGroupId": {"value":"17ba8236-a5e8-4173-8ce9-c69b17743ac2"},"dcVmContributorsRoleAssignmentID": {"value":["184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"]}</v>
+        <v>"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetBastionAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},"dcVmContributorsAadGroupId": {"value":"17ba8236-a5e8-4173-8ce9-c69b17743ac2"},"dcVmContributorsRoleAssignmentID": {"value":["184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"]}</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1951,9 +1973,11 @@
 CHAR(34), "spokeSubnet2Name", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", spokeSubnet2Name,"]},",
 CHAR(34), "spokeSubnet2AddressSpace", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", spokeSubnet2AddressSpace,"]},",
 CHAR(34), "spokeSubnet3Name", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", spokeSubnet3Name,"]},",
-CHAR(34), "spokeSubnet3AddressSpace", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", spokeSubnet3AddressSpace,"]}"
+CHAR(34), "spokeSubnet3AddressSpace", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", spokeSubnet3AddressSpace,"]},",
+CHAR(34), "spokeVmContributorsAadGroupId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", CHAR(34), appTeamsAadGroupObjectId, CHAR(34), "]},",
+CHAR(34), "spokeVmContributorsRoleAssignmentID", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", spokeVmContributorsRoleAssignmentID,"]}"
 )</f>
-        <v>"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01","Spoke-Dev-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16","10.3.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["","c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02","16936380-29b0-4326-8f6b-db86da154736/HubSpoke-03"]},"spokeSubnetBastionAddressSpace": {"value":["0.0.0.0/0","0.0.0.0/0","0.0.0.0/0"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25","10.3.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24","10.3.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24","10.3.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24","10.3.3.0/24"]}</v>
+        <v>"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01","Spoke-Dev-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16","10.3.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["","c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02","16936380-29b0-4326-8f6b-db86da154736/HubSpoke-03"]},"spokeSubnetBastionAddressSpace": {"value":["0.0.0.0/0"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25","10.3.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24","10.3.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24","10.3.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24","10.3.3.0/24"]},"spokeVmContributorsAadGroupId": {"value":["c2ecad99-6ed7-4e11-8acc-0fa0262a2c69"]},"spokeVmContributorsRoleAssignmentID": {"value":["5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6","b2b76710-60c9-4826-b864-272c7c115806"]}</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1968,32 +1992,32 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B9" s="3"/>
+      <c r="A9" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" s="7"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B10" t="str">
         <f>IF(hubSubnetFirewallDeploy = "Deploy", hubSubnetFirewallAddressSpace, "0.0.0.0/0")</f>
-        <v>10.0.0.64/26</v>
+        <v>0.0.0.0/0</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B11" t="str">
         <f>IF(hubSubnetBastionDeploy = "Deploy", hubSubnetBastionAddressSpace, "0.0.0.0/0")</f>
-        <v>10.0.0.128/26</v>
+        <v>0.0.0.0/0</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B12" t="str">
         <f>IF(hubSubnetJumpHostsDeploy = "Deploy", hubSubnetJumpHostsAddressSpace, "0.0.0.0/0")</f>
@@ -2002,7 +2026,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B13" t="str">
         <f>IF(hubSubnet1Deploy = "Deploy", hubSubnet1AddressSpace, "0.0.0.0/0")</f>
@@ -2011,7 +2035,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B14" t="str">
         <f>IF(
@@ -2023,7 +2047,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B15" t="str">
         <f>IF(
@@ -2035,7 +2059,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B16" t="str">
         <f>IF(
@@ -2046,10 +2070,10 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B19" s="3"/>
+      <c r="B19" s="7"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -2083,20 +2107,20 @@
         <v>94</v>
       </c>
       <c r="B23" t="str">
-        <f>_xlfn.CONCAT(
-IF(Spoke1!$D$6 = "Don't Deploy", """" &amp; "0.0.0.0/0" &amp; """" &amp; ",", """" &amp; Spoke1!$C$6 &amp; """" &amp; ","),
-IF(
-OR(AND(Spoke1!$E$6 = "Common", Spoke1!$D$6 = "Don't Deploy"), AND(Spoke1!$E$6 = "Unique", Spoke2!$D$6 = "Don't Deploy")),
-"""" &amp; "0.0.0.0/0" &amp; """" &amp; ",",
-"""" &amp; Spoke2!$C$6 &amp; """" &amp; ","
-),
-IF(
-OR(AND(Spoke1!$E$6 = "Common", Spoke1!$D$6 = "Don't Deploy"), AND(Spoke1!$E$6 = "Unique", Spoke3!$D$6 = "Don't Deploy")),
-"""" &amp; "0.0.0.0/0" &amp; """",
-"""" &amp; Spoke3!$C$6 &amp; """"
+        <f>IF(
+Spoke1!$E$7 = "Common",
+IF(Spoke1!$D$7 = "Don't Deploy", """"  &amp; "0.0.0.0/0" &amp; """", """" &amp;  Spoke1!$C$7 &amp; """" &amp; "," &amp;   """" &amp; Spoke2!$C$7  &amp; """" &amp; "," &amp;   """" &amp; Spoke3!$C$7),
+_xlfn.CONCAT(
+"""",
+IF(Spoke1!$D$7 = "Don't Deploy", "0.0.0.0/0", Spoke1!$C$7),
+"""", ",", """",
+IF(Spoke2!$D$7 = "Don't Deploy", "0.0.0.0/0", Spoke2!$C$7),
+"""", ",", """",
+IF(Spoke3!$D$7 = "Don't Deploy", "0.0.0.0/0", Spoke3!$C$7),
+""""
 )
 )</f>
-        <v>"0.0.0.0/0","0.0.0.0/0","0.0.0.0/0"</v>
+        <v>"0.0.0.0/0"</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2105,9 +2129,9 @@
       </c>
       <c r="B24" s="5" t="str">
         <f>IF(
-Spoke1!$E$7 = "Common",
-"""" &amp; Spoke1!$B$7 &amp; """",
-_xlfn.CONCAT("""", Spoke1!$B$7, """", ",", """", Spoke2!$B$7, """", ",", """", Spoke3!$B$7, """")
+Spoke1!$E$8 = "Common",
+"""" &amp; Spoke1!$B$8 &amp; """",
+_xlfn.CONCAT("""", Spoke1!$B$8, """", ",", """", Spoke2!$B$8, """", ",", """", Spoke3!$B$8, """")
 )</f>
         <v>"AppGW"</v>
       </c>
@@ -2116,18 +2140,18 @@
       <c r="A25" t="s">
         <v>93</v>
       </c>
-      <c r="B25" t="str">
-        <f>_xlfn.CONCAT(
-IF(Spoke1!$D$7 = "Don't Deploy", """" &amp; "0.0.0.0/0" &amp; """" &amp; ",", """" &amp; Spoke1!$C$7 &amp; """" &amp; ","),
-IF(
-OR(AND(Spoke1!$E$7 = "Common", Spoke1!$D$7 = "Don't Deploy"), AND(Spoke1!$E$7 = "Unique", Spoke2!$D$7 = "Don't Deploy")),
-"""" &amp; "0.0.0.0/0" &amp; """" &amp; ",",
-"""" &amp; Spoke2!$C$7 &amp; """" &amp; ","
-),
-IF(
-OR(AND(Spoke1!$E$7 = "Common", Spoke1!$D$7 = "Don't Deploy"), AND(Spoke1!$E$7 = "Unique", Spoke3!$D$7 = "Don't Deploy")),
-"""" &amp; "0.0.0.0/0" &amp; """",
-"""" &amp; Spoke3!$C$7 &amp; """"
+      <c r="B25" s="3" t="str">
+        <f>IF(
+Spoke1!$E$8 = "Common",
+IF(Spoke1!$D$8 = "Don't Deploy", """"  &amp; "0.0.0.0/0" &amp; """", """" &amp;  Spoke1!$C$8 &amp; """" &amp; "," &amp;   """" &amp; Spoke2!$C$8  &amp; """" &amp; "," &amp;   """" &amp; Spoke3!$C$8 &amp; """"),
+_xlfn.CONCAT(
+"""",
+IF(Spoke1!$D$8 = "Don't Deploy", "0.0.0.0/0", Spoke1!$C$8),
+"""", ",", """",
+IF(Spoke2!$D$8 = "Don't Deploy", "0.0.0.0/0", Spoke2!$C$8),
+"""", ",", """",
+IF(Spoke3!$D$8 = "Don't Deploy", "0.0.0.0/0", Spoke3!$C$8),
+""""
 )
 )</f>
         <v>"10.1.0.128/25","10.2.0.128/25","10.3.0.128/25"</v>
@@ -2139,9 +2163,9 @@
       </c>
       <c r="B26" s="5" t="str">
         <f>IF(
-Spoke1!$E$7 = "Common",
-"""" &amp; Spoke1!$B$8 &amp; """",
-_xlfn.CONCAT("""", Spoke1!$B$8, """", ",", """", Spoke2!$B$8, """", ",", """", Spoke3!$B$8, """")
+Spoke1!$E$8 = "Common",
+"""" &amp; Spoke1!$B$9 &amp; """",
+_xlfn.CONCAT("""", Spoke1!$B$9, """", ",", """", Spoke2!$B$9, """", ",", """", Spoke3!$B$9, """")
 )</f>
         <v>"Subnet1"</v>
       </c>
@@ -2150,18 +2174,18 @@
       <c r="A27" t="s">
         <v>97</v>
       </c>
-      <c r="B27" t="str">
-        <f>_xlfn.CONCAT(
-IF(Spoke1!$D$8 = "Don't Deploy", """" &amp; "0.0.0.0/0" &amp; """" &amp; ",", """" &amp; Spoke1!$C$8 &amp; """" &amp; ","),
-IF(
-OR(AND(Spoke1!$E$8 = "Common", Spoke1!$D$8 = "Don't Deploy"), AND(Spoke1!$E$8 = "Unique", Spoke2!$D$8 = "Don't Deploy")),
-"""" &amp; "0.0.0.0/0" &amp; """" &amp; ",",
- """" &amp; Spoke2!$C$8 &amp; """" &amp; ","
-),
-IF(
-OR(AND(Spoke1!$E$8 = "Common", Spoke1!$D$8 = "Don't Deploy"), AND(Spoke1!$E$8 = "Unique", Spoke3!$D$8 = "Don't Deploy")),
-"""" &amp; "0.0.0.0/0" &amp; """",
- """" &amp; Spoke3!$C$8 &amp; """"
+      <c r="B27" s="3" t="str">
+        <f>IF(
+Spoke1!$E$9 = "Common",
+IF(Spoke1!$D$9 = "Don't Deploy", """"  &amp; "0.0.0.0/0" &amp; """", """" &amp;  Spoke1!$C$9 &amp; """" &amp; "," &amp;   """" &amp; Spoke2!$C$9  &amp; """" &amp; "," &amp;   """" &amp; Spoke3!$C$9 &amp; """"),
+_xlfn.CONCAT(
+"""",
+IF(Spoke1!$D$9 = "Don't Deploy", "0.0.0.0/0", Spoke1!$C$9),
+"""", ",", """",
+IF(Spoke2!$D$9 = "Don't Deploy", "0.0.0.0/0", Spoke2!$C$9),
+"""", ",", """",
+IF(Spoke3!$D$9 = "Don't Deploy", "0.0.0.0/0", Spoke3!$C$9),
+""""
 )
 )</f>
         <v>"10.1.1.0/24","10.2.1.0/24","10.3.1.0/24"</v>
@@ -2173,9 +2197,9 @@
       </c>
       <c r="B28" s="5" t="str">
         <f>IF(
-Spoke1!$E$9 = "Common",
-"""" &amp; Spoke1!$B$9 &amp; """",
-_xlfn.CONCAT("""", Spoke1!$B$9, """", ",", """", Spoke2!$B$9, """", ",", """", Spoke3!$B$9, """")
+Spoke1!$E$10 = "Common",
+"""" &amp; Spoke1!$B$10 &amp; """",
+_xlfn.CONCAT("""", Spoke1!$B$10, """", ",", """", Spoke2!$B$10, """", ",", """", Spoke3!$B$10, """")
 )</f>
         <v>"Subnet2"</v>
       </c>
@@ -2184,18 +2208,18 @@
       <c r="A29" t="s">
         <v>99</v>
       </c>
-      <c r="B29" t="str">
-        <f>_xlfn.CONCAT(
-IF(Spoke1!$D$9 = "Don't Deploy", """" &amp; "0.0.0.0/0" &amp; """" &amp; ",", """" &amp; Spoke1!$C$9 &amp; """" &amp; ","),
-IF(
-OR(AND(Spoke1!$E$9 = "Common", Spoke1!$D$9 = "Don't Deploy"), AND(Spoke1!$E$9 = "Unique", Spoke2!$D$9 = "Don't Deploy")),
-"""" &amp; "0.0.0.0/0" &amp; """" &amp; ",",
- """" &amp; Spoke2!$C$9 &amp; """" &amp; ","
-),
-IF(
-OR(AND(Spoke1!$E$9 = "Common", Spoke1!$D$9 = "Don't Deploy"), AND(Spoke1!$E$9 = "Unique", Spoke3!$D$9 = "Don't Deploy")),
-"""" &amp; "0.0.0.0/0" &amp; """",
- """" &amp; Spoke3!$C$9 &amp; """"
+      <c r="B29" s="3" t="str">
+        <f>IF(
+Spoke1!$E$10 = "Common",
+IF(Spoke1!$D$10 = "Don't Deploy", """"  &amp; "0.0.0.0/0" &amp; """", """" &amp;  Spoke1!$C$10 &amp; """" &amp; "," &amp;   """" &amp; Spoke2!$C$10  &amp; """" &amp; "," &amp;   """" &amp; Spoke3!$C$10 &amp; """"),
+_xlfn.CONCAT(
+"""",
+IF(Spoke1!$D$10 = "Don't Deploy", "0.0.0.0/0", Spoke1!$C$10),
+"""", ",", """",
+IF(Spoke2!$D$10 = "Don't Deploy", "0.0.0.0/0", Spoke2!$C$10),
+"""", ",", """",
+IF(Spoke3!$D$10 = "Don't Deploy", "0.0.0.0/0", Spoke3!$C$10),
+""""
 )
 )</f>
         <v>"10.1.2.0/24","10.2.2.0/24","10.3.2.0/24"</v>
@@ -2207,9 +2231,9 @@
       </c>
       <c r="B30" s="5" t="str">
         <f>IF(
-Spoke1!$E$7 = "Common",
-"""" &amp; Spoke1!$B$10 &amp; """",
-_xlfn.CONCAT("""", Spoke1!$B$10, """", ",", """", Spoke2!$B$10, """", ",", """", Spoke3!$B$10, """")
+Spoke1!$E$8 = "Common",
+"""" &amp; Spoke1!$B$11 &amp; """",
+_xlfn.CONCAT("""", Spoke1!$B$11, """", ",", """", Spoke2!$B$11, """", ",", """", Spoke3!$B$11, """")
 )</f>
         <v>"Subnet3"</v>
       </c>
@@ -2218,21 +2242,34 @@
       <c r="A31" t="s">
         <v>101</v>
       </c>
-      <c r="B31" t="str">
-        <f>_xlfn.CONCAT(
-IF(Spoke1!$D$10 = "Don't Deploy", """" &amp; "0.0.0.0/0" &amp; """" &amp; ",", """" &amp; Spoke1!$C$10 &amp; """" &amp; ","),
-IF(
-OR(AND(Spoke1!$E$10 = "Common", Spoke1!$D$10 = "Don't Deploy"), AND(Spoke1!$E$10 = "Unique", Spoke2!$D$10 = "Don't Deploy")),
-"""" &amp; "0.0.0.0/0" &amp; """" &amp; ",",
- """" &amp; Spoke2!$C$10 &amp; """" &amp; ","
-),
-IF(
-OR(AND(Spoke1!$E$10 = "Common", Spoke1!$D$10 = "Don't Deploy"), AND(Spoke1!$E$10 = "Unique", Spoke3!$D$10 = "Don't Deploy")),
-"""" &amp; "0.0.0.0/0" &amp; """",
- """" &amp; Spoke3!$C$10 &amp; """"
+      <c r="B31" s="3" t="str">
+        <f>IF(
+Spoke1!$E$11 = "Common",
+IF(OR(Spoke1!$D$11 = "Don't Deploy", Spoke1!$D$10 = "Don't Deploy"),
+ """"  &amp; "0.0.0.0/0" &amp; """",
+ """" &amp;  IF(Spoke1!$D$10 = "Don't Deploy", "0.0.0.0/0", Spoke1!$C$11) &amp; """" &amp; "," &amp;
+"""" &amp; IF(Spoke2!$D$10 = "Don't Deploy", "0.0.0.0/0", Spoke2!$C$11)  &amp; """" &amp; "," &amp;
+"""" &amp; IF(Spoke3!$D$10 = "Don't Deploy", "0.0.0.0/0", Spoke3!$C$11) &amp; """"),
+_xlfn.CONCAT(
+"""",
+IF(OR(Spoke1!$D$11 = "Don't Deploy", Spoke1!$D$10 = "Don't Deploy"), "0.0.0.0/0", Spoke1!$C$11),
+"""", ",", """",
+IF(OR(Spoke2!$D$11 = "Don't Deploy", Spoke2!$D$10 = "Don't Deploy"), "0.0.0.0/0", Spoke2!$C$11),
+"""", ",", """",
+IF(OR(Spoke3!$D$11 = "Don't Deploy", Spoke3!$D$10 = "Don't Deploy"), "0.0.0.0/0",  Spoke3!$C$11),
+""""
 )
 )</f>
         <v>"10.1.3.0/24","10.2.3.0/24","10.3.3.0/24"</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>133</v>
+      </c>
+      <c r="B32" t="str">
+        <f>_xlfn.CONCAT("""",Spoke1!D15,"""",",","""",Spoke2!D15,"""",",","""",Spoke3!D15,"""")</f>
+        <v>"5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6","b2b76710-60c9-4826-b864-272c7c115806"</v>
       </c>
     </row>
   </sheetData>
@@ -2269,10 +2306,10 @@
         <v>31</v>
       </c>
       <c r="E1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2283,10 +2320,10 @@
         <v>117</v>
       </c>
       <c r="E2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2297,10 +2334,10 @@
         <v>70</v>
       </c>
       <c r="E3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Renamed AAD group parameters/variables for clarity
</commit_message>
<xml_diff>
--- a/PowerShell/ParametersFileBuilder_3-Spoke.xlsx
+++ b/PowerShell/ParametersFileBuilder_3-Spoke.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mark.bakunas\Documents\GitHub\Azure-HubSpoke\PowerShell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3D7725-3B28-4271-8F53-20F728B505B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5102CD9F-C413-4641-9B83-8788DF4427F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25545" yWindow="1065" windowWidth="21600" windowHeight="13650" activeTab="2" xr2:uid="{74A5C2AD-3876-4989-8818-24030CBF60E7}"/>
+    <workbookView xWindow="-25545" yWindow="1065" windowWidth="21600" windowHeight="13650" activeTab="1" xr2:uid="{74A5C2AD-3876-4989-8818-24030CBF60E7}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="4" r:id="rId1"/>
@@ -1002,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC352499-16C6-4142-B6A7-FED4572A9C0C}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1290,7 +1290,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4D3422A-C2D2-42AC-9F3F-3909382DD971}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1890,8 +1890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E5F0421-4CC3-4847-AE8E-9E8CD1C6E8C6}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1906,7 +1906,7 @@
       </c>
       <c r="B1" s="4" t="str">
         <f>_xlfn.CONCAT(B3, ",", B4, ",", B5,  B6)</f>
-        <v>{"$schema":"https://schema.management.azure.com/schemas/2019-04-01/deploymentParameters.json#","contentVersion":"1.0.0.0","parameters":{"assetLocationURI": {"value":"https://raw.githubusercontent.com/mbakunas/Azure-HubSpoke/master/"},"vnetDdosProtectionLevel": {"value":"Basic"},"vnetDdosProtectionPlanName": {"value":"DDOS-Plan-01"},"vnetNsgSecurityLevel": {"value":"Medium"},"routeTableName": {"value":"RouteTable-01"},"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetBastionAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},"dcVmContributorsAadGroupId": {"value":"17ba8236-a5e8-4173-8ce9-c69b17743ac2"},"dcVmContributorsRoleAssignmentID": {"value":["184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"]},"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01","Spoke-Dev-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16","10.3.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["","c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02","16936380-29b0-4326-8f6b-db86da154736/HubSpoke-03"]},"spokeSubnetBastionAddressSpace": {"value":["0.0.0.0/0"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25","10.3.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24","10.3.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24","10.3.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24","10.3.3.0/24"]},"spokeVmContributorsAadGroupId": {"value":["c2ecad99-6ed7-4e11-8acc-0fa0262a2c69"]},"spokeVmContributorsRoleAssignmentID": {"value":["5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6","b2b76710-60c9-4826-b864-272c7c115806"]}}}</v>
+        <v>{"$schema":"https://schema.management.azure.com/schemas/2019-04-01/deploymentParameters.json#","contentVersion":"1.0.0.0","parameters":{"assetLocationURI": {"value":"https://raw.githubusercontent.com/mbakunas/Azure-HubSpoke/master/"},"vnetDdosProtectionLevel": {"value":"Basic"},"vnetDdosProtectionPlanName": {"value":"DDOS-Plan-01"},"vnetNsgSecurityLevel": {"value":"Medium"},"routeTableName": {"value":"RouteTable-01"},"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetBastionAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},"dcAdminsAadGroupId": {"value":"17ba8236-a5e8-4173-8ce9-c69b17743ac2"},"dcVmContributorsRoleAssignmentID": {"value":["184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"]},"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01","Spoke-Dev-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16","10.3.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["","c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02","16936380-29b0-4326-8f6b-db86da154736/HubSpoke-03"]},"spokeSubnetBastionAddressSpace": {"value":["0.0.0.0/0"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25","10.3.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24","10.3.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24","10.3.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24","10.3.3.0/24"]},"appTeamsAadGroupId": {"value":["c2ecad99-6ed7-4e11-8acc-0fa0262a2c69"]},"spokeVmContributorsRoleAssignmentID": {"value":["5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6","b2b76710-60c9-4826-b864-272c7c115806"]}}}</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1950,10 +1950,10 @@
 CHAR(34), "hubSubnet3AddressSpace", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), calcHubSubnet3AddressSpace, CHAR(34), "},",
 CHAR(34), "hubSubnet4Name", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), hubSubnet4Name, CHAR(34), "},",
 CHAR(34), "hubSubnet4AddressSpace", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), calcHubSubnet4AddressSpace, CHAR(34), "},",
-CHAR(34), "dcVmContributorsAadGroupId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), dcAdminsAadGroupObjectId, CHAR(34), "},",
+CHAR(34), "dcAdminsAadGroupId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), dcAdminsAadGroupObjectId, CHAR(34), "},",
 CHAR(34), "dcVmContributorsRoleAssignmentID", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", CHAR(34), Hub!D15, CHAR(34), ",", CHAR(34),Hub!D16, CHAR(34), "]}",
 )</f>
-        <v>"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetBastionAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},"dcVmContributorsAadGroupId": {"value":"17ba8236-a5e8-4173-8ce9-c69b17743ac2"},"dcVmContributorsRoleAssignmentID": {"value":["184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"]}</v>
+        <v>"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetBastionAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},"dcAdminsAadGroupId": {"value":"17ba8236-a5e8-4173-8ce9-c69b17743ac2"},"dcVmContributorsRoleAssignmentID": {"value":["184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"]}</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1974,10 +1974,10 @@
 CHAR(34), "spokeSubnet2AddressSpace", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", spokeSubnet2AddressSpace,"]},",
 CHAR(34), "spokeSubnet3Name", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", spokeSubnet3Name,"]},",
 CHAR(34), "spokeSubnet3AddressSpace", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", spokeSubnet3AddressSpace,"]},",
-CHAR(34), "spokeVmContributorsAadGroupId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", CHAR(34), appTeamsAadGroupObjectId, CHAR(34), "]},",
+CHAR(34), "appTeamsAadGroupId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", CHAR(34), appTeamsAadGroupObjectId, CHAR(34), "]},",
 CHAR(34), "spokeVmContributorsRoleAssignmentID", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", spokeVmContributorsRoleAssignmentID,"]}"
 )</f>
-        <v>"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01","Spoke-Dev-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16","10.3.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["","c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02","16936380-29b0-4326-8f6b-db86da154736/HubSpoke-03"]},"spokeSubnetBastionAddressSpace": {"value":["0.0.0.0/0"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25","10.3.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24","10.3.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24","10.3.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24","10.3.3.0/24"]},"spokeVmContributorsAadGroupId": {"value":["c2ecad99-6ed7-4e11-8acc-0fa0262a2c69"]},"spokeVmContributorsRoleAssignmentID": {"value":["5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6","b2b76710-60c9-4826-b864-272c7c115806"]}</v>
+        <v>"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01","Spoke-Dev-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16","10.3.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["","c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02","16936380-29b0-4326-8f6b-db86da154736/HubSpoke-03"]},"spokeSubnetBastionAddressSpace": {"value":["0.0.0.0/0"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25","10.3.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24","10.3.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24","10.3.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24","10.3.3.0/24"]},"appTeamsAadGroupId": {"value":["c2ecad99-6ed7-4e11-8acc-0fa0262a2c69"]},"spokeVmContributorsRoleAssignmentID": {"value":["5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6","b2b76710-60c9-4826-b864-272c7c115806"]}</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added additional RBAC to hub subnets
</commit_message>
<xml_diff>
--- a/PowerShell/ParametersFileBuilder_3-Spoke.xlsx
+++ b/PowerShell/ParametersFileBuilder_3-Spoke.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mark.bakunas\Documents\GitHub\Azure-HubSpoke\PowerShell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5102CD9F-C413-4641-9B83-8788DF4427F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F17D6B-93F2-403D-9577-C849D12162DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25545" yWindow="1065" windowWidth="21600" windowHeight="13650" activeTab="1" xr2:uid="{74A5C2AD-3876-4989-8818-24030CBF60E7}"/>
+    <workbookView xWindow="-25545" yWindow="1065" windowWidth="21600" windowHeight="13650" xr2:uid="{74A5C2AD-3876-4989-8818-24030CBF60E7}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="4" r:id="rId1"/>
@@ -32,6 +32,7 @@
     <definedName name="calcHubSubnetBastionAddressSpace">ParametersFile!$B$11</definedName>
     <definedName name="calcHubSubnetJumpHostsAddressSpace">ParametersFile!$B$12</definedName>
     <definedName name="dcAdminsAadGroupObjectId">General!$B$10</definedName>
+    <definedName name="dcVmContributorsRoleAssignmentID">ParametersFile!$B$19</definedName>
     <definedName name="deployOptions_List">Lists!$E$2:$E$3</definedName>
     <definedName name="hubSubnet1AddressSpace">Hub!$C$9</definedName>
     <definedName name="hubSubnet1Deploy">Hub!$D$9</definedName>
@@ -55,24 +56,25 @@
     <definedName name="hubSubnetJumpHostsAddressSpace">Hub!$C$8</definedName>
     <definedName name="hubSubnetJumpHostsDeploy">Hub!$D$8</definedName>
     <definedName name="hubSubnetJumpHostsName">Hub!$B$8</definedName>
+    <definedName name="hubSubnetVmContRoleAssignmantId">ParametersFile!$B$20</definedName>
     <definedName name="hubVnetAddressSpace">Hub!$C$2</definedName>
     <definedName name="hubVnetName">Hub!$B$2</definedName>
     <definedName name="routeTableName">General!$B$7</definedName>
     <definedName name="serverTeamAadGroupObjectId">General!$B$11</definedName>
-    <definedName name="spokeDeploySubscriptionResourceGroup">ParametersFile!$B$22</definedName>
-    <definedName name="spokeSubnet1AddressSpace">ParametersFile!$B$27</definedName>
-    <definedName name="spokeSubnet1Name">ParametersFile!$B$26</definedName>
-    <definedName name="spokeSubnet2AddressSpace">ParametersFile!$B$29</definedName>
-    <definedName name="spokeSubnet2Name">ParametersFile!$B$28</definedName>
-    <definedName name="spokeSubnet3AddressSpace">ParametersFile!$B$31</definedName>
-    <definedName name="spokeSubnet3Name">ParametersFile!$B$30</definedName>
-    <definedName name="spokeSubnetAppGwAddressSpace">ParametersFile!$B$25</definedName>
-    <definedName name="spokeSubnetAppGwName">ParametersFile!$B$24</definedName>
-    <definedName name="spokeSubnetBastionAddressSpace">ParametersFile!$B$23</definedName>
+    <definedName name="spokeDeploySubscriptionResourceGroup">ParametersFile!$B$26</definedName>
+    <definedName name="spokeSubnet1AddressSpace">ParametersFile!$B$31</definedName>
+    <definedName name="spokeSubnet1Name">ParametersFile!$B$30</definedName>
+    <definedName name="spokeSubnet2AddressSpace">ParametersFile!$B$33</definedName>
+    <definedName name="spokeSubnet2Name">ParametersFile!$B$32</definedName>
+    <definedName name="spokeSubnet3AddressSpace">ParametersFile!$B$35</definedName>
+    <definedName name="spokeSubnet3Name">ParametersFile!$B$34</definedName>
+    <definedName name="spokeSubnetAppGwAddressSpace">ParametersFile!$B$29</definedName>
+    <definedName name="spokeSubnetAppGwName">ParametersFile!$B$28</definedName>
+    <definedName name="spokeSubnetBastionAddressSpace">ParametersFile!$B$27</definedName>
     <definedName name="spokeSubnetUniqueness_List">Lists!$G$2:$G$3</definedName>
-    <definedName name="spokeVmContributorsRoleAssignmentID">ParametersFile!$B$32</definedName>
-    <definedName name="spokeVnetAddressSpace">ParametersFile!$B$21</definedName>
-    <definedName name="spokeVnetName">ParametersFile!$B$20</definedName>
+    <definedName name="spokeVmContributorsRoleAssignmentID">ParametersFile!$B$36</definedName>
+    <definedName name="spokeVnetAddressSpace">ParametersFile!$B$25</definedName>
+    <definedName name="spokeVnetName">ParametersFile!$B$24</definedName>
     <definedName name="vnetDdosProtectionLevel">General!$B$4</definedName>
     <definedName name="vnetDdosProtectionLevel_List">Lists!$A$2:$A$4</definedName>
     <definedName name="vnetDdosProtectionPlanName">General!$B$5</definedName>
@@ -97,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="142">
   <si>
     <t>Name</t>
   </si>
@@ -234,12 +236,6 @@
     <t>RBAC</t>
   </si>
   <si>
-    <t>Server Team</t>
-  </si>
-  <si>
-    <t>App Teams</t>
-  </si>
-  <si>
     <t>Role</t>
   </si>
   <si>
@@ -264,9 +260,6 @@
     <t>17ba8236-a5e8-4173-8ce9-c69b17743ac2</t>
   </si>
   <si>
-    <t>DC Admins</t>
-  </si>
-  <si>
     <t>184540aa-dae3-42cd-a5aa-0f1c34c17d98</t>
   </si>
   <si>
@@ -502,6 +495,36 @@
   </si>
   <si>
     <t>Azure AD group object ID</t>
+  </si>
+  <si>
+    <t>Sopke VM contributors</t>
+  </si>
+  <si>
+    <t>Spoke VM contrib.</t>
+  </si>
+  <si>
+    <t>HubDCs subnet VM contributors</t>
+  </si>
+  <si>
+    <t>Hub other subnets VM contributors</t>
+  </si>
+  <si>
+    <t>DCs subnet VM contrib</t>
+  </si>
+  <si>
+    <t>other subnets VM contrib</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>hubSubnetVmContRoleAssignmantId</t>
+  </si>
+  <si>
+    <t>dcVmContributorsRoleAssignmentID</t>
+  </si>
+  <si>
+    <t>Hub Array Values</t>
   </si>
 </sst>
 </file>
@@ -564,7 +587,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
@@ -574,6 +597,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
@@ -898,23 +922,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27806494-5F45-4C9A-ADBE-3476E1448E75}">
   <dimension ref="A2:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="78.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -922,7 +946,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -930,7 +954,7 @@
         <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -938,47 +962,47 @@
         <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>134</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>132</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1000,10 +1024,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC352499-16C6-4142-B6A7-FED4572A9C0C}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1014,7 +1038,7 @@
     <col min="4" max="5" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1022,7 +1046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1033,11 +1057,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1045,7 +1069,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1053,10 +1077,10 @@
         <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1064,10 +1088,10 @@
         <v>15</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1078,7 +1102,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1089,10 +1113,10 @@
         <v>20</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1103,10 +1127,10 @@
         <v>25</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1117,10 +1141,10 @@
         <v>26</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1131,10 +1155,10 @@
         <v>27</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1145,133 +1169,169 @@
         <v>28</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>55</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>136</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>55</v>
+        <v>53</v>
+      </c>
+      <c r="E15" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>136</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>45</v>
+        <v>54</v>
+      </c>
+      <c r="E16" t="str">
+        <f>IF(dcAdminsAadGroupObjectId = "", "Not needed", "Required")</f>
+        <v>Required</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>137</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>45</v>
+        <v>58</v>
+      </c>
+      <c r="E17" t="str">
+        <f>IF(hubSubnetJumpHostsDeploy = "Deploy", "Required", "Not Needed")</f>
+        <v>Required</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>137</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>45</v>
+        <v>59</v>
+      </c>
+      <c r="E18" s="7" t="str">
+        <f>IF(hubSubnet1Deploy = "Don't Deploy", "Not Needed", "Required")</f>
+        <v>Required</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>137</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
         <v>9</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>45</v>
+        <v>60</v>
+      </c>
+      <c r="E19" s="7" t="str">
+        <f>IF(
+OR(hubSubnet1Deploy = "Don't Deploy", hubSubnet2Deploy = "Don't Deploy"),
+"Not Needed", "Required")</f>
+        <v>Required</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>137</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
         <v>10</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>45</v>
+        <v>61</v>
+      </c>
+      <c r="E20" s="7" t="str">
+        <f>IF(
+OR(hubSubnet1Deploy = "Don't Deploy", hubSubnet2Deploy = "Don't Deploy", hubSubnet3Deploy = "Don't Deploy"),
+"Not Needed", "Required")</f>
+        <v>Required</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>137</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C21" t="s">
         <v>11</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>45</v>
+        <v>62</v>
+      </c>
+      <c r="E21" s="7" t="str">
+        <f>IF(
+OR(hubSubnet1Deploy = "Don't Deploy", hubSubnet2Deploy = "Don't Deploy", hubSubnet3Deploy = "Don't Deploy", hubSubnet4Deploy = "Don't Deploy"),
+"Not Needed", "Required")</f>
+        <v>Required</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>137</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C22" t="s">
         <v>2</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
+      </c>
+      <c r="E22" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1310,7 +1370,7 @@
         <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1355,10 +1415,10 @@
         <v>37</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1372,10 +1432,10 @@
         <v>36</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1389,7 +1449,7 @@
         <v>38</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1403,10 +1463,10 @@
         <v>39</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1420,10 +1480,10 @@
         <v>40</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1431,41 +1491,32 @@
         <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>133</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" t="s">
-        <v>2</v>
-      </c>
       <c r="D15" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1506,7 +1557,7 @@
         <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1514,10 +1565,10 @@
         <v>41</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D2" t="str">
         <f>IF(B2 &lt;&gt; "", _xlfn.CONCAT(CHAR(34), B2, "/", C2, CHAR(34)), _xlfn.CONCAT("""", """"))</f>
@@ -1537,10 +1588,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1552,10 +1603,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E7" t="str">
         <f>Spoke1!E7</f>
@@ -1570,10 +1621,10 @@
         <v>33</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E8" t="str">
         <f>Spoke1!E8</f>
@@ -1588,7 +1639,7 @@
         <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E9" t="str">
         <f>Spoke1!E9</f>
@@ -1603,10 +1654,10 @@
         <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E10" t="str">
         <f>Spoke1!E10</f>
@@ -1621,10 +1672,10 @@
         <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E11" t="str">
         <f>Spoke1!E11</f>
@@ -1636,41 +1687,32 @@
         <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>45</v>
+      <c r="A14" s="7" t="s">
+        <v>133</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" t="s">
-        <v>2</v>
-      </c>
       <c r="D15" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1708,7 +1750,7 @@
         <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1716,10 +1758,10 @@
         <v>41</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D2" t="str">
         <f>IF(B2 &lt;&gt; "", _xlfn.CONCAT(CHAR(34), B2, "/", C2, CHAR(34)), _xlfn.CONCAT("""", """"))</f>
@@ -1739,10 +1781,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1754,10 +1796,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E7" t="str">
         <f>Spoke1!E7</f>
@@ -1772,10 +1814,10 @@
         <v>33</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E8" t="str">
         <f>Spoke1!E8</f>
@@ -1790,7 +1832,7 @@
         <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E9" t="str">
         <f>Spoke1!E9</f>
@@ -1805,10 +1847,10 @@
         <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E10" t="str">
         <f>Spoke1!E10</f>
@@ -1823,10 +1865,10 @@
         <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E11" t="str">
         <f>Spoke1!E11</f>
@@ -1838,41 +1880,32 @@
         <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>45</v>
+      <c r="A14" s="7" t="s">
+        <v>133</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" t="s">
-        <v>2</v>
-      </c>
       <c r="D15" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1888,7 +1921,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E5F0421-4CC3-4847-AE8E-9E8CD1C6E8C6}">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -1902,16 +1935,16 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B1" s="4" t="str">
         <f>_xlfn.CONCAT(B3, ",", B4, ",", B5,  B6)</f>
-        <v>{"$schema":"https://schema.management.azure.com/schemas/2019-04-01/deploymentParameters.json#","contentVersion":"1.0.0.0","parameters":{"assetLocationURI": {"value":"https://raw.githubusercontent.com/mbakunas/Azure-HubSpoke/master/"},"vnetDdosProtectionLevel": {"value":"Basic"},"vnetDdosProtectionPlanName": {"value":"DDOS-Plan-01"},"vnetNsgSecurityLevel": {"value":"Medium"},"routeTableName": {"value":"RouteTable-01"},"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetBastionAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},"dcAdminsAadGroupId": {"value":"17ba8236-a5e8-4173-8ce9-c69b17743ac2"},"dcVmContributorsRoleAssignmentID": {"value":["184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"]},"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01","Spoke-Dev-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16","10.3.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["","c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02","16936380-29b0-4326-8f6b-db86da154736/HubSpoke-03"]},"spokeSubnetBastionAddressSpace": {"value":["0.0.0.0/0"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25","10.3.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24","10.3.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24","10.3.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24","10.3.3.0/24"]},"appTeamsAadGroupId": {"value":["c2ecad99-6ed7-4e11-8acc-0fa0262a2c69"]},"spokeVmContributorsRoleAssignmentID": {"value":["5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6","b2b76710-60c9-4826-b864-272c7c115806"]}}}</v>
+        <v>{"$schema":"https://schema.management.azure.com/schemas/2019-04-01/deploymentParameters.json#","contentVersion":"1.0.0.0","parameters":{"assetLocationURI": {"value":"https://raw.githubusercontent.com/mbakunas/Azure-HubSpoke/master/"},"vnetDdosProtectionLevel": {"value":"Basic"},"vnetDdosProtectionPlanName": {"value":"DDOS-Plan-01"},"vnetNsgSecurityLevel": {"value":"Medium"},"routeTableName": {"value":"RouteTable-01"},"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetBastionAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},"dcSubnetVmContAadGroupId": {"value":"17ba8236-a5e8-4173-8ce9-c69b17743ac2"},"dcVmContributorsRoleAssignmentID": {"value":["184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"]},"hubSubnetVmContAadGroupId": {"value":"5eb970ea-e71a-4bf9-ba78-0529b3aeb2f3"},"hubSubnetVmContRoleAssignmantId": {"value":["0702dcd4-0b65-4ebb-8ebd-873e2729904b","594fd8bf-f554-4272-8b19-9725c7b706b4","b3f5340d-28be-4029-bc10-56af7e20ac75","7a1689a7-66d8-4010-9213-c837316f8a30","d83bc577-1b03-4604-94a1-150ba7198ed0","6cba977a-462f-4d8c-b291-2dad991f85a0"]},"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01","Spoke-Dev-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16","10.3.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["","c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02","16936380-29b0-4326-8f6b-db86da154736/HubSpoke-03"]},"spokeSubnetBastionAddressSpace": {"value":["0.0.0.0/0"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25","10.3.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24","10.3.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24","10.3.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24","10.3.3.0/24"]},"spokeVmContAadGroupId": {"value":["c2ecad99-6ed7-4e11-8acc-0fa0262a2c69"]},"spokeVmContributorsRoleAssignmentID": {"value":["5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6","b2b76710-60c9-4826-b864-272c7c115806"]}}}</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B3" t="str">
         <f>_xlfn.CONCAT("{",
@@ -1929,7 +1962,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B4" t="str">
         <f>_xlfn.CONCAT(
@@ -1950,15 +1983,17 @@
 CHAR(34), "hubSubnet3AddressSpace", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), calcHubSubnet3AddressSpace, CHAR(34), "},",
 CHAR(34), "hubSubnet4Name", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), hubSubnet4Name, CHAR(34), "},",
 CHAR(34), "hubSubnet4AddressSpace", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), calcHubSubnet4AddressSpace, CHAR(34), "},",
-CHAR(34), "dcAdminsAadGroupId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), dcAdminsAadGroupObjectId, CHAR(34), "},",
-CHAR(34), "dcVmContributorsRoleAssignmentID", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", CHAR(34), Hub!D15, CHAR(34), ",", CHAR(34),Hub!D16, CHAR(34), "]}",
+CHAR(34), "dcSubnetVmContAadGroupId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), dcAdminsAadGroupObjectId, CHAR(34), "},",
+CHAR(34), "dcVmContributorsRoleAssignmentID", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", dcVmContributorsRoleAssignmentID, "]},",
+CHAR(34), "hubSubnetVmContAadGroupId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), serverTeamAadGroupObjectId, CHAR(34), "},",
+CHAR(34), "hubSubnetVmContRoleAssignmantId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", hubSubnetVmContRoleAssignmantId, "]}"
 )</f>
-        <v>"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetBastionAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},"dcAdminsAadGroupId": {"value":"17ba8236-a5e8-4173-8ce9-c69b17743ac2"},"dcVmContributorsRoleAssignmentID": {"value":["184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"]}</v>
+        <v>"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetBastionAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},"dcSubnetVmContAadGroupId": {"value":"17ba8236-a5e8-4173-8ce9-c69b17743ac2"},"dcVmContributorsRoleAssignmentID": {"value":["184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"]},"hubSubnetVmContAadGroupId": {"value":"5eb970ea-e71a-4bf9-ba78-0529b3aeb2f3"},"hubSubnetVmContRoleAssignmantId": {"value":["0702dcd4-0b65-4ebb-8ebd-873e2729904b","594fd8bf-f554-4272-8b19-9725c7b706b4","b3f5340d-28be-4029-bc10-56af7e20ac75","7a1689a7-66d8-4010-9213-c837316f8a30","d83bc577-1b03-4604-94a1-150ba7198ed0","6cba977a-462f-4d8c-b291-2dad991f85a0"]}</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B5" t="str">
         <f>_xlfn.CONCAT(
@@ -1974,15 +2009,15 @@
 CHAR(34), "spokeSubnet2AddressSpace", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", spokeSubnet2AddressSpace,"]},",
 CHAR(34), "spokeSubnet3Name", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", spokeSubnet3Name,"]},",
 CHAR(34), "spokeSubnet3AddressSpace", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", spokeSubnet3AddressSpace,"]},",
-CHAR(34), "appTeamsAadGroupId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", CHAR(34), appTeamsAadGroupObjectId, CHAR(34), "]},",
+CHAR(34), "spokeVmContAadGroupId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", CHAR(34), appTeamsAadGroupObjectId, CHAR(34), "]},",
 CHAR(34), "spokeVmContributorsRoleAssignmentID", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", spokeVmContributorsRoleAssignmentID,"]}"
 )</f>
-        <v>"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01","Spoke-Dev-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16","10.3.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["","c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02","16936380-29b0-4326-8f6b-db86da154736/HubSpoke-03"]},"spokeSubnetBastionAddressSpace": {"value":["0.0.0.0/0"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25","10.3.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24","10.3.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24","10.3.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24","10.3.3.0/24"]},"appTeamsAadGroupId": {"value":["c2ecad99-6ed7-4e11-8acc-0fa0262a2c69"]},"spokeVmContributorsRoleAssignmentID": {"value":["5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6","b2b76710-60c9-4826-b864-272c7c115806"]}</v>
+        <v>"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01","Spoke-Dev-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16","10.3.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["","c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02","16936380-29b0-4326-8f6b-db86da154736/HubSpoke-03"]},"spokeSubnetBastionAddressSpace": {"value":["0.0.0.0/0"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25","10.3.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24","10.3.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24","10.3.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24","10.3.3.0/24"]},"spokeVmContAadGroupId": {"value":["c2ecad99-6ed7-4e11-8acc-0fa0262a2c69"]},"spokeVmContributorsRoleAssignmentID": {"value":["5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6","b2b76710-60c9-4826-b864-272c7c115806"]}</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B6" t="str">
         <f>_xlfn.CONCAT(
@@ -1992,14 +2027,14 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="B9" s="7"/>
+      <c r="A9" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" s="8"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B10" t="str">
         <f>IF(hubSubnetFirewallDeploy = "Deploy", hubSubnetFirewallAddressSpace, "0.0.0.0/0")</f>
@@ -2008,7 +2043,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B11" t="str">
         <f>IF(hubSubnetBastionDeploy = "Deploy", hubSubnetBastionAddressSpace, "0.0.0.0/0")</f>
@@ -2017,7 +2052,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B12" t="str">
         <f>IF(hubSubnetJumpHostsDeploy = "Deploy", hubSubnetJumpHostsAddressSpace, "0.0.0.0/0")</f>
@@ -2026,7 +2061,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B13" t="str">
         <f>IF(hubSubnet1Deploy = "Deploy", hubSubnet1AddressSpace, "0.0.0.0/0")</f>
@@ -2035,7 +2070,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B14" t="str">
         <f>IF(
@@ -2047,7 +2082,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B15" t="str">
         <f>IF(
@@ -2059,7 +2094,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B16" t="str">
         <f>IF(
@@ -2069,44 +2104,76 @@
         <v>10.0.1.96/27</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="B19" s="7"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>87</v>
-      </c>
-      <c r="B20" t="str">
+        <v>140</v>
+      </c>
+      <c r="B19" s="7" t="str">
+        <f>_xlfn.CONCAT("""", Hub!D15, """", ",", """", Hub!D16, """")</f>
+        <v>"184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B20" s="7" t="str">
+        <f>_xlfn.CONCAT(
+"""", Hub!D22, """",
+IF(Hub!E17 = "Required", "," &amp; """" &amp; Hub!D17 &amp; """", ""),
+IF(Hub!E18 = "Required", "," &amp; """" &amp; Hub!D18 &amp; """", ""),
+IF(Hub!E19 = "Required", "," &amp; """" &amp; Hub!D19 &amp; """", ""),
+IF(Hub!E20 = "Required", "," &amp; """" &amp; Hub!D20 &amp; """", ""),
+IF(Hub!E21 = "Required", "," &amp; """" &amp; Hub!D21 &amp; """", "")
+)</f>
+        <v>"0702dcd4-0b65-4ebb-8ebd-873e2729904b","594fd8bf-f554-4272-8b19-9725c7b706b4","b3f5340d-28be-4029-bc10-56af7e20ac75","7a1689a7-66d8-4010-9213-c837316f8a30","d83bc577-1b03-4604-94a1-150ba7198ed0","6cba977a-462f-4d8c-b291-2dad991f85a0"</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" s="8"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" t="str">
         <f>_xlfn.CONCAT(CHAR(34), Spoke1!$B$5, CHAR(34), ",", CHAR(34), Spoke2!$B$5, CHAR(34), ",", CHAR(34), Spoke3!$B$5, CHAR(34))</f>
         <v>"Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01","Spoke-Dev-EastUS2-01"</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>88</v>
-      </c>
-      <c r="B21" t="str">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" t="str">
         <f>_xlfn.CONCAT(CHAR(34), Spoke1!$C$5, CHAR(34), ",", CHAR(34), Spoke2!$C$5, CHAR(34), ",", CHAR(34), Spoke3!$C$5, CHAR(34))</f>
         <v>"10.1.0.0/16","10.2.0.0/16","10.3.0.0/16"</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>89</v>
-      </c>
-      <c r="B22" t="str">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" t="str">
         <f>_xlfn.CONCAT(Spoke1!$D$2, ",", Spoke2!$D$2, ",", Spoke3!$D$2)</f>
         <v>"","c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02","16936380-29b0-4326-8f6b-db86da154736/HubSpoke-03"</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>94</v>
-      </c>
-      <c r="B23" t="str">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" t="str">
         <f>IF(
 Spoke1!$E$7 = "Common",
 IF(Spoke1!$D$7 = "Don't Deploy", """"  &amp; "0.0.0.0/0" &amp; """", """" &amp;  Spoke1!$C$7 &amp; """" &amp; "," &amp;   """" &amp; Spoke2!$C$7  &amp; """" &amp; "," &amp;   """" &amp; Spoke3!$C$7),
@@ -2123,11 +2190,11 @@
         <v>"0.0.0.0/0"</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>92</v>
-      </c>
-      <c r="B24" s="5" t="str">
+    <row r="28" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28" s="5" t="str">
         <f>IF(
 Spoke1!$E$8 = "Common",
 """" &amp; Spoke1!$B$8 &amp; """",
@@ -2136,11 +2203,11 @@
         <v>"AppGW"</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>93</v>
-      </c>
-      <c r="B25" s="3" t="str">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" s="3" t="str">
         <f>IF(
 Spoke1!$E$8 = "Common",
 IF(Spoke1!$D$8 = "Don't Deploy", """"  &amp; "0.0.0.0/0" &amp; """", """" &amp;  Spoke1!$C$8 &amp; """" &amp; "," &amp;   """" &amp; Spoke2!$C$8  &amp; """" &amp; "," &amp;   """" &amp; Spoke3!$C$8 &amp; """"),
@@ -2157,11 +2224,11 @@
         <v>"10.1.0.128/25","10.2.0.128/25","10.3.0.128/25"</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>96</v>
-      </c>
-      <c r="B26" s="5" t="str">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" s="5" t="str">
         <f>IF(
 Spoke1!$E$8 = "Common",
 """" &amp; Spoke1!$B$9 &amp; """",
@@ -2170,11 +2237,11 @@
         <v>"Subnet1"</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>97</v>
-      </c>
-      <c r="B27" s="3" t="str">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31" s="3" t="str">
         <f>IF(
 Spoke1!$E$9 = "Common",
 IF(Spoke1!$D$9 = "Don't Deploy", """"  &amp; "0.0.0.0/0" &amp; """", """" &amp;  Spoke1!$C$9 &amp; """" &amp; "," &amp;   """" &amp; Spoke2!$C$9  &amp; """" &amp; "," &amp;   """" &amp; Spoke3!$C$9 &amp; """"),
@@ -2191,11 +2258,11 @@
         <v>"10.1.1.0/24","10.2.1.0/24","10.3.1.0/24"</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>98</v>
-      </c>
-      <c r="B28" s="5" t="str">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>95</v>
+      </c>
+      <c r="B32" s="5" t="str">
         <f>IF(
 Spoke1!$E$10 = "Common",
 """" &amp; Spoke1!$B$10 &amp; """",
@@ -2204,11 +2271,11 @@
         <v>"Subnet2"</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>99</v>
-      </c>
-      <c r="B29" s="3" t="str">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>96</v>
+      </c>
+      <c r="B33" s="3" t="str">
         <f>IF(
 Spoke1!$E$10 = "Common",
 IF(Spoke1!$D$10 = "Don't Deploy", """"  &amp; "0.0.0.0/0" &amp; """", """" &amp;  Spoke1!$C$10 &amp; """" &amp; "," &amp;   """" &amp; Spoke2!$C$10  &amp; """" &amp; "," &amp;   """" &amp; Spoke3!$C$10 &amp; """"),
@@ -2225,11 +2292,11 @@
         <v>"10.1.2.0/24","10.2.2.0/24","10.3.2.0/24"</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>100</v>
-      </c>
-      <c r="B30" s="5" t="str">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" s="5" t="str">
         <f>IF(
 Spoke1!$E$8 = "Common",
 """" &amp; Spoke1!$B$11 &amp; """",
@@ -2238,11 +2305,11 @@
         <v>"Subnet3"</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>101</v>
-      </c>
-      <c r="B31" s="3" t="str">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>98</v>
+      </c>
+      <c r="B35" s="3" t="str">
         <f>IF(
 Spoke1!$E$11 = "Common",
 IF(OR(Spoke1!$D$11 = "Don't Deploy", Spoke1!$D$10 = "Don't Deploy"),
@@ -2263,11 +2330,11 @@
         <v>"10.1.3.0/24","10.2.3.0/24","10.3.3.0/24"</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>133</v>
-      </c>
-      <c r="B32" t="str">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>130</v>
+      </c>
+      <c r="B36" t="str">
         <f>_xlfn.CONCAT("""",Spoke1!D15,"""",",","""",Spoke2!D15,"""",",","""",Spoke3!D15,"""")</f>
         <v>"5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6","b2b76710-60c9-4826-b864-272c7c115806"</v>
       </c>
@@ -2275,7 +2342,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A23:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2306,46 +2373,46 @@
         <v>31</v>
       </c>
       <c r="E1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added explicit sub/RG parameters/variables
</commit_message>
<xml_diff>
--- a/PowerShell/ParametersFileBuilder_3-Spoke.xlsx
+++ b/PowerShell/ParametersFileBuilder_3-Spoke.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mark.bakunas\Documents\GitHub\Azure-HubSpoke\PowerShell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E2FBD8-9446-47A1-BF7A-8CFE43A505C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D61806-ED20-454A-AE11-5DE83A0D631D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4365" yWindow="600" windowWidth="21600" windowHeight="13650" activeTab="1" xr2:uid="{74A5C2AD-3876-4989-8818-24030CBF60E7}"/>
+    <workbookView xWindow="3855" yWindow="1860" windowWidth="21600" windowHeight="11385" xr2:uid="{74A5C2AD-3876-4989-8818-24030CBF60E7}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="4" r:id="rId1"/>
@@ -24,57 +24,58 @@
   <definedNames>
     <definedName name="appTeamsAadGroupObjectId">General!$B$12</definedName>
     <definedName name="assetLocationURI">General!$B$2</definedName>
-    <definedName name="calcHhubSubnetFirewallAddressSpace">ParametersFile!$B$10</definedName>
-    <definedName name="calcHubSubnet1AddressSpace">ParametersFile!$B$13</definedName>
-    <definedName name="calcHubSubnet2AddressSpace">ParametersFile!$B$14</definedName>
-    <definedName name="calcHubSubnet3AddressSpace">ParametersFile!$B$15</definedName>
-    <definedName name="calcHubSubnet4AddressSpace">ParametersFile!$B$16</definedName>
-    <definedName name="calcHubSubnetBastionAddressSpace">ParametersFile!$B$11</definedName>
-    <definedName name="calcHubSubnetJumpHostsAddressSpace">ParametersFile!$B$12</definedName>
+    <definedName name="calcHhubSubnetFirewallAddressSpace">ParametersFile!$B$11</definedName>
+    <definedName name="calcHubSubnet1AddressSpace">ParametersFile!$B$14</definedName>
+    <definedName name="calcHubSubnet2AddressSpace">ParametersFile!$B$15</definedName>
+    <definedName name="calcHubSubnet3AddressSpace">ParametersFile!$B$16</definedName>
+    <definedName name="calcHubSubnet4AddressSpace">ParametersFile!$B$17</definedName>
+    <definedName name="calcHubSubnetBastionAddressSpace">ParametersFile!$B$12</definedName>
+    <definedName name="calcHubSubnetJumpHostsAddressSpace">ParametersFile!$B$13</definedName>
     <definedName name="dcAdminsAadGroupObjectId">General!$B$10</definedName>
-    <definedName name="dcVmContributorsRoleAssignmentID">ParametersFile!$B$19</definedName>
+    <definedName name="dcVmContributorsRoleAssignmentID">ParametersFile!$B$20</definedName>
     <definedName name="deployOptions_List">Lists!$E$2:$E$3</definedName>
-    <definedName name="hubSubnet1AddressSpace">Hub!$C$9</definedName>
-    <definedName name="hubSubnet1Deploy">Hub!$D$9</definedName>
-    <definedName name="hubSubnet1Name">Hub!$B$9</definedName>
-    <definedName name="hubSubnet2AddressSpace">Hub!$C$10</definedName>
-    <definedName name="hubSubnet2Deploy">Hub!$D$10</definedName>
-    <definedName name="hubSubnet2Name">Hub!$B$10</definedName>
-    <definedName name="hubSubnet3AddressSpace">Hub!$C$11</definedName>
-    <definedName name="hubSubnet3Deploy">Hub!$D$11</definedName>
-    <definedName name="hubSubnet3Name">Hub!$B$11</definedName>
-    <definedName name="hubSubnet4AddressSpace">Hub!$C$12</definedName>
-    <definedName name="hubSubnet4Deploy">Hub!$D$12</definedName>
-    <definedName name="hubSubnet4Name">Hub!$B$12</definedName>
-    <definedName name="hubSubnetBastionAddressSpace">Hub!$C$6</definedName>
-    <definedName name="hubSubnetBastionDeploy">Hub!$D$6</definedName>
-    <definedName name="hubSubnetDcAddressSpace">Hub!$C$7</definedName>
-    <definedName name="hubSubnetDcName">Hub!$B$7</definedName>
-    <definedName name="hubSubnetFirewallAddressSpace">Hub!$C$5</definedName>
-    <definedName name="hubSubnetFirewallDeploy">Hub!$D$5</definedName>
-    <definedName name="hubSubnetGatewayAddressSpace">Hub!$C$4</definedName>
-    <definedName name="hubSubnetJumpHostsAddressSpace">Hub!$C$8</definedName>
-    <definedName name="hubSubnetJumpHostsDeploy">Hub!$D$8</definedName>
-    <definedName name="hubSubnetJumpHostsName">Hub!$B$8</definedName>
-    <definedName name="hubSubnetVmContRoleAssignmantId">ParametersFile!$B$20</definedName>
-    <definedName name="hubVnetAddressSpace">Hub!$C$2</definedName>
-    <definedName name="hubVnetName">Hub!$B$2</definedName>
+    <definedName name="hubDeploySubscriptionResourceGroup">Hub!$D$2</definedName>
+    <definedName name="hubSubnet1AddressSpace">Hub!$C$12</definedName>
+    <definedName name="hubSubnet1Deploy">Hub!$D$12</definedName>
+    <definedName name="hubSubnet1Name">Hub!$B$12</definedName>
+    <definedName name="hubSubnet2AddressSpace">Hub!$C$13</definedName>
+    <definedName name="hubSubnet2Deploy">Hub!$D$13</definedName>
+    <definedName name="hubSubnet2Name">Hub!$B$13</definedName>
+    <definedName name="hubSubnet3AddressSpace">Hub!$C$14</definedName>
+    <definedName name="hubSubnet3Deploy">Hub!$D$14</definedName>
+    <definedName name="hubSubnet3Name">Hub!$B$14</definedName>
+    <definedName name="hubSubnet4AddressSpace">Hub!$C$15</definedName>
+    <definedName name="hubSubnet4Deploy">Hub!$D$15</definedName>
+    <definedName name="hubSubnet4Name">Hub!$B$15</definedName>
+    <definedName name="hubSubnetBastionAddressSpace">Hub!$C$9</definedName>
+    <definedName name="hubSubnetBastionDeploy">Hub!$D$9</definedName>
+    <definedName name="hubSubnetDcAddressSpace">Hub!$C$10</definedName>
+    <definedName name="hubSubnetDcName">Hub!$B$10</definedName>
+    <definedName name="hubSubnetFirewallAddressSpace">Hub!$C$8</definedName>
+    <definedName name="hubSubnetFirewallDeploy">Hub!$D$8</definedName>
+    <definedName name="hubSubnetGatewayAddressSpace">Hub!$C$7</definedName>
+    <definedName name="hubSubnetJumpHostsAddressSpace">Hub!$C$11</definedName>
+    <definedName name="hubSubnetJumpHostsDeploy">Hub!$D$11</definedName>
+    <definedName name="hubSubnetJumpHostsName">Hub!$B$11</definedName>
+    <definedName name="hubSubnetVmContRoleAssignmantId">ParametersFile!$B$21</definedName>
+    <definedName name="hubVnetAddressSpace">Hub!$C$5</definedName>
+    <definedName name="hubVnetName">Hub!$B$5</definedName>
     <definedName name="routeTableName">General!$B$7</definedName>
     <definedName name="serverTeamAadGroupObjectId">General!$B$11</definedName>
-    <definedName name="spokeDeploySubscriptionResourceGroup">ParametersFile!$B$26</definedName>
-    <definedName name="spokeSubnet1AddressSpace">ParametersFile!$B$31</definedName>
-    <definedName name="spokeSubnet1Name">ParametersFile!$B$30</definedName>
-    <definedName name="spokeSubnet2AddressSpace">ParametersFile!$B$33</definedName>
-    <definedName name="spokeSubnet2Name">ParametersFile!$B$32</definedName>
-    <definedName name="spokeSubnet3AddressSpace">ParametersFile!$B$35</definedName>
-    <definedName name="spokeSubnet3Name">ParametersFile!$B$34</definedName>
-    <definedName name="spokeSubnetAppGwAddressSpace">ParametersFile!$B$29</definedName>
-    <definedName name="spokeSubnetAppGwName">ParametersFile!$B$28</definedName>
-    <definedName name="spokeSubnetBastionAddressSpace">ParametersFile!$B$27</definedName>
+    <definedName name="spokeDeploySubscriptionResourceGroup">ParametersFile!$B$27</definedName>
+    <definedName name="spokeSubnet1AddressSpace">ParametersFile!$B$32</definedName>
+    <definedName name="spokeSubnet1Name">ParametersFile!$B$31</definedName>
+    <definedName name="spokeSubnet2AddressSpace">ParametersFile!$B$34</definedName>
+    <definedName name="spokeSubnet2Name">ParametersFile!$B$33</definedName>
+    <definedName name="spokeSubnet3AddressSpace">ParametersFile!$B$36</definedName>
+    <definedName name="spokeSubnet3Name">ParametersFile!$B$35</definedName>
+    <definedName name="spokeSubnetAppGwAddressSpace">ParametersFile!$B$30</definedName>
+    <definedName name="spokeSubnetAppGwName">ParametersFile!$B$29</definedName>
+    <definedName name="spokeSubnetBastionAddressSpace">ParametersFile!$B$28</definedName>
     <definedName name="spokeSubnetUniqueness_List">Lists!$G$2:$G$3</definedName>
-    <definedName name="spokeVmContributorsRoleAssignmentID">ParametersFile!$B$36</definedName>
-    <definedName name="spokeVnetAddressSpace">ParametersFile!$B$25</definedName>
-    <definedName name="spokeVnetName">ParametersFile!$B$24</definedName>
+    <definedName name="spokeVmContributorsRoleAssignmentID">ParametersFile!$B$37</definedName>
+    <definedName name="spokeVnetAddressSpace">ParametersFile!$B$26</definedName>
+    <definedName name="spokeVnetName">ParametersFile!$B$25</definedName>
     <definedName name="vnetDdosProtectionLevel">General!$B$4</definedName>
     <definedName name="vnetDdosProtectionLevel_List">Lists!$A$2:$A$4</definedName>
     <definedName name="vnetDdosProtectionPlanName">General!$B$5</definedName>
@@ -99,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="146">
   <si>
     <t>Name</t>
   </si>
@@ -299,9 +300,6 @@
     <t>Route Table Name</t>
   </si>
   <si>
-    <t>RouteTable-01</t>
-  </si>
-  <si>
     <t>Header</t>
   </si>
   <si>
@@ -525,6 +523,21 @@
   </si>
   <si>
     <t>002984bd-b5ce-445d-8138-d19b514550c7</t>
+  </si>
+  <si>
+    <t>hubDeploySubscriptionResourceGroup</t>
+  </si>
+  <si>
+    <t>f0bb6c48-80fd-445c-98cb-c38b5f817d52</t>
+  </si>
+  <si>
+    <t>HubSpoke-01</t>
+  </si>
+  <si>
+    <t>Hub RBAC</t>
+  </si>
+  <si>
+    <t>RouteTable-EastUS2-01</t>
   </si>
 </sst>
 </file>
@@ -587,7 +600,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
@@ -597,6 +610,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
@@ -922,7 +936,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27806494-5F45-4C9A-ADBE-3476E1448E75}">
   <dimension ref="A2:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -946,7 +960,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>109</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -970,39 +984,39 @@
         <v>65</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>66</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -1024,320 +1038,347 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC352499-16C6-4142-B6A7-FED4572A9C0C}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D2" s="8" t="str">
+        <f>_xlfn.CONCAT(B2, "/", C2)</f>
+        <v>f0bb6c48-80fd-445c-98cb-c38b5f817d52/HubSpoke-01</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="D8" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="D9" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="D11" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="D12" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="D13" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="D14" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="D15" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>44</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B17" t="s">
         <v>45</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C17" t="s">
         <v>52</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B18" t="s">
         <v>46</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C18" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E15" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="E18" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B19" t="s">
         <v>54</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C19" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E16" t="str">
+      <c r="E19" t="str">
         <f>IF(dcAdminsAadGroupObjectId = "", "Not needed", "Required")</f>
         <v>Required</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B20" t="s">
         <v>46</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C20" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E17" t="str">
+      <c r="E20" t="str">
         <f>IF(hubSubnetJumpHostsDeploy = "Deploy", "Required", "Not Needed")</f>
         <v>Required</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="B18" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B21" t="s">
         <v>46</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C21" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="7" t="str">
+      <c r="E21" s="7" t="str">
         <f>IF(hubSubnet1Deploy = "Don't Deploy", "Not Needed", "Required")</f>
         <v>Required</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B22" t="s">
         <v>46</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C22" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E19" s="7" t="str">
+      <c r="E22" s="7" t="str">
         <f>IF(
 OR(hubSubnet1Deploy = "Don't Deploy", hubSubnet2Deploy = "Don't Deploy"),
 "Not Needed", "Required")</f>
         <v>Required</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="B20" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B23" t="s">
         <v>46</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C23" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E20" s="7" t="str">
+      <c r="E23" s="7" t="str">
         <f>IF(
 OR(hubSubnet1Deploy = "Don't Deploy", hubSubnet2Deploy = "Don't Deploy", hubSubnet3Deploy = "Don't Deploy"),
 "Not Needed", "Required")</f>
         <v>Required</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="B21" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B24" t="s">
         <v>46</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C24" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E21" s="7" t="str">
+      <c r="E24" s="7" t="str">
         <f>IF(
 OR(hubSubnet1Deploy = "Don't Deploy", hubSubnet2Deploy = "Don't Deploy", hubSubnet3Deploy = "Don't Deploy", hubSubnet4Deploy = "Don't Deploy"),
 "Not Needed", "Required")</f>
         <v>Required</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E25" t="s">
         <v>134</v>
-      </c>
-      <c r="B22" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E22" t="s">
-        <v>135</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D6 D8:D12" xr:uid="{D9354EF7-27D1-4C1F-B57B-07A789DEC96E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:D9 D11:D15" xr:uid="{D9354EF7-27D1-4C1F-B57B-07A789DEC96E}">
       <formula1>deployOptions_List</formula1>
     </dataValidation>
   </dataValidations>
@@ -1370,18 +1411,22 @@
         <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="D2" t="str">
         <f>IF(B2 &lt;&gt; "", _xlfn.CONCAT(CHAR(34), B2, "/", C2, CHAR(34)), _xlfn.CONCAT("""", """"))</f>
-        <v>""</v>
+        <v>"f0bb6c48-80fd-445c-98cb-c38b5f817d52/HubSpoke-01"</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1415,10 +1460,10 @@
         <v>37</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1432,10 +1477,10 @@
         <v>36</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1449,7 +1494,7 @@
         <v>38</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1463,10 +1508,10 @@
         <v>39</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1480,10 +1525,10 @@
         <v>40</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1502,7 +1547,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B14" t="s">
         <v>46</v>
@@ -1557,7 +1602,7 @@
         <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1565,10 +1610,10 @@
         <v>41</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="D2" t="str">
         <f>IF(B2 &lt;&gt; "", _xlfn.CONCAT(CHAR(34), B2, "/", C2, CHAR(34)), _xlfn.CONCAT("""", """"))</f>
@@ -1588,10 +1633,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1603,10 +1648,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E7" t="str">
         <f>Spoke1!E7</f>
@@ -1621,10 +1666,10 @@
         <v>33</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E8" t="str">
         <f>Spoke1!E8</f>
@@ -1639,7 +1684,7 @@
         <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E9" t="str">
         <f>Spoke1!E9</f>
@@ -1654,10 +1699,10 @@
         <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E10" t="str">
         <f>Spoke1!E10</f>
@@ -1672,10 +1717,10 @@
         <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E11" t="str">
         <f>Spoke1!E11</f>
@@ -1698,7 +1743,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B14" t="s">
         <v>46</v>
@@ -1707,12 +1752,12 @@
         <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D15" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1750,7 +1795,7 @@
         <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1758,10 +1803,10 @@
         <v>41</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="D2" t="str">
         <f>IF(B2 &lt;&gt; "", _xlfn.CONCAT(CHAR(34), B2, "/", C2, CHAR(34)), _xlfn.CONCAT("""", """"))</f>
@@ -1781,10 +1826,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1796,10 +1841,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E7" t="str">
         <f>Spoke1!E7</f>
@@ -1814,10 +1859,10 @@
         <v>33</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E8" t="str">
         <f>Spoke1!E8</f>
@@ -1832,7 +1877,7 @@
         <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E9" t="str">
         <f>Spoke1!E9</f>
@@ -1847,10 +1892,10 @@
         <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E10" t="str">
         <f>Spoke1!E10</f>
@@ -1865,10 +1910,10 @@
         <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E11" t="str">
         <f>Spoke1!E11</f>
@@ -1891,7 +1936,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B14" t="s">
         <v>46</v>
@@ -1900,12 +1945,12 @@
         <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D15" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1921,7 +1966,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E5F0421-4CC3-4847-AE8E-9E8CD1C6E8C6}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -1935,16 +1980,16 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="4" t="str">
-        <f>_xlfn.CONCAT(B3, ",", B4, ",", B5,  B6)</f>
-        <v>{"$schema":"https://schema.management.azure.com/schemas/2019-04-01/deploymentParameters.json#","contentVersion":"1.0.0.0","parameters":{"assetLocationURI": {"value":"https://raw.githubusercontent.com/mbakunas/Azure-HubSpoke/master/"},"vnetDdosProtectionLevel": {"value":"Standard - Create New"},"vnetDdosProtectionPlanName": {"value":"DDOS-Plan-01"},"vnetNsgSecurityLevel": {"value":"Medium"},"routeTableName": {"value":"RouteTable-01"},"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"10.0.0.64/26"},"hubSubnetBastionAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},"dcSubnetVmContAadGroupId": {"value":"83578c91-9919-4bd8-bee8-2649f6eb7c13"},"dcVmContributorsRoleAssignmentID": {"value":["184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"]},"hubSubnetVmContAadGroupId": {"value":"57f2ff92-300b-4075-a7ab-2030b46ebe2f"},"hubSubnetVmContRoleAssignmantId": {"value":["0702dcd4-0b65-4ebb-8ebd-873e2729904b","594fd8bf-f554-4272-8b19-9725c7b706b4","b3f5340d-28be-4029-bc10-56af7e20ac75","7a1689a7-66d8-4010-9213-c837316f8a30","d83bc577-1b03-4604-94a1-150ba7198ed0","6cba977a-462f-4d8c-b291-2dad991f85a0"]},"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01","Spoke-Dev-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16","10.3.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["","c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02","16936380-29b0-4326-8f6b-db86da154736/HubSpoke-03"]},"spokeSubnetBastionAddressSpace": {"value":["0.0.0.0/0"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25","10.3.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24","10.3.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24","10.3.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24","10.3.3.0/24"]},"spokeVmContAadGroupId": {"value":["002984bd-b5ce-445d-8138-d19b514550c7"]},"spokeVmContributorsRoleAssignmentID": {"value":["5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6","b2b76710-60c9-4826-b864-272c7c115806"]}}}</v>
+        <f>_xlfn.CONCAT(B3, ",", B4, B5, ",", B6,  B7)</f>
+        <v>{"$schema":"https://schema.management.azure.com/schemas/2019-04-01/deploymentParameters.json#","contentVersion":"1.0.0.0","parameters":{"assetLocationURI": {"value":"https://raw.githubusercontent.com/mbakunas/Azure-HubSpoke/master/"},"vnetDdosProtectionLevel": {"value":"Basic"},"vnetDdosProtectionPlanName": {"value":"DDOS-Plan-01"},"vnetNsgSecurityLevel": {"value":"Medium"},"routeTableName": {"value":"RouteTable-EastUS2-01"},"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubDeploySubscriptionResourceGroup": {"value":"f0bb6c48-80fd-445c-98cb-c38b5f817d52/HubSpoke-01"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetBastionAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},"dcSubnetVmContAadGroupId": {"value":"83578c91-9919-4bd8-bee8-2649f6eb7c13"},"dcVmContributorsRoleAssignmentID": {"value":["184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"]},"hubSubnetVmContAadGroupId": {"value":"57f2ff92-300b-4075-a7ab-2030b46ebe2f"},"hubSubnetVmContRoleAssignmantId": {"value":["0702dcd4-0b65-4ebb-8ebd-873e2729904b","594fd8bf-f554-4272-8b19-9725c7b706b4","b3f5340d-28be-4029-bc10-56af7e20ac75","7a1689a7-66d8-4010-9213-c837316f8a30","d83bc577-1b03-4604-94a1-150ba7198ed0","6cba977a-462f-4d8c-b291-2dad991f85a0"]},"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01","Spoke-Dev-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16","10.3.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["f0bb6c48-80fd-445c-98cb-c38b5f817d52/HubSpoke-01","c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02","16936380-29b0-4326-8f6b-db86da154736/HubSpoke-03"]},"spokeSubnetBastionAddressSpace": {"value":["0.0.0.0/0"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25","10.3.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24","10.3.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24","10.3.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24","10.3.3.0/24"]},"spokeVmContAadGroupId": {"value":["002984bd-b5ce-445d-8138-d19b514550c7"]},"spokeVmContributorsRoleAssignmentID": {"value":["5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6","b2b76710-60c9-4826-b864-272c7c115806"]}}}</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" t="str">
         <f>_xlfn.CONCAT("{",
@@ -1957,17 +2002,18 @@
 CHAR(34),"vnetNsgSecurityLevel",CHAR(34),": {",CHAR(34),"value",CHAR(34),":",CHAR(34),vnetNsgSecurityLevel,CHAR(34),"},",
 CHAR(34),"routeTableName",CHAR(34),": {",CHAR(34),"value",CHAR(34),":",CHAR(34),routeTableName,CHAR(34),"}"
 )</f>
-        <v>{"$schema":"https://schema.management.azure.com/schemas/2019-04-01/deploymentParameters.json#","contentVersion":"1.0.0.0","parameters":{"assetLocationURI": {"value":"https://raw.githubusercontent.com/mbakunas/Azure-HubSpoke/master/"},"vnetDdosProtectionLevel": {"value":"Standard - Create New"},"vnetDdosProtectionPlanName": {"value":"DDOS-Plan-01"},"vnetNsgSecurityLevel": {"value":"Medium"},"routeTableName": {"value":"RouteTable-01"}</v>
+        <v>{"$schema":"https://schema.management.azure.com/schemas/2019-04-01/deploymentParameters.json#","contentVersion":"1.0.0.0","parameters":{"assetLocationURI": {"value":"https://raw.githubusercontent.com/mbakunas/Azure-HubSpoke/master/"},"vnetDdosProtectionLevel": {"value":"Basic"},"vnetDdosProtectionPlanName": {"value":"DDOS-Plan-01"},"vnetNsgSecurityLevel": {"value":"Medium"},"routeTableName": {"value":"RouteTable-EastUS2-01"}</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" t="str">
         <f>_xlfn.CONCAT(
 CHAR(34), "hubVnetName", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), hubVnetName, CHAR(34), "},",
 CHAR(34), "hubVnetAddressSpace", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), hubVnetAddressSpace, CHAR(34), "},",
+CHAR(34), "hubDeploySubscriptionResourceGroup", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), hubDeploySubscriptionResourceGroup, CHAR(34), "},",
 CHAR(34), "hubSubnetGatewayAddressSpace", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), hubSubnetGatewayAddressSpace, CHAR(34), "},",
 CHAR(34), "hubSubnetFirewallAddressSpace", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), calcHhubSubnetFirewallAddressSpace, CHAR(34), "},",
 CHAR(34), "hubSubnetBastionAddressSpace", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), calcHubSubnetBastionAddressSpace, CHAR(34), "},",
@@ -1982,20 +2028,30 @@
 CHAR(34), "hubSubnet3Name", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), hubSubnet3Name, CHAR(34), "},",
 CHAR(34), "hubSubnet3AddressSpace", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), calcHubSubnet3AddressSpace, CHAR(34), "},",
 CHAR(34), "hubSubnet4Name", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), hubSubnet4Name, CHAR(34), "},",
-CHAR(34), "hubSubnet4AddressSpace", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), calcHubSubnet4AddressSpace, CHAR(34), "},",
+CHAR(34), "hubSubnet4AddressSpace", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), calcHubSubnet4AddressSpace, CHAR(34), "},"
+)</f>
+        <v>"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubDeploySubscriptionResourceGroup": {"value":"f0bb6c48-80fd-445c-98cb-c38b5f817d52/HubSpoke-01"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetBastionAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5" s="8" t="str">
+        <f>_xlfn.CONCAT(
 CHAR(34), "dcSubnetVmContAadGroupId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), dcAdminsAadGroupObjectId, CHAR(34), "},",
 CHAR(34), "dcVmContributorsRoleAssignmentID", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", dcVmContributorsRoleAssignmentID, "]},",
 CHAR(34), "hubSubnetVmContAadGroupId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), serverTeamAadGroupObjectId, CHAR(34), "},",
 CHAR(34), "hubSubnetVmContRoleAssignmantId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", hubSubnetVmContRoleAssignmantId, "]}"
 )</f>
-        <v>"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"10.0.0.64/26"},"hubSubnetBastionAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},"dcSubnetVmContAadGroupId": {"value":"83578c91-9919-4bd8-bee8-2649f6eb7c13"},"dcVmContributorsRoleAssignmentID": {"value":["184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"]},"hubSubnetVmContAadGroupId": {"value":"57f2ff92-300b-4075-a7ab-2030b46ebe2f"},"hubSubnetVmContRoleAssignmantId": {"value":["0702dcd4-0b65-4ebb-8ebd-873e2729904b","594fd8bf-f554-4272-8b19-9725c7b706b4","b3f5340d-28be-4029-bc10-56af7e20ac75","7a1689a7-66d8-4010-9213-c837316f8a30","d83bc577-1b03-4604-94a1-150ba7198ed0","6cba977a-462f-4d8c-b291-2dad991f85a0"]}</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B5" t="str">
+        <v>"dcSubnetVmContAadGroupId": {"value":"83578c91-9919-4bd8-bee8-2649f6eb7c13"},"dcVmContributorsRoleAssignmentID": {"value":["184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"]},"hubSubnetVmContAadGroupId": {"value":"57f2ff92-300b-4075-a7ab-2030b46ebe2f"},"hubSubnetVmContRoleAssignmantId": {"value":["0702dcd4-0b65-4ebb-8ebd-873e2729904b","594fd8bf-f554-4272-8b19-9725c7b706b4","b3f5340d-28be-4029-bc10-56af7e20ac75","7a1689a7-66d8-4010-9213-c837316f8a30","d83bc577-1b03-4604-94a1-150ba7198ed0","6cba977a-462f-4d8c-b291-2dad991f85a0"]}</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" t="str">
         <f>_xlfn.CONCAT(
 CHAR(34), "spokeVnetName", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", spokeVnetName, "]},",
 CHAR(34), "spokeVnetAddressSpace", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", spokeVnetAddressSpace,"]},",
@@ -2012,67 +2068,67 @@
 CHAR(34), "spokeVmContAadGroupId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", CHAR(34), appTeamsAadGroupObjectId, CHAR(34), "]},",
 CHAR(34), "spokeVmContributorsRoleAssignmentID", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", spokeVmContributorsRoleAssignmentID,"]}"
 )</f>
-        <v>"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01","Spoke-Dev-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16","10.3.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["","c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02","16936380-29b0-4326-8f6b-db86da154736/HubSpoke-03"]},"spokeSubnetBastionAddressSpace": {"value":["0.0.0.0/0"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25","10.3.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24","10.3.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24","10.3.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24","10.3.3.0/24"]},"spokeVmContAadGroupId": {"value":["002984bd-b5ce-445d-8138-d19b514550c7"]},"spokeVmContributorsRoleAssignmentID": {"value":["5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6","b2b76710-60c9-4826-b864-272c7c115806"]}</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B6" t="str">
+        <v>"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01","Spoke-Dev-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16","10.3.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["f0bb6c48-80fd-445c-98cb-c38b5f817d52/HubSpoke-01","c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02","16936380-29b0-4326-8f6b-db86da154736/HubSpoke-03"]},"spokeSubnetBastionAddressSpace": {"value":["0.0.0.0/0"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25","10.3.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24","10.3.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24","10.3.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24","10.3.3.0/24"]},"spokeVmContAadGroupId": {"value":["002984bd-b5ce-445d-8138-d19b514550c7"]},"spokeVmContributorsRoleAssignmentID": {"value":["5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6","b2b76710-60c9-4826-b864-272c7c115806"]}</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" t="str">
         <f>_xlfn.CONCAT(
 "}",
  "}")</f>
         <v>}}</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="B9" s="8"/>
-    </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>116</v>
-      </c>
-      <c r="B10" t="str">
-        <f>IF(hubSubnetFirewallDeploy = "Deploy", hubSubnetFirewallAddressSpace, "0.0.0.0/0")</f>
-        <v>10.0.0.64/26</v>
-      </c>
+      <c r="A10" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" s="9"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B11" t="str">
+        <f>IF(hubSubnetFirewallDeploy = "Deploy", hubSubnetFirewallAddressSpace, "0.0.0.0/0")</f>
+        <v>0.0.0.0/0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B12" t="str">
         <f>IF(hubSubnetBastionDeploy = "Deploy", hubSubnetBastionAddressSpace, "0.0.0.0/0")</f>
         <v>0.0.0.0/0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>118</v>
-      </c>
-      <c r="B12" t="str">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" t="str">
         <f>IF(hubSubnetJumpHostsDeploy = "Deploy", hubSubnetJumpHostsAddressSpace, "0.0.0.0/0")</f>
         <v>10.0.0.224/27</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>119</v>
-      </c>
-      <c r="B13" t="str">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>118</v>
+      </c>
+      <c r="B14" t="str">
         <f>IF(hubSubnet1Deploy = "Deploy", hubSubnet1AddressSpace, "0.0.0.0/0")</f>
         <v>10.0.1.0/27</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>120</v>
-      </c>
-      <c r="B14" t="str">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>119</v>
+      </c>
+      <c r="B15" t="str">
         <f>IF(
 OR(hubSubnet1Deploy = "Don't Deploy", hubSubnet2Deploy = "Don't Deploy"),
 "0.0.0.0/0",
@@ -2080,11 +2136,11 @@
         <v>10.0.1.32/27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>121</v>
-      </c>
-      <c r="B15" t="str">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>120</v>
+      </c>
+      <c r="B16" t="str">
         <f>IF(
 OR(hubSubnet1Deploy = "Don't Deploy", hubSubnet2Deploy = "Don't Deploy", hubSubnet3Deploy = "Don't Deploy"),
 "0.0.0.0/0",
@@ -2092,11 +2148,11 @@
         <v>10.0.1.64/27</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>122</v>
-      </c>
-      <c r="B16" t="str">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17" t="str">
         <f>IF(
 OR(hubSubnet1Deploy = "Don't Deploy", hubSubnet2Deploy = "Don't Deploy", hubSubnet3Deploy = "Don't Deploy", hubSubnet4Deploy = "Don't Deploy"),
 "0.0.0.0/0",
@@ -2104,18 +2160,9 @@
         <v>10.0.1.96/27</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>137</v>
-      </c>
-      <c r="B19" s="7" t="str">
-        <f>_xlfn.CONCAT("""", Hub!D15, """", ",", """", Hub!D16, """")</f>
-        <v>"184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"</v>
       </c>
     </row>
     <row r="20" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2123,57 +2170,66 @@
         <v>136</v>
       </c>
       <c r="B20" s="7" t="str">
+        <f>_xlfn.CONCAT("""", Hub!D18, """", ",", """", Hub!D19, """")</f>
+        <v>"184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B21" s="7" t="str">
         <f>_xlfn.CONCAT(
-"""", Hub!D22, """",
-IF(Hub!E17 = "Required", "," &amp; """" &amp; Hub!D17 &amp; """", ""),
-IF(Hub!E18 = "Required", "," &amp; """" &amp; Hub!D18 &amp; """", ""),
-IF(Hub!E19 = "Required", "," &amp; """" &amp; Hub!D19 &amp; """", ""),
+"""", Hub!D25, """",
 IF(Hub!E20 = "Required", "," &amp; """" &amp; Hub!D20 &amp; """", ""),
-IF(Hub!E21 = "Required", "," &amp; """" &amp; Hub!D21 &amp; """", "")
+IF(Hub!E21 = "Required", "," &amp; """" &amp; Hub!D21 &amp; """", ""),
+IF(Hub!E22 = "Required", "," &amp; """" &amp; Hub!D22 &amp; """", ""),
+IF(Hub!E23 = "Required", "," &amp; """" &amp; Hub!D23 &amp; """", ""),
+IF(Hub!E24 = "Required", "," &amp; """" &amp; Hub!D24 &amp; """", "")
 )</f>
         <v>"0702dcd4-0b65-4ebb-8ebd-873e2729904b","594fd8bf-f554-4272-8b19-9725c7b706b4","b3f5340d-28be-4029-bc10-56af7e20ac75","7a1689a7-66d8-4010-9213-c837316f8a30","d83bc577-1b03-4604-94a1-150ba7198ed0","6cba977a-462f-4d8c-b291-2dad991f85a0"</v>
       </c>
     </row>
-    <row r="21" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="B23" s="8"/>
-    </row>
+    <row r="23" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>81</v>
-      </c>
-      <c r="B24" t="str">
+      <c r="A24" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="9"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" t="str">
         <f>_xlfn.CONCAT(CHAR(34), Spoke1!$B$5, CHAR(34), ",", CHAR(34), Spoke2!$B$5, CHAR(34), ",", CHAR(34), Spoke3!$B$5, CHAR(34))</f>
         <v>"Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01","Spoke-Dev-EastUS2-01"</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>82</v>
-      </c>
-      <c r="B25" t="str">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" t="str">
         <f>_xlfn.CONCAT(CHAR(34), Spoke1!$C$5, CHAR(34), ",", CHAR(34), Spoke2!$C$5, CHAR(34), ",", CHAR(34), Spoke3!$C$5, CHAR(34))</f>
         <v>"10.1.0.0/16","10.2.0.0/16","10.3.0.0/16"</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>83</v>
-      </c>
-      <c r="B26" t="str">
-        <f>_xlfn.CONCAT(Spoke1!$D$2, ",", Spoke2!$D$2, ",", Spoke3!$D$2)</f>
-        <v>"","c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02","16936380-29b0-4326-8f6b-db86da154736/HubSpoke-03"</v>
-      </c>
-    </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B27" t="str">
+        <f>_xlfn.CONCAT(Spoke1!$D$2, ",", Spoke2!$D$2, ",", Spoke3!$D$2)</f>
+        <v>"f0bb6c48-80fd-445c-98cb-c38b5f817d52/HubSpoke-01","c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02","16936380-29b0-4326-8f6b-db86da154736/HubSpoke-03"</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" t="str">
         <f>IF(
 Spoke1!$E$7 = "Common",
 IF(Spoke1!$D$7 = "Don't Deploy", """"  &amp; "0.0.0.0/0" &amp; """", """" &amp;  Spoke1!$C$7 &amp; """" &amp; "," &amp;   """" &amp; Spoke2!$C$7  &amp; """" &amp; "," &amp;   """" &amp; Spoke3!$C$7),
@@ -2190,11 +2246,11 @@
         <v>"0.0.0.0/0"</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>86</v>
-      </c>
-      <c r="B28" s="5" t="str">
+    <row r="29" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" s="5" t="str">
         <f>IF(
 Spoke1!$E$8 = "Common",
 """" &amp; Spoke1!$B$8 &amp; """",
@@ -2203,11 +2259,11 @@
         <v>"AppGW"</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>87</v>
-      </c>
-      <c r="B29" s="3" t="str">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>86</v>
+      </c>
+      <c r="B30" s="3" t="str">
         <f>IF(
 Spoke1!$E$8 = "Common",
 IF(Spoke1!$D$8 = "Don't Deploy", """"  &amp; "0.0.0.0/0" &amp; """", """" &amp;  Spoke1!$C$8 &amp; """" &amp; "," &amp;   """" &amp; Spoke2!$C$8  &amp; """" &amp; "," &amp;   """" &amp; Spoke3!$C$8 &amp; """"),
@@ -2224,11 +2280,11 @@
         <v>"10.1.0.128/25","10.2.0.128/25","10.3.0.128/25"</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>90</v>
-      </c>
-      <c r="B30" s="5" t="str">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>89</v>
+      </c>
+      <c r="B31" s="5" t="str">
         <f>IF(
 Spoke1!$E$8 = "Common",
 """" &amp; Spoke1!$B$9 &amp; """",
@@ -2237,11 +2293,11 @@
         <v>"Subnet1"</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>91</v>
-      </c>
-      <c r="B31" s="3" t="str">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" s="3" t="str">
         <f>IF(
 Spoke1!$E$9 = "Common",
 IF(Spoke1!$D$9 = "Don't Deploy", """"  &amp; "0.0.0.0/0" &amp; """", """" &amp;  Spoke1!$C$9 &amp; """" &amp; "," &amp;   """" &amp; Spoke2!$C$9  &amp; """" &amp; "," &amp;   """" &amp; Spoke3!$C$9 &amp; """"),
@@ -2258,11 +2314,11 @@
         <v>"10.1.1.0/24","10.2.1.0/24","10.3.1.0/24"</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>92</v>
-      </c>
-      <c r="B32" s="5" t="str">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>91</v>
+      </c>
+      <c r="B33" s="5" t="str">
         <f>IF(
 Spoke1!$E$10 = "Common",
 """" &amp; Spoke1!$B$10 &amp; """",
@@ -2271,11 +2327,11 @@
         <v>"Subnet2"</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>93</v>
-      </c>
-      <c r="B33" s="3" t="str">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>92</v>
+      </c>
+      <c r="B34" s="3" t="str">
         <f>IF(
 Spoke1!$E$10 = "Common",
 IF(Spoke1!$D$10 = "Don't Deploy", """"  &amp; "0.0.0.0/0" &amp; """", """" &amp;  Spoke1!$C$10 &amp; """" &amp; "," &amp;   """" &amp; Spoke2!$C$10  &amp; """" &amp; "," &amp;   """" &amp; Spoke3!$C$10 &amp; """"),
@@ -2292,11 +2348,11 @@
         <v>"10.1.2.0/24","10.2.2.0/24","10.3.2.0/24"</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>94</v>
-      </c>
-      <c r="B34" s="5" t="str">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>93</v>
+      </c>
+      <c r="B35" s="5" t="str">
         <f>IF(
 Spoke1!$E$8 = "Common",
 """" &amp; Spoke1!$B$11 &amp; """",
@@ -2305,11 +2361,11 @@
         <v>"Subnet3"</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>95</v>
-      </c>
-      <c r="B35" s="3" t="str">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>94</v>
+      </c>
+      <c r="B36" s="3" t="str">
         <f>IF(
 Spoke1!$E$11 = "Common",
 IF(OR(Spoke1!$D$11 = "Don't Deploy", Spoke1!$D$10 = "Don't Deploy"),
@@ -2330,19 +2386,19 @@
         <v>"10.1.3.0/24","10.2.3.0/24","10.3.3.0/24"</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>127</v>
-      </c>
-      <c r="B36" t="str">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>126</v>
+      </c>
+      <c r="B37" t="str">
         <f>_xlfn.CONCAT("""",Spoke1!D15,"""",",","""",Spoke2!D15,"""",",","""",Spoke3!D15,"""")</f>
         <v>"5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6","b2b76710-60c9-4826-b864-272c7c115806"</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2373,10 +2429,10 @@
         <v>31</v>
       </c>
       <c r="E1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2384,35 +2440,35 @@
         <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3" t="s">
         <v>64</v>
       </c>
       <c r="E3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Switched deployment scope to management group
</commit_message>
<xml_diff>
--- a/PowerShell/ParametersFileBuilder_3-Spoke.xlsx
+++ b/PowerShell/ParametersFileBuilder_3-Spoke.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mark.bakunas\Documents\GitHub\Azure-HubSpoke\PowerShell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D61806-ED20-454A-AE11-5DE83A0D631D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A98FAE7-D045-408E-A9D0-16293F67EDED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="1860" windowWidth="21600" windowHeight="11385" xr2:uid="{74A5C2AD-3876-4989-8818-24030CBF60E7}"/>
+    <workbookView xWindow="31125" yWindow="1980" windowWidth="21600" windowHeight="11385" xr2:uid="{74A5C2AD-3876-4989-8818-24030CBF60E7}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="4" r:id="rId1"/>
@@ -22,8 +22,9 @@
     <sheet name="Lists" sheetId="9" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="appTeamsAadGroupObjectId">General!$B$12</definedName>
+    <definedName name="appTeamsAadGroupObjectId">General!$B$13</definedName>
     <definedName name="assetLocationURI">General!$B$2</definedName>
+    <definedName name="AzureRegions">Lists!$I$2:$I$42</definedName>
     <definedName name="calcHhubSubnetFirewallAddressSpace">ParametersFile!$B$11</definedName>
     <definedName name="calcHubSubnet1AddressSpace">ParametersFile!$B$14</definedName>
     <definedName name="calcHubSubnet2AddressSpace">ParametersFile!$B$15</definedName>
@@ -31,7 +32,7 @@
     <definedName name="calcHubSubnet4AddressSpace">ParametersFile!$B$17</definedName>
     <definedName name="calcHubSubnetBastionAddressSpace">ParametersFile!$B$12</definedName>
     <definedName name="calcHubSubnetJumpHostsAddressSpace">ParametersFile!$B$13</definedName>
-    <definedName name="dcAdminsAadGroupObjectId">General!$B$10</definedName>
+    <definedName name="dcAdminsAadGroupObjectId">General!$B$11</definedName>
     <definedName name="dcVmContributorsRoleAssignmentID">ParametersFile!$B$20</definedName>
     <definedName name="deployOptions_List">Lists!$E$2:$E$3</definedName>
     <definedName name="hubDeploySubscriptionResourceGroup">Hub!$D$2</definedName>
@@ -60,8 +61,9 @@
     <definedName name="hubSubnetVmContRoleAssignmantId">ParametersFile!$B$21</definedName>
     <definedName name="hubVnetAddressSpace">Hub!$C$5</definedName>
     <definedName name="hubVnetName">Hub!$B$5</definedName>
+    <definedName name="resourceGroupsRegion">General!$B$8</definedName>
     <definedName name="routeTableName">General!$B$7</definedName>
-    <definedName name="serverTeamAadGroupObjectId">General!$B$11</definedName>
+    <definedName name="serverTeamAadGroupObjectId">General!$B$12</definedName>
     <definedName name="spokeDeploySubscriptionResourceGroup">ParametersFile!$B$27</definedName>
     <definedName name="spokeSubnet1AddressSpace">ParametersFile!$B$32</definedName>
     <definedName name="spokeSubnet1Name">ParametersFile!$B$31</definedName>
@@ -100,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="189">
   <si>
     <t>Name</t>
   </si>
@@ -538,6 +540,135 @@
   </si>
   <si>
     <t>RouteTable-EastUS2-01</t>
+  </si>
+  <si>
+    <t>Resource Group Azure Region</t>
+  </si>
+  <si>
+    <t>Azure Regions</t>
+  </si>
+  <si>
+    <t>East Asia</t>
+  </si>
+  <si>
+    <t>Southeast Asia</t>
+  </si>
+  <si>
+    <t>Central US</t>
+  </si>
+  <si>
+    <t>East US</t>
+  </si>
+  <si>
+    <t>East US 2</t>
+  </si>
+  <si>
+    <t>West US</t>
+  </si>
+  <si>
+    <t>North Central US</t>
+  </si>
+  <si>
+    <t>South Central US</t>
+  </si>
+  <si>
+    <t>North Europe</t>
+  </si>
+  <si>
+    <t>West Europe</t>
+  </si>
+  <si>
+    <t>Japan West</t>
+  </si>
+  <si>
+    <t>Japan East</t>
+  </si>
+  <si>
+    <t>Brazil South</t>
+  </si>
+  <si>
+    <t>Australia East</t>
+  </si>
+  <si>
+    <t>Australia Southeast</t>
+  </si>
+  <si>
+    <t>South India</t>
+  </si>
+  <si>
+    <t>Central India</t>
+  </si>
+  <si>
+    <t>West India</t>
+  </si>
+  <si>
+    <t>Canada Central</t>
+  </si>
+  <si>
+    <t>Canada East</t>
+  </si>
+  <si>
+    <t>UK South</t>
+  </si>
+  <si>
+    <t>UK West</t>
+  </si>
+  <si>
+    <t>West Central US</t>
+  </si>
+  <si>
+    <t>West US 2</t>
+  </si>
+  <si>
+    <t>Korea Central</t>
+  </si>
+  <si>
+    <t>Korea South</t>
+  </si>
+  <si>
+    <t>France Central</t>
+  </si>
+  <si>
+    <t>France South</t>
+  </si>
+  <si>
+    <t>Australia Central</t>
+  </si>
+  <si>
+    <t>Australia Central 2</t>
+  </si>
+  <si>
+    <t>UAE Central</t>
+  </si>
+  <si>
+    <t>UAE North</t>
+  </si>
+  <si>
+    <t>South Africa North</t>
+  </si>
+  <si>
+    <t>South Africa West</t>
+  </si>
+  <si>
+    <t>Switzerland North</t>
+  </si>
+  <si>
+    <t>Switzerland West</t>
+  </si>
+  <si>
+    <t>Germany North</t>
+  </si>
+  <si>
+    <t>Germany West Central</t>
+  </si>
+  <si>
+    <t>Norway West</t>
+  </si>
+  <si>
+    <t>Norway East</t>
+  </si>
+  <si>
+    <t>Brazil Southeast</t>
   </si>
 </sst>
 </file>
@@ -600,7 +731,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
@@ -610,6 +741,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -934,10 +1066,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27806494-5F45-4C9A-ADBE-3476E1448E75}">
-  <dimension ref="A2:B12"/>
+  <dimension ref="A2:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,45 +1119,56 @@
         <v>145</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>95</v>
-      </c>
-      <c r="B9" t="s">
-        <v>127</v>
+    <row r="8" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>130</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>138</v>
+        <v>95</v>
+      </c>
+      <c r="B10" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>128</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>140</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{96676D08-4819-43A2-BFC9-9A9587D2C709}">
       <formula1>vnetDdosProtectionLevel_List</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="NSG Security Level" prompt="The level of NSG rule security restrictions._x000a_Low = only the default rules._x000a_Medium = inbound restrictions but allowing intra-subnet traffic._x000a_High = micro-segmentation." sqref="B6" xr:uid="{5171F9AB-7721-4324-A490-715DDC661BFC}">
       <formula1>vnetNsgSecurityLevel_List</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8" xr:uid="{637E07F8-6F84-4F5D-ACF6-FF1D4B2D1FC6}">
+      <formula1>AzureRegions</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -1984,7 +2127,7 @@
       </c>
       <c r="B1" s="4" t="str">
         <f>_xlfn.CONCAT(B3, ",", B4, B5, ",", B6,  B7)</f>
-        <v>{"$schema":"https://schema.management.azure.com/schemas/2019-04-01/deploymentParameters.json#","contentVersion":"1.0.0.0","parameters":{"assetLocationURI": {"value":"https://raw.githubusercontent.com/mbakunas/Azure-HubSpoke/master/"},"vnetDdosProtectionLevel": {"value":"Basic"},"vnetDdosProtectionPlanName": {"value":"DDOS-Plan-01"},"vnetNsgSecurityLevel": {"value":"Medium"},"routeTableName": {"value":"RouteTable-EastUS2-01"},"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubDeploySubscriptionResourceGroup": {"value":"f0bb6c48-80fd-445c-98cb-c38b5f817d52/HubSpoke-01"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetBastionAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},"dcSubnetVmContAadGroupId": {"value":"83578c91-9919-4bd8-bee8-2649f6eb7c13"},"dcVmContributorsRoleAssignmentID": {"value":["184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"]},"hubSubnetVmContAadGroupId": {"value":"57f2ff92-300b-4075-a7ab-2030b46ebe2f"},"hubSubnetVmContRoleAssignmantId": {"value":["0702dcd4-0b65-4ebb-8ebd-873e2729904b","594fd8bf-f554-4272-8b19-9725c7b706b4","b3f5340d-28be-4029-bc10-56af7e20ac75","7a1689a7-66d8-4010-9213-c837316f8a30","d83bc577-1b03-4604-94a1-150ba7198ed0","6cba977a-462f-4d8c-b291-2dad991f85a0"]},"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01","Spoke-Dev-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16","10.3.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["f0bb6c48-80fd-445c-98cb-c38b5f817d52/HubSpoke-01","c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02","16936380-29b0-4326-8f6b-db86da154736/HubSpoke-03"]},"spokeSubnetBastionAddressSpace": {"value":["0.0.0.0/0"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25","10.3.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24","10.3.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24","10.3.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24","10.3.3.0/24"]},"spokeVmContAadGroupId": {"value":["002984bd-b5ce-445d-8138-d19b514550c7"]},"spokeVmContributorsRoleAssignmentID": {"value":["5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6","b2b76710-60c9-4826-b864-272c7c115806"]}}}</v>
+        <v>{"$schema":"https://schema.management.azure.com/schemas/2019-04-01/deploymentParameters.json#","contentVersion":"1.0.0.0","parameters":{"assetLocationURI": {"value":"https://raw.githubusercontent.com/mbakunas/Azure-HubSpoke/master/"},"resourceGroupsRegion": {"value":"East US 2"},"vnetDdosProtectionLevel": {"value":"Basic"},"vnetDdosProtectionPlanName": {"value":"DDOS-Plan-01"},"vnetNsgSecurityLevel": {"value":"Medium"},"routeTableName": {"value":"RouteTable-EastUS2-01"},"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubDeploySubscriptionResourceGroup": {"value":"f0bb6c48-80fd-445c-98cb-c38b5f817d52/HubSpoke-01"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetBastionAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},"dcSubnetVmContAadGroupId": {"value":"83578c91-9919-4bd8-bee8-2649f6eb7c13"},"dcVmContributorsRoleAssignmentID": {"value":["184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"]},"hubSubnetVmContAadGroupId": {"value":"57f2ff92-300b-4075-a7ab-2030b46ebe2f"},"hubSubnetVmContRoleAssignmantId": {"value":["0702dcd4-0b65-4ebb-8ebd-873e2729904b","594fd8bf-f554-4272-8b19-9725c7b706b4","b3f5340d-28be-4029-bc10-56af7e20ac75","7a1689a7-66d8-4010-9213-c837316f8a30","d83bc577-1b03-4604-94a1-150ba7198ed0","6cba977a-462f-4d8c-b291-2dad991f85a0"]},"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01","Spoke-Dev-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16","10.3.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["f0bb6c48-80fd-445c-98cb-c38b5f817d52/HubSpoke-01","c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02","16936380-29b0-4326-8f6b-db86da154736/HubSpoke-03"]},"spokeSubnetBastionAddressSpace": {"value":["0.0.0.0/0"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25","10.3.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24","10.3.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24","10.3.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24","10.3.3.0/24"]},"spokeVmContAadGroupId": {"value":["002984bd-b5ce-445d-8138-d19b514550c7"]},"spokeVmContributorsRoleAssignmentID": {"value":["5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6","b2b76710-60c9-4826-b864-272c7c115806"]}}}</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1997,12 +2140,13 @@
 CHAR(34),"contentVersion",CHAR(34),":",CHAR(34),"1.0.0.0",CHAR(34),",",
 CHAR(34),"parameters",CHAR(34),":","{",
 CHAR(34),"assetLocationURI",CHAR(34),": {",CHAR(34),"value",CHAR(34),":",CHAR(34),assetLocationURI,CHAR(34),"},",
+CHAR(34),"resourceGroupsRegion",CHAR(34),": {",CHAR(34),"value",CHAR(34),":",CHAR(34),resourceGroupsRegion,CHAR(34),"},",
 CHAR(34),"vnetDdosProtectionLevel",CHAR(34),": {",CHAR(34),"value",CHAR(34),":",CHAR(34),vnetDdosProtectionLevel,CHAR(34),"},",
 CHAR(34),"vnetDdosProtectionPlanName",CHAR(34),": {",CHAR(34),"value",CHAR(34),":",CHAR(34),vnetDdosProtectionPlanName,CHAR(34),"},",
 CHAR(34),"vnetNsgSecurityLevel",CHAR(34),": {",CHAR(34),"value",CHAR(34),":",CHAR(34),vnetNsgSecurityLevel,CHAR(34),"},",
 CHAR(34),"routeTableName",CHAR(34),": {",CHAR(34),"value",CHAR(34),":",CHAR(34),routeTableName,CHAR(34),"}"
 )</f>
-        <v>{"$schema":"https://schema.management.azure.com/schemas/2019-04-01/deploymentParameters.json#","contentVersion":"1.0.0.0","parameters":{"assetLocationURI": {"value":"https://raw.githubusercontent.com/mbakunas/Azure-HubSpoke/master/"},"vnetDdosProtectionLevel": {"value":"Basic"},"vnetDdosProtectionPlanName": {"value":"DDOS-Plan-01"},"vnetNsgSecurityLevel": {"value":"Medium"},"routeTableName": {"value":"RouteTable-EastUS2-01"}</v>
+        <v>{"$schema":"https://schema.management.azure.com/schemas/2019-04-01/deploymentParameters.json#","contentVersion":"1.0.0.0","parameters":{"assetLocationURI": {"value":"https://raw.githubusercontent.com/mbakunas/Azure-HubSpoke/master/"},"resourceGroupsRegion": {"value":"East US 2"},"vnetDdosProtectionLevel": {"value":"Basic"},"vnetDdosProtectionPlanName": {"value":"DDOS-Plan-01"},"vnetNsgSecurityLevel": {"value":"Medium"},"routeTableName": {"value":"RouteTable-EastUS2-01"}</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2083,10 +2227,10 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="B10" s="9"/>
+      <c r="B10" s="10"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -2193,10 +2337,10 @@
     <row r="22" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B24" s="9"/>
+      <c r="B24" s="10"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -2407,10 +2551,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CC06067-7B7A-4158-B8EE-51370472C64C}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G3"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2419,9 +2563,10 @@
     <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -2434,8 +2579,11 @@
       <c r="G1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -2448,8 +2596,11 @@
       <c r="G2" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I2" s="9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>108</v>
       </c>
@@ -2462,16 +2613,215 @@
       <c r="G3" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I3" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>109</v>
       </c>
       <c r="C4" t="s">
         <v>111</v>
       </c>
+      <c r="I4" s="9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I5" s="9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I6" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I7" s="9" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I8" s="9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I9" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I10" s="9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I11" s="9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I12" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I13" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I14" s="9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I15" s="9" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I16" s="9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I17" s="9" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="18" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I18" s="9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="19" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I19" s="9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="20" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I20" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I21" s="9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="22" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I22" s="9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="23" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I23" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="24" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I24" s="9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="25" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I25" s="9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="26" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I26" s="9" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="27" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I27" s="9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="28" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I28" s="9" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="29" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I29" s="9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="30" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I30" s="9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="31" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I31" s="9" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="32" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I32" s="9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I33" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="34" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I34" s="9" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="35" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I35" s="9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="36" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I36" s="9" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="37" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I37" s="9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="38" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I38" s="9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="39" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I39" s="9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="40" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I40" s="9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="41" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I41" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="42" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I42" s="9" t="s">
+        <v>171</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I2:I42">
+    <sortCondition ref="I2:I42"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added resource group RBAC
</commit_message>
<xml_diff>
--- a/PowerShell/ParametersFileBuilder_3-Spoke.xlsx
+++ b/PowerShell/ParametersFileBuilder_3-Spoke.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mark.bakunas\Documents\GitHub\Azure-HubSpoke\PowerShell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A98FAE7-D045-408E-A9D0-16293F67EDED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC856769-101F-4044-A61B-375498C461D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31125" yWindow="1980" windowWidth="21600" windowHeight="11385" xr2:uid="{74A5C2AD-3876-4989-8818-24030CBF60E7}"/>
+    <workbookView xWindow="2370" yWindow="900" windowWidth="21600" windowHeight="11385" xr2:uid="{74A5C2AD-3876-4989-8818-24030CBF60E7}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="4" r:id="rId1"/>
@@ -25,15 +25,15 @@
     <definedName name="appTeamsAadGroupObjectId">General!$B$13</definedName>
     <definedName name="assetLocationURI">General!$B$2</definedName>
     <definedName name="AzureRegions">Lists!$I$2:$I$42</definedName>
-    <definedName name="calcHhubSubnetFirewallAddressSpace">ParametersFile!$B$11</definedName>
-    <definedName name="calcHubSubnet1AddressSpace">ParametersFile!$B$14</definedName>
-    <definedName name="calcHubSubnet2AddressSpace">ParametersFile!$B$15</definedName>
-    <definedName name="calcHubSubnet3AddressSpace">ParametersFile!$B$16</definedName>
-    <definedName name="calcHubSubnet4AddressSpace">ParametersFile!$B$17</definedName>
-    <definedName name="calcHubSubnetBastionAddressSpace">ParametersFile!$B$12</definedName>
-    <definedName name="calcHubSubnetJumpHostsAddressSpace">ParametersFile!$B$13</definedName>
+    <definedName name="calcHhubSubnetFirewallAddressSpace">ParametersFile!$B$12</definedName>
+    <definedName name="calcHubSubnet1AddressSpace">ParametersFile!$B$15</definedName>
+    <definedName name="calcHubSubnet2AddressSpace">ParametersFile!$B$16</definedName>
+    <definedName name="calcHubSubnet3AddressSpace">ParametersFile!$B$17</definedName>
+    <definedName name="calcHubSubnet4AddressSpace">ParametersFile!$B$18</definedName>
+    <definedName name="calcHubSubnetBastionAddressSpace">ParametersFile!$B$13</definedName>
+    <definedName name="calcHubSubnetJumpHostsAddressSpace">ParametersFile!$B$14</definedName>
     <definedName name="dcAdminsAadGroupObjectId">General!$B$11</definedName>
-    <definedName name="dcVmContributorsRoleAssignmentID">ParametersFile!$B$20</definedName>
+    <definedName name="dcVmContributorsRoleAssignmentID">ParametersFile!$B$21</definedName>
     <definedName name="deployOptions_List">Lists!$E$2:$E$3</definedName>
     <definedName name="hubDeploySubscriptionResourceGroup">Hub!$D$2</definedName>
     <definedName name="hubSubnet1AddressSpace">Hub!$C$12</definedName>
@@ -58,26 +58,30 @@
     <definedName name="hubSubnetJumpHostsAddressSpace">Hub!$C$11</definedName>
     <definedName name="hubSubnetJumpHostsDeploy">Hub!$D$11</definedName>
     <definedName name="hubSubnetJumpHostsName">Hub!$B$11</definedName>
-    <definedName name="hubSubnetVmContRoleAssignmantId">ParametersFile!$B$21</definedName>
+    <definedName name="hubSubnetVmContRoleAssignmantId">ParametersFile!$B$22</definedName>
     <definedName name="hubVnetAddressSpace">Hub!$C$5</definedName>
     <definedName name="hubVnetName">Hub!$B$5</definedName>
+    <definedName name="networkAdmins">General!$B$14</definedName>
+    <definedName name="networkContributorsAadGroupId">ParametersFile!$B$41</definedName>
+    <definedName name="networkContributorsRoleAssignmentId">ParametersFile!$B$42</definedName>
+    <definedName name="ResourceGroups">Hub:Spoke3!$C$2</definedName>
     <definedName name="resourceGroupsRegion">General!$B$8</definedName>
     <definedName name="routeTableName">General!$B$7</definedName>
     <definedName name="serverTeamAadGroupObjectId">General!$B$12</definedName>
-    <definedName name="spokeDeploySubscriptionResourceGroup">ParametersFile!$B$27</definedName>
-    <definedName name="spokeSubnet1AddressSpace">ParametersFile!$B$32</definedName>
-    <definedName name="spokeSubnet1Name">ParametersFile!$B$31</definedName>
-    <definedName name="spokeSubnet2AddressSpace">ParametersFile!$B$34</definedName>
-    <definedName name="spokeSubnet2Name">ParametersFile!$B$33</definedName>
-    <definedName name="spokeSubnet3AddressSpace">ParametersFile!$B$36</definedName>
-    <definedName name="spokeSubnet3Name">ParametersFile!$B$35</definedName>
-    <definedName name="spokeSubnetAppGwAddressSpace">ParametersFile!$B$30</definedName>
-    <definedName name="spokeSubnetAppGwName">ParametersFile!$B$29</definedName>
-    <definedName name="spokeSubnetBastionAddressSpace">ParametersFile!$B$28</definedName>
+    <definedName name="spokeDeploySubscriptionResourceGroup">ParametersFile!$B$28</definedName>
+    <definedName name="spokeSubnet1AddressSpace">ParametersFile!$B$33</definedName>
+    <definedName name="spokeSubnet1Name">ParametersFile!$B$32</definedName>
+    <definedName name="spokeSubnet2AddressSpace">ParametersFile!$B$35</definedName>
+    <definedName name="spokeSubnet2Name">ParametersFile!$B$34</definedName>
+    <definedName name="spokeSubnet3AddressSpace">ParametersFile!$B$37</definedName>
+    <definedName name="spokeSubnet3Name">ParametersFile!$B$36</definedName>
+    <definedName name="spokeSubnetAppGwAddressSpace">ParametersFile!$B$31</definedName>
+    <definedName name="spokeSubnetAppGwName">ParametersFile!$B$30</definedName>
+    <definedName name="spokeSubnetBastionAddressSpace">ParametersFile!$B$29</definedName>
     <definedName name="spokeSubnetUniqueness_List">Lists!$G$2:$G$3</definedName>
-    <definedName name="spokeVmContributorsRoleAssignmentID">ParametersFile!$B$37</definedName>
-    <definedName name="spokeVnetAddressSpace">ParametersFile!$B$26</definedName>
-    <definedName name="spokeVnetName">ParametersFile!$B$25</definedName>
+    <definedName name="spokeVmContributorsRoleAssignmentID">ParametersFile!$B$38</definedName>
+    <definedName name="spokeVnetAddressSpace">ParametersFile!$B$27</definedName>
+    <definedName name="spokeVnetName">ParametersFile!$B$26</definedName>
     <definedName name="vnetDdosProtectionLevel">General!$B$4</definedName>
     <definedName name="vnetDdosProtectionLevel_List">Lists!$A$2:$A$4</definedName>
     <definedName name="vnetDdosProtectionPlanName">General!$B$5</definedName>
@@ -102,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="199">
   <si>
     <t>Name</t>
   </si>
@@ -356,9 +360,6 @@
     <t>c64ca001-2cce-46de-837e-03f5564fc802</t>
   </si>
   <si>
-    <t>HubSpoke-02</t>
-  </si>
-  <si>
     <t>spokeSubnetAppGwName</t>
   </si>
   <si>
@@ -404,9 +405,6 @@
     <t>16936380-29b0-4326-8f6b-db86da154736</t>
   </si>
   <si>
-    <t>HubSpoke-03</t>
-  </si>
-  <si>
     <t>Spoke-Dev-EastUS2-01</t>
   </si>
   <si>
@@ -533,9 +531,6 @@
     <t>f0bb6c48-80fd-445c-98cb-c38b5f817d52</t>
   </si>
   <si>
-    <t>HubSpoke-01</t>
-  </si>
-  <si>
     <t>Hub RBAC</t>
   </si>
   <si>
@@ -669,6 +664,45 @@
   </si>
   <si>
     <t>Brazil Southeast</t>
+  </si>
+  <si>
+    <t>Nework contributors</t>
+  </si>
+  <si>
+    <t>931fbead-2296-4d2b-ac29-da61f92c413b</t>
+  </si>
+  <si>
+    <t>networkContributorsRoleAssignmentId</t>
+  </si>
+  <si>
+    <t>8e5b5f19-21b9-4ed9-b601-799b23a5a1a8</t>
+  </si>
+  <si>
+    <t>HS-01</t>
+  </si>
+  <si>
+    <t>HS-02</t>
+  </si>
+  <si>
+    <t>f4c29215-1369-42c2-8e19-055adfaa7bd4</t>
+  </si>
+  <si>
+    <t>f9370c43-cf0d-42d3-b83d-6f3412e5f5ee</t>
+  </si>
+  <si>
+    <t>Resource group RBAC values</t>
+  </si>
+  <si>
+    <t>networkContributorsAadGroupId</t>
+  </si>
+  <si>
+    <t>Resource group RBAC</t>
+  </si>
+  <si>
+    <t>Guids for network contributors role assignment (one per resource group)</t>
+  </si>
+  <si>
+    <t>HS-03</t>
   </si>
 </sst>
 </file>
@@ -731,7 +765,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
@@ -745,6 +779,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1066,10 +1104,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27806494-5F45-4C9A-ADBE-3476E1448E75}">
-  <dimension ref="A2:B13"/>
+  <dimension ref="A2:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1116,50 +1154,81 @@
         <v>65</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>186</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="B17" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="1" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A16:A18"/>
+  </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{96676D08-4819-43A2-BFC9-9A9587D2C709}">
       <formula1>vnetDdosProtectionLevel_List</formula1>
@@ -1184,7 +1253,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1203,7 +1272,7 @@
         <v>43</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1211,14 +1280,14 @@
         <v>41</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>143</v>
+        <v>190</v>
       </c>
       <c r="D2" s="8" t="str">
         <f>_xlfn.CONCAT(B2, "/", C2)</f>
-        <v>f0bb6c48-80fd-445c-98cb-c38b5f817d52/HubSpoke-01</v>
+        <v>f0bb6c48-80fd-445c-98cb-c38b5f817d52/HS-01</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -1261,7 +1330,7 @@
         <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1272,7 +1341,7 @@
         <v>15</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1297,7 +1366,7 @@
         <v>20</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1311,7 +1380,7 @@
         <v>25</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1325,7 +1394,7 @@
         <v>26</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1339,7 +1408,7 @@
         <v>27</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1353,7 +1422,7 @@
         <v>28</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1372,7 +1441,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B18" t="s">
         <v>46</v>
@@ -1384,12 +1453,12 @@
         <v>50</v>
       </c>
       <c r="E18" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B19" t="s">
         <v>54</v>
@@ -1407,7 +1476,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B20" t="s">
         <v>46</v>
@@ -1425,7 +1494,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B21" t="s">
         <v>46</v>
@@ -1443,7 +1512,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B22" t="s">
         <v>46</v>
@@ -1463,7 +1532,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B23" t="s">
         <v>46</v>
@@ -1483,7 +1552,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B24" t="s">
         <v>46</v>
@@ -1503,7 +1572,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B25" t="s">
         <v>54</v>
@@ -1512,10 +1581,10 @@
         <v>2</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E25" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1535,7 +1604,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1562,14 +1631,14 @@
         <v>41</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>143</v>
+        <v>190</v>
       </c>
       <c r="D2" t="str">
         <f>IF(B2 &lt;&gt; "", _xlfn.CONCAT(CHAR(34), B2, "/", C2, CHAR(34)), _xlfn.CONCAT("""", """"))</f>
-        <v>"f0bb6c48-80fd-445c-98cb-c38b5f817d52/HubSpoke-01"</v>
+        <v>"f0bb6c48-80fd-445c-98cb-c38b5f817d52/HS-01"</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1603,10 +1672,10 @@
         <v>37</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1620,10 +1689,10 @@
         <v>36</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1637,7 +1706,7 @@
         <v>38</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1651,10 +1720,10 @@
         <v>39</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1668,10 +1737,10 @@
         <v>40</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1690,7 +1759,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B14" t="s">
         <v>46</v>
@@ -1726,7 +1795,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1756,11 +1825,11 @@
         <v>83</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>84</v>
+        <v>191</v>
       </c>
       <c r="D2" t="str">
         <f>IF(B2 &lt;&gt; "", _xlfn.CONCAT(CHAR(34), B2, "/", C2, CHAR(34)), _xlfn.CONCAT("""", """"))</f>
-        <v>"c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02"</v>
+        <v>"c64ca001-2cce-46de-837e-03f5564fc802/HS-02"</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1794,7 +1863,7 @@
         <v>73</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E7" t="str">
         <f>Spoke1!E7</f>
@@ -1812,7 +1881,7 @@
         <v>74</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E8" t="str">
         <f>Spoke1!E8</f>
@@ -1845,7 +1914,7 @@
         <v>76</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E10" t="str">
         <f>Spoke1!E10</f>
@@ -1863,7 +1932,7 @@
         <v>77</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E11" t="str">
         <f>Spoke1!E11</f>
@@ -1886,7 +1955,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B14" t="s">
         <v>46</v>
@@ -1919,7 +1988,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1946,14 +2015,14 @@
         <v>41</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>100</v>
+        <v>198</v>
       </c>
       <c r="D2" t="str">
         <f>IF(B2 &lt;&gt; "", _xlfn.CONCAT(CHAR(34), B2, "/", C2, CHAR(34)), _xlfn.CONCAT("""", """"))</f>
-        <v>"16936380-29b0-4326-8f6b-db86da154736/HubSpoke-03"</v>
+        <v>"16936380-29b0-4326-8f6b-db86da154736/HS-03"</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1969,10 +2038,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1984,10 +2053,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E7" t="str">
         <f>Spoke1!E7</f>
@@ -2002,10 +2071,10 @@
         <v>33</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E8" t="str">
         <f>Spoke1!E8</f>
@@ -2020,7 +2089,7 @@
         <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E9" t="str">
         <f>Spoke1!E9</f>
@@ -2035,10 +2104,10 @@
         <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E10" t="str">
         <f>Spoke1!E10</f>
@@ -2053,10 +2122,10 @@
         <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E11" t="str">
         <f>Spoke1!E11</f>
@@ -2079,7 +2148,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B14" t="s">
         <v>46</v>
@@ -2088,12 +2157,12 @@
         <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D15" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2109,7 +2178,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E5F0421-4CC3-4847-AE8E-9E8CD1C6E8C6}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -2126,8 +2195,8 @@
         <v>69</v>
       </c>
       <c r="B1" s="4" t="str">
-        <f>_xlfn.CONCAT(B3, ",", B4, B5, ",", B6,  B7)</f>
-        <v>{"$schema":"https://schema.management.azure.com/schemas/2019-04-01/deploymentParameters.json#","contentVersion":"1.0.0.0","parameters":{"assetLocationURI": {"value":"https://raw.githubusercontent.com/mbakunas/Azure-HubSpoke/master/"},"resourceGroupsRegion": {"value":"East US 2"},"vnetDdosProtectionLevel": {"value":"Basic"},"vnetDdosProtectionPlanName": {"value":"DDOS-Plan-01"},"vnetNsgSecurityLevel": {"value":"Medium"},"routeTableName": {"value":"RouteTable-EastUS2-01"},"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubDeploySubscriptionResourceGroup": {"value":"f0bb6c48-80fd-445c-98cb-c38b5f817d52/HubSpoke-01"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetBastionAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},"dcSubnetVmContAadGroupId": {"value":"83578c91-9919-4bd8-bee8-2649f6eb7c13"},"dcVmContributorsRoleAssignmentID": {"value":["184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"]},"hubSubnetVmContAadGroupId": {"value":"57f2ff92-300b-4075-a7ab-2030b46ebe2f"},"hubSubnetVmContRoleAssignmantId": {"value":["0702dcd4-0b65-4ebb-8ebd-873e2729904b","594fd8bf-f554-4272-8b19-9725c7b706b4","b3f5340d-28be-4029-bc10-56af7e20ac75","7a1689a7-66d8-4010-9213-c837316f8a30","d83bc577-1b03-4604-94a1-150ba7198ed0","6cba977a-462f-4d8c-b291-2dad991f85a0"]},"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01","Spoke-Dev-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16","10.3.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["f0bb6c48-80fd-445c-98cb-c38b5f817d52/HubSpoke-01","c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02","16936380-29b0-4326-8f6b-db86da154736/HubSpoke-03"]},"spokeSubnetBastionAddressSpace": {"value":["0.0.0.0/0"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25","10.3.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24","10.3.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24","10.3.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24","10.3.3.0/24"]},"spokeVmContAadGroupId": {"value":["002984bd-b5ce-445d-8138-d19b514550c7"]},"spokeVmContributorsRoleAssignmentID": {"value":["5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6","b2b76710-60c9-4826-b864-272c7c115806"]}}}</v>
+        <f>_xlfn.CONCAT(B3, ",", B4, B5, B6, ",", B7,  B8)</f>
+        <v>{"$schema":"https://schema.management.azure.com/schemas/2019-04-01/deploymentParameters.json#","contentVersion":"1.0.0.0","parameters":{"assetLocationURI": {"value":"https://raw.githubusercontent.com/mbakunas/Azure-HubSpoke/master/"},"resourceGroupsRegion": {"value":"East US 2"},"vnetDdosProtectionLevel": {"value":"Basic"},"vnetDdosProtectionPlanName": {"value":"DDOS-Plan-01"},"vnetNsgSecurityLevel": {"value":"Medium"},"routeTableName": {"value":"RouteTable-EastUS2-01"},"networkContributorsAadGroupId": {"value":"931fbead-2296-4d2b-ac29-da61f92c413b"},"networkContributorsRoleAssignmentId": {"value":["8e5b5f19-21b9-4ed9-b601-799b23a5a1a8","f4c29215-1369-42c2-8e19-055adfaa7bd4","f9370c43-cf0d-42d3-b83d-6f3412e5f5ee"]},"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubDeploySubscriptionResourceGroup": {"value":"f0bb6c48-80fd-445c-98cb-c38b5f817d52/HS-01"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetBastionAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},"dcSubnetVmContAadGroupId": {"value":"83578c91-9919-4bd8-bee8-2649f6eb7c13"},"dcVmContributorsRoleAssignmentID": {"value":["184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"]},"hubSubnetVmContAadGroupId": {"value":"57f2ff92-300b-4075-a7ab-2030b46ebe2f"},"hubSubnetVmContRoleAssignmantId": {"value":["0702dcd4-0b65-4ebb-8ebd-873e2729904b","594fd8bf-f554-4272-8b19-9725c7b706b4","b3f5340d-28be-4029-bc10-56af7e20ac75","7a1689a7-66d8-4010-9213-c837316f8a30","d83bc577-1b03-4604-94a1-150ba7198ed0","6cba977a-462f-4d8c-b291-2dad991f85a0"]},"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01","Spoke-Dev-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16","10.3.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["f0bb6c48-80fd-445c-98cb-c38b5f817d52/HS-01","c64ca001-2cce-46de-837e-03f5564fc802/HS-02","16936380-29b0-4326-8f6b-db86da154736/HS-03"]},"spokeSubnetBastionAddressSpace": {"value":["0.0.0.0/0"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25","10.3.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24","10.3.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24","10.3.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24","10.3.3.0/24"]},"spokeVmContAadGroupId": {"value":["002984bd-b5ce-445d-8138-d19b514550c7"]},"spokeVmContributorsRoleAssignmentID": {"value":["5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6","b2b76710-60c9-4826-b864-272c7c115806"]}}}</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2149,11 +2218,23 @@
         <v>{"$schema":"https://schema.management.azure.com/schemas/2019-04-01/deploymentParameters.json#","contentVersion":"1.0.0.0","parameters":{"assetLocationURI": {"value":"https://raw.githubusercontent.com/mbakunas/Azure-HubSpoke/master/"},"resourceGroupsRegion": {"value":"East US 2"},"vnetDdosProtectionLevel": {"value":"Basic"},"vnetDdosProtectionPlanName": {"value":"DDOS-Plan-01"},"vnetNsgSecurityLevel": {"value":"Medium"},"routeTableName": {"value":"RouteTable-EastUS2-01"}</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:2" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="B4" s="10" t="str">
+        <f>_xlfn.CONCAT(
+CHAR(34), "networkContributorsAadGroupId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), networkContributorsAadGroupId, CHAR(34), "},",
+CHAR(34), "networkContributorsRoleAssignmentId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", networkContributorsRoleAssignmentId, "]},"
+)</f>
+        <v>"networkContributorsAadGroupId": {"value":"931fbead-2296-4d2b-ac29-da61f92c413b"},"networkContributorsRoleAssignmentId": {"value":["8e5b5f19-21b9-4ed9-b601-799b23a5a1a8","f4c29215-1369-42c2-8e19-055adfaa7bd4","f9370c43-cf0d-42d3-b83d-6f3412e5f5ee"]},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>67</v>
       </c>
-      <c r="B4" t="str">
+      <c r="B5" t="str">
         <f>_xlfn.CONCAT(
 CHAR(34), "hubVnetName", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), hubVnetName, CHAR(34), "},",
 CHAR(34), "hubVnetAddressSpace", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), hubVnetAddressSpace, CHAR(34), "},",
@@ -2174,14 +2255,14 @@
 CHAR(34), "hubSubnet4Name", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), hubSubnet4Name, CHAR(34), "},",
 CHAR(34), "hubSubnet4AddressSpace", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), calcHubSubnet4AddressSpace, CHAR(34), "},"
 )</f>
-        <v>"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubDeploySubscriptionResourceGroup": {"value":"f0bb6c48-80fd-445c-98cb-c38b5f817d52/HubSpoke-01"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetBastionAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="B5" s="8" t="str">
+        <v>"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubDeploySubscriptionResourceGroup": {"value":"f0bb6c48-80fd-445c-98cb-c38b5f817d52/HS-01"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetBastionAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B6" s="8" t="str">
         <f>_xlfn.CONCAT(
 CHAR(34), "dcSubnetVmContAadGroupId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), dcAdminsAadGroupObjectId, CHAR(34), "},",
 CHAR(34), "dcVmContributorsRoleAssignmentID", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", dcVmContributorsRoleAssignmentID, "]},",
@@ -2191,11 +2272,11 @@
         <v>"dcSubnetVmContAadGroupId": {"value":"83578c91-9919-4bd8-bee8-2649f6eb7c13"},"dcVmContributorsRoleAssignmentID": {"value":["184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"]},"hubSubnetVmContAadGroupId": {"value":"57f2ff92-300b-4075-a7ab-2030b46ebe2f"},"hubSubnetVmContRoleAssignmantId": {"value":["0702dcd4-0b65-4ebb-8ebd-873e2729904b","594fd8bf-f554-4272-8b19-9725c7b706b4","b3f5340d-28be-4029-bc10-56af7e20ac75","7a1689a7-66d8-4010-9213-c837316f8a30","d83bc577-1b03-4604-94a1-150ba7198ed0","6cba977a-462f-4d8c-b291-2dad991f85a0"]}</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>70</v>
       </c>
-      <c r="B6" t="str">
+      <c r="B7" t="str">
         <f>_xlfn.CONCAT(
 CHAR(34), "spokeVnetName", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", spokeVnetName, "]},",
 CHAR(34), "spokeVnetAddressSpace", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", spokeVnetAddressSpace,"]},",
@@ -2212,67 +2293,67 @@
 CHAR(34), "spokeVmContAadGroupId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", CHAR(34), appTeamsAadGroupObjectId, CHAR(34), "]},",
 CHAR(34), "spokeVmContributorsRoleAssignmentID", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", spokeVmContributorsRoleAssignmentID,"]}"
 )</f>
-        <v>"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01","Spoke-Dev-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16","10.3.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["f0bb6c48-80fd-445c-98cb-c38b5f817d52/HubSpoke-01","c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02","16936380-29b0-4326-8f6b-db86da154736/HubSpoke-03"]},"spokeSubnetBastionAddressSpace": {"value":["0.0.0.0/0"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25","10.3.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24","10.3.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24","10.3.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24","10.3.3.0/24"]},"spokeVmContAadGroupId": {"value":["002984bd-b5ce-445d-8138-d19b514550c7"]},"spokeVmContributorsRoleAssignmentID": {"value":["5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6","b2b76710-60c9-4826-b864-272c7c115806"]}</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+        <v>"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01","Spoke-Dev-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16","10.3.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["f0bb6c48-80fd-445c-98cb-c38b5f817d52/HS-01","c64ca001-2cce-46de-837e-03f5564fc802/HS-02","16936380-29b0-4326-8f6b-db86da154736/HS-03"]},"spokeSubnetBastionAddressSpace": {"value":["0.0.0.0/0"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25","10.3.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24","10.3.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24","10.3.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24","10.3.3.0/24"]},"spokeVmContAadGroupId": {"value":["002984bd-b5ce-445d-8138-d19b514550c7"]},"spokeVmContributorsRoleAssignmentID": {"value":["5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6","b2b76710-60c9-4826-b864-272c7c115806"]}</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>68</v>
       </c>
-      <c r="B7" t="str">
+      <c r="B8" t="str">
         <f>_xlfn.CONCAT(
 "}",
  "}")</f>
         <v>}}</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="B10" s="10"/>
-    </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>115</v>
-      </c>
-      <c r="B11" t="str">
+      <c r="A11" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B11" s="11"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B12" t="str">
         <f>IF(hubSubnetFirewallDeploy = "Deploy", hubSubnetFirewallAddressSpace, "0.0.0.0/0")</f>
         <v>0.0.0.0/0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>116</v>
-      </c>
-      <c r="B12" t="str">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13" t="str">
         <f>IF(hubSubnetBastionDeploy = "Deploy", hubSubnetBastionAddressSpace, "0.0.0.0/0")</f>
         <v>0.0.0.0/0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B13" t="str">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>115</v>
+      </c>
+      <c r="B14" t="str">
         <f>IF(hubSubnetJumpHostsDeploy = "Deploy", hubSubnetJumpHostsAddressSpace, "0.0.0.0/0")</f>
         <v>10.0.0.224/27</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>118</v>
-      </c>
-      <c r="B14" t="str">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>116</v>
+      </c>
+      <c r="B15" t="str">
         <f>IF(hubSubnet1Deploy = "Deploy", hubSubnet1AddressSpace, "0.0.0.0/0")</f>
         <v>10.0.1.0/27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>119</v>
-      </c>
-      <c r="B15" t="str">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>117</v>
+      </c>
+      <c r="B16" t="str">
         <f>IF(
 OR(hubSubnet1Deploy = "Don't Deploy", hubSubnet2Deploy = "Don't Deploy"),
 "0.0.0.0/0",
@@ -2280,11 +2361,11 @@
         <v>10.0.1.32/27</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>120</v>
-      </c>
-      <c r="B16" t="str">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>118</v>
+      </c>
+      <c r="B17" t="str">
         <f>IF(
 OR(hubSubnet1Deploy = "Don't Deploy", hubSubnet2Deploy = "Don't Deploy", hubSubnet3Deploy = "Don't Deploy"),
 "0.0.0.0/0",
@@ -2292,11 +2373,11 @@
         <v>10.0.1.64/27</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>121</v>
-      </c>
-      <c r="B17" t="str">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B18" t="str">
         <f>IF(
 OR(hubSubnet1Deploy = "Don't Deploy", hubSubnet2Deploy = "Don't Deploy", hubSubnet3Deploy = "Don't Deploy", hubSubnet4Deploy = "Don't Deploy"),
 "0.0.0.0/0",
@@ -2304,25 +2385,25 @@
         <v>10.0.1.96/27</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="B20" s="7" t="str">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B21" s="7" t="str">
         <f>_xlfn.CONCAT("""", Hub!D18, """", ",", """", Hub!D19, """")</f>
         <v>"184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"</v>
       </c>
     </row>
-    <row r="21" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="B21" s="7" t="str">
+    <row r="22" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B22" s="7" t="str">
         <f>_xlfn.CONCAT(
 """", Hub!D25, """",
 IF(Hub!E20 = "Required", "," &amp; """" &amp; Hub!D20 &amp; """", ""),
@@ -2334,46 +2415,46 @@
         <v>"0702dcd4-0b65-4ebb-8ebd-873e2729904b","594fd8bf-f554-4272-8b19-9725c7b706b4","b3f5340d-28be-4029-bc10-56af7e20ac75","7a1689a7-66d8-4010-9213-c837316f8a30","d83bc577-1b03-4604-94a1-150ba7198ed0","6cba977a-462f-4d8c-b291-2dad991f85a0"</v>
       </c>
     </row>
-    <row r="22" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="B24" s="10"/>
-    </row>
+    <row r="24" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25" s="11"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>80</v>
       </c>
-      <c r="B25" t="str">
+      <c r="B26" t="str">
         <f>_xlfn.CONCAT(CHAR(34), Spoke1!$B$5, CHAR(34), ",", CHAR(34), Spoke2!$B$5, CHAR(34), ",", CHAR(34), Spoke3!$B$5, CHAR(34))</f>
         <v>"Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01","Spoke-Dev-EastUS2-01"</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>81</v>
       </c>
-      <c r="B26" t="str">
+      <c r="B27" t="str">
         <f>_xlfn.CONCAT(CHAR(34), Spoke1!$C$5, CHAR(34), ",", CHAR(34), Spoke2!$C$5, CHAR(34), ",", CHAR(34), Spoke3!$C$5, CHAR(34))</f>
         <v>"10.1.0.0/16","10.2.0.0/16","10.3.0.0/16"</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>82</v>
-      </c>
-      <c r="B27" t="str">
-        <f>_xlfn.CONCAT(Spoke1!$D$2, ",", Spoke2!$D$2, ",", Spoke3!$D$2)</f>
-        <v>"f0bb6c48-80fd-445c-98cb-c38b5f817d52/HubSpoke-01","c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02","16936380-29b0-4326-8f6b-db86da154736/HubSpoke-03"</v>
-      </c>
-    </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B28" t="str">
+        <f>_xlfn.CONCAT(Spoke1!$D$2, ",", Spoke2!$D$2, ",", Spoke3!$D$2)</f>
+        <v>"f0bb6c48-80fd-445c-98cb-c38b5f817d52/HS-01","c64ca001-2cce-46de-837e-03f5564fc802/HS-02","16936380-29b0-4326-8f6b-db86da154736/HS-03"</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" t="str">
         <f>IF(
 Spoke1!$E$7 = "Common",
 IF(Spoke1!$D$7 = "Don't Deploy", """"  &amp; "0.0.0.0/0" &amp; """", """" &amp;  Spoke1!$C$7 &amp; """" &amp; "," &amp;   """" &amp; Spoke2!$C$7  &amp; """" &amp; "," &amp;   """" &amp; Spoke3!$C$7),
@@ -2390,11 +2471,11 @@
         <v>"0.0.0.0/0"</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>85</v>
-      </c>
-      <c r="B29" s="5" t="str">
+    <row r="30" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="5" t="str">
         <f>IF(
 Spoke1!$E$8 = "Common",
 """" &amp; Spoke1!$B$8 &amp; """",
@@ -2403,11 +2484,11 @@
         <v>"AppGW"</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>86</v>
-      </c>
-      <c r="B30" s="3" t="str">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" s="3" t="str">
         <f>IF(
 Spoke1!$E$8 = "Common",
 IF(Spoke1!$D$8 = "Don't Deploy", """"  &amp; "0.0.0.0/0" &amp; """", """" &amp;  Spoke1!$C$8 &amp; """" &amp; "," &amp;   """" &amp; Spoke2!$C$8  &amp; """" &amp; "," &amp;   """" &amp; Spoke3!$C$8 &amp; """"),
@@ -2424,11 +2505,11 @@
         <v>"10.1.0.128/25","10.2.0.128/25","10.3.0.128/25"</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>89</v>
-      </c>
-      <c r="B31" s="5" t="str">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" s="5" t="str">
         <f>IF(
 Spoke1!$E$8 = "Common",
 """" &amp; Spoke1!$B$9 &amp; """",
@@ -2437,11 +2518,11 @@
         <v>"Subnet1"</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>90</v>
-      </c>
-      <c r="B32" s="3" t="str">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" s="3" t="str">
         <f>IF(
 Spoke1!$E$9 = "Common",
 IF(Spoke1!$D$9 = "Don't Deploy", """"  &amp; "0.0.0.0/0" &amp; """", """" &amp;  Spoke1!$C$9 &amp; """" &amp; "," &amp;   """" &amp; Spoke2!$C$9  &amp; """" &amp; "," &amp;   """" &amp; Spoke3!$C$9 &amp; """"),
@@ -2458,11 +2539,11 @@
         <v>"10.1.1.0/24","10.2.1.0/24","10.3.1.0/24"</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>91</v>
-      </c>
-      <c r="B33" s="5" t="str">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>90</v>
+      </c>
+      <c r="B34" s="5" t="str">
         <f>IF(
 Spoke1!$E$10 = "Common",
 """" &amp; Spoke1!$B$10 &amp; """",
@@ -2471,11 +2552,11 @@
         <v>"Subnet2"</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>92</v>
-      </c>
-      <c r="B34" s="3" t="str">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>91</v>
+      </c>
+      <c r="B35" s="3" t="str">
         <f>IF(
 Spoke1!$E$10 = "Common",
 IF(Spoke1!$D$10 = "Don't Deploy", """"  &amp; "0.0.0.0/0" &amp; """", """" &amp;  Spoke1!$C$10 &amp; """" &amp; "," &amp;   """" &amp; Spoke2!$C$10  &amp; """" &amp; "," &amp;   """" &amp; Spoke3!$C$10 &amp; """"),
@@ -2492,11 +2573,11 @@
         <v>"10.1.2.0/24","10.2.2.0/24","10.3.2.0/24"</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>93</v>
-      </c>
-      <c r="B35" s="5" t="str">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>92</v>
+      </c>
+      <c r="B36" s="5" t="str">
         <f>IF(
 Spoke1!$E$8 = "Common",
 """" &amp; Spoke1!$B$11 &amp; """",
@@ -2505,11 +2586,11 @@
         <v>"Subnet3"</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>94</v>
-      </c>
-      <c r="B36" s="3" t="str">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37" s="3" t="str">
         <f>IF(
 Spoke1!$E$11 = "Common",
 IF(OR(Spoke1!$D$11 = "Don't Deploy", Spoke1!$D$10 = "Don't Deploy"),
@@ -2530,19 +2611,42 @@
         <v>"10.1.3.0/24","10.2.3.0/24","10.3.3.0/24"</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>126</v>
-      </c>
-      <c r="B37" t="str">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>124</v>
+      </c>
+      <c r="B38" t="str">
         <f>_xlfn.CONCAT("""",Spoke1!D15,"""",",","""",Spoke2!D15,"""",",","""",Spoke3!D15,"""")</f>
         <v>"5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6","b2b76710-60c9-4826-b864-272c7c115806"</v>
       </c>
     </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="B41" t="str">
+        <f>networkAdmins</f>
+        <v>931fbead-2296-4d2b-ac29-da61f92c413b</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>188</v>
+      </c>
+      <c r="B42" t="str">
+        <f>_xlfn.CONCAT("""", General!B16, """", ",", """", General!B17, """", ",", """", General!B18, """")</f>
+        <v>"8e5b5f19-21b9-4ed9-b601-799b23a5a1a8","f4c29215-1369-42c2-8e19-055adfaa7bd4","f9370c43-cf0d-42d3-b83d-6f3412e5f5ee"</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A25:B25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2553,8 +2657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CC06067-7B7A-4158-B8EE-51370472C64C}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2574,13 +2678,13 @@
         <v>31</v>
       </c>
       <c r="E1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2588,234 +2692,234 @@
         <v>62</v>
       </c>
       <c r="C2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" t="s">
         <v>110</v>
       </c>
-      <c r="E2" t="s">
-        <v>112</v>
-      </c>
       <c r="G2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C3" t="s">
         <v>64</v>
       </c>
       <c r="E3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" t="s">
         <v>109</v>
       </c>
-      <c r="C4" t="s">
-        <v>111</v>
-      </c>
       <c r="I4" s="9" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I5" s="9" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I6" s="9" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I7" s="9" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I8" s="9" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I9" s="9" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I10" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I11" s="9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I12" s="9" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I13" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I14" s="9" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I15" s="9" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I16" s="9" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I17" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="18" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I18" s="9" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I19" s="9" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I20" s="9" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I21" s="9" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="22" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I22" s="9" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="23" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I23" s="9" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I24" s="9" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="25" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I25" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="26" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I26" s="9" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="27" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I27" s="9" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="28" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I28" s="9" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="29" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I29" s="9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I30" s="9" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="31" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I31" s="9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="32" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I32" s="9" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="33" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I33" s="9" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I34" s="9" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="35" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I35" s="9" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="36" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I36" s="9" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="37" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I37" s="9" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="38" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I38" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="39" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I39" s="9" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="40" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I40" s="9" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="41" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I41" s="9" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="42" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I42" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moved subscription/RGs to General tab
</commit_message>
<xml_diff>
--- a/PowerShell/ParametersFileBuilder_3-Spoke.xlsx
+++ b/PowerShell/ParametersFileBuilder_3-Spoke.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mark.bakunas\Documents\GitHub\Azure-HubSpoke\PowerShell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFEAB753-00B3-48C5-9A5B-5896F29EB9EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6823CC3-5213-40A1-AAD8-82C815DE55A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2370" yWindow="900" windowWidth="21600" windowHeight="11385" xr2:uid="{74A5C2AD-3876-4989-8818-24030CBF60E7}"/>
+    <workbookView xWindow="3600" yWindow="630" windowWidth="21600" windowHeight="14655" xr2:uid="{74A5C2AD-3876-4989-8818-24030CBF60E7}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,8 @@
     <definedName name="dcAdminsAadGroupObjectId">General!$B$11</definedName>
     <definedName name="dcVmContributorsRoleAssignmentID">ParametersFile!$B$21</definedName>
     <definedName name="deployOptions_List">Lists!$E$2:$E$3</definedName>
-    <definedName name="hubDeploySubscriptionResourceGroup">Hub!$D$2</definedName>
+    <definedName name="deploySubscriptionResourceGroup">Lists!$K$2:$K$5</definedName>
+    <definedName name="hubDeploySubscriptionResourceGroup">Hub!$B$2</definedName>
     <definedName name="hubSubnet1AddressSpace">Hub!$C$12</definedName>
     <definedName name="hubSubnet1Deploy">Hub!$D$12</definedName>
     <definedName name="hubSubnet1Name">Hub!$B$12</definedName>
@@ -106,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="209">
   <si>
     <t>Name</t>
   </si>
@@ -234,9 +235,6 @@
     <t>Deployment location</t>
   </si>
   <si>
-    <t>SubscriptionID</t>
-  </si>
-  <si>
     <t>Resource Group</t>
   </si>
   <si>
@@ -525,9 +523,6 @@
     <t>002984bd-b5ce-445d-8138-d19b514550c7</t>
   </si>
   <si>
-    <t>hubDeploySubscriptionResourceGroup</t>
-  </si>
-  <si>
     <t>f0bb6c48-80fd-445c-98cb-c38b5f817d52</t>
   </si>
   <si>
@@ -678,12 +673,6 @@
     <t>8e5b5f19-21b9-4ed9-b601-799b23a5a1a8</t>
   </si>
   <si>
-    <t>HS-01</t>
-  </si>
-  <si>
-    <t>HS-02</t>
-  </si>
-  <si>
     <t>f4c29215-1369-42c2-8e19-055adfaa7bd4</t>
   </si>
   <si>
@@ -699,10 +688,52 @@
     <t>Resource group RBAC</t>
   </si>
   <si>
-    <t>Guids for network contributors role assignment (one per resource group)</t>
-  </si>
-  <si>
-    <t>HS-03</t>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>Subscription ID</t>
+  </si>
+  <si>
+    <t>Resource Group Name</t>
+  </si>
+  <si>
+    <t>Network role assignment ID</t>
+  </si>
+  <si>
+    <t>fac1ea11-e5a7-4e74-8d7e-965344c54f56</t>
+  </si>
+  <si>
+    <t>8d7739f2-1859-44c0-a184-b45e84ba363d</t>
+  </si>
+  <si>
+    <t>CoreNetwork-01</t>
+  </si>
+  <si>
+    <t>CoreNetwork-02</t>
+  </si>
+  <si>
+    <t>CoreNetwork-03</t>
+  </si>
+  <si>
+    <t>CoreNetwork-04</t>
+  </si>
+  <si>
+    <t>deploySubscriptionResourceGroup</t>
+  </si>
+  <si>
+    <t>f0bb6c48-80fd-445c-98cb-c38b5f817d52/CoreNetwork-01</t>
+  </si>
+  <si>
+    <t>c64ca001-2cce-46de-837e-03f5564fc802/CoreNetwork-02</t>
+  </si>
+  <si>
+    <t>fac1ea11-e5a7-4e74-8d7e-965344c54f56/CoreNetwork-03</t>
+  </si>
+  <si>
+    <t>16936380-29b0-4326-8f6b-db86da154736/CoreNetwork-04</t>
+  </si>
+  <si>
+    <t>Resource Groups (up to 4 in any combination of subscriptions, don't enter more than are used)</t>
   </si>
 </sst>
 </file>
@@ -765,7 +796,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
@@ -779,10 +810,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1104,25 +1134,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27806494-5F45-4C9A-ADBE-3476E1448E75}">
-  <dimension ref="A2:B18"/>
+  <dimension ref="A2:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A16" sqref="A16:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="78.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1130,7 +1161,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1138,7 +1169,7 @@
         <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1146,89 +1177,134 @@
         <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="B16" s="12"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>193</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C17" t="s">
+        <v>195</v>
+      </c>
+      <c r="D17" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C20" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="1" t="s">
-        <v>193</v>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>198</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A16:B16"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{96676D08-4819-43A2-BFC9-9A9587D2C709}">
       <formula1>vnetDdosProtectionLevel_List</formula1>
@@ -1253,7 +1329,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1265,30 +1341,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>139</v>
-      </c>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D2" s="8" t="str">
-        <f>_xlfn.CONCAT(B2, "/", C2)</f>
-        <v>f0bb6c48-80fd-445c-98cb-c38b5f817d52/HS-01</v>
-      </c>
+      <c r="B2" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1330,7 +1395,7 @@
         <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1341,7 +1406,7 @@
         <v>15</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1366,7 +1431,7 @@
         <v>20</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1380,7 +1445,7 @@
         <v>25</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1394,7 +1459,7 @@
         <v>26</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1408,7 +1473,7 @@
         <v>27</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1422,52 +1487,52 @@
         <v>28</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" t="s">
         <v>44</v>
       </c>
-      <c r="B17" t="s">
-        <v>45</v>
-      </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E19" t="str">
         <f>IF(dcAdminsAadGroupObjectId = "", "Not needed", "Required")</f>
@@ -1476,16 +1541,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C20" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E20" t="str">
         <f>IF(hubSubnetJumpHostsDeploy = "Deploy", "Required", "Not Needed")</f>
@@ -1494,16 +1559,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E21" s="7" t="str">
         <f>IF(hubSubnet1Deploy = "Don't Deploy", "Not Needed", "Required")</f>
@@ -1512,16 +1577,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E22" s="7" t="str">
         <f>IF(
@@ -1532,16 +1597,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C23" t="s">
         <v>10</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E23" s="7" t="str">
         <f>IF(
@@ -1552,16 +1617,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C24" t="s">
         <v>11</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E24" s="7" t="str">
         <f>IF(
@@ -1572,26 +1637,33 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C25" t="s">
         <v>2</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:D9 D11:D15" xr:uid="{D9354EF7-27D1-4C1F-B57B-07A789DEC96E}">
       <formula1>deployOptions_List</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C2" xr:uid="{2E60E4C6-90C3-4006-952F-A9D87C061684}">
+      <formula1>OFFSET(deploySubscriptionResourceGroup, 0, 0, COUNTIF(deploySubscriptionResourceGroup,"*/*"))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1604,7 +1676,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1616,30 +1688,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+      <c r="B1" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" t="s">
-        <v>82</v>
-      </c>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D2" t="str">
-        <f>IF(B2 &lt;&gt; "", _xlfn.CONCAT(CHAR(34), B2, "/", C2, CHAR(34)), _xlfn.CONCAT("""", """"))</f>
-        <v>"f0bb6c48-80fd-445c-98cb-c38b5f817d52/HS-01"</v>
-      </c>
+      <c r="B2" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="C2" s="13"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -1672,10 +1733,10 @@
         <v>37</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1689,10 +1750,10 @@
         <v>36</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1706,7 +1767,7 @@
         <v>38</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1720,10 +1781,10 @@
         <v>39</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1737,52 +1798,59 @@
         <v>40</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s">
         <v>44</v>
       </c>
-      <c r="B13" t="s">
-        <v>45</v>
-      </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D15" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <mergeCells count="2">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D8 D10:D11" xr:uid="{0CD32938-FC7D-4A2D-89DA-FA2CAD0BA150}">
       <formula1>deployOptions_List</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E11" xr:uid="{EBB888DC-D06B-428F-9A6F-3A30046B1109}">
       <formula1>spokeSubnetUniqueness_List</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C2" xr:uid="{053EDBAA-1350-43DF-9970-8F5A43FEFE3D}">
+      <formula1>OFFSET(deploySubscriptionResourceGroup, 0, 0, COUNTIF(deploySubscriptionResourceGroup,"*/*"))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1795,7 +1863,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1807,30 +1875,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+      <c r="B1" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" t="s">
-        <v>82</v>
-      </c>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D2" t="str">
-        <f>IF(B2 &lt;&gt; "", _xlfn.CONCAT(CHAR(34), B2, "/", C2, CHAR(34)), _xlfn.CONCAT("""", """"))</f>
-        <v>"c64ca001-2cce-46de-837e-03f5564fc802/HS-02"</v>
-      </c>
+      <c r="B2" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="C2" s="13"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -1845,10 +1902,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1860,10 +1917,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E7" t="str">
         <f>Spoke1!E7</f>
@@ -1878,10 +1935,10 @@
         <v>33</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E8" t="str">
         <f>Spoke1!E8</f>
@@ -1896,7 +1953,7 @@
         <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E9" t="str">
         <f>Spoke1!E9</f>
@@ -1911,10 +1968,10 @@
         <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E10" t="str">
         <f>Spoke1!E10</f>
@@ -1929,10 +1986,10 @@
         <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E11" t="str">
         <f>Spoke1!E11</f>
@@ -1941,41 +1998,48 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s">
         <v>44</v>
       </c>
-      <c r="B13" t="s">
-        <v>45</v>
-      </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D15" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <mergeCells count="2">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D8 D10:D11" xr:uid="{01786FD6-A133-4CF7-BD55-62BA227952C7}">
       <formula1>deployOptions_List</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C2" xr:uid="{730CD524-8872-40A7-9E15-B3C5DCC3B13A}">
+      <formula1>OFFSET(deploySubscriptionResourceGroup, 0, 0, COUNTIF(deploySubscriptionResourceGroup,"*/*"))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1988,7 +2052,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2000,30 +2064,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+      <c r="B1" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" t="s">
-        <v>82</v>
-      </c>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D2" t="str">
-        <f>IF(B2 &lt;&gt; "", _xlfn.CONCAT(CHAR(34), B2, "/", C2, CHAR(34)), _xlfn.CONCAT("""", """"))</f>
-        <v>"16936380-29b0-4326-8f6b-db86da154736/HS-03"</v>
-      </c>
+      <c r="B2" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="C2" s="13"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -2038,10 +2091,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2053,10 +2106,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E7" t="str">
         <f>Spoke1!E7</f>
@@ -2071,10 +2124,10 @@
         <v>33</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E8" t="str">
         <f>Spoke1!E8</f>
@@ -2089,7 +2142,7 @@
         <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E9" t="str">
         <f>Spoke1!E9</f>
@@ -2104,10 +2157,10 @@
         <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E10" t="str">
         <f>Spoke1!E10</f>
@@ -2122,10 +2175,10 @@
         <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E11" t="str">
         <f>Spoke1!E11</f>
@@ -2134,41 +2187,48 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s">
         <v>44</v>
       </c>
-      <c r="B13" t="s">
-        <v>45</v>
-      </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D15" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <mergeCells count="2">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D8 D10:D11" xr:uid="{18BEFA5C-BFE0-444D-A090-ECC81E547311}">
       <formula1>deployOptions_List</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C2" xr:uid="{8CBD754D-140D-4828-ABAB-ED9BEE7D3127}">
+      <formula1>OFFSET(deploySubscriptionResourceGroup, 0, 0, COUNTIF(deploySubscriptionResourceGroup,"*/*"))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2192,16 +2252,16 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" s="4" t="str">
         <f>_xlfn.CONCAT(B3, ",", B4, B5, B6, ",", B7,  B8)</f>
-        <v>{"$schema":"https://schema.management.azure.com/schemas/2019-04-01/deploymentParameters.json#","contentVersion":"1.0.0.0","parameters":{"assetLocationURI": {"value":"https://raw.githubusercontent.com/mbakunas/Azure-HubSpoke/master/"},"resourceGroupsRegion": {"value":"East US 2"},"vnetDdosProtectionLevel": {"value":"Standard - Create New"},"vnetDdosProtectionPlanName": {"value":"DDOS-Plan-01"},"vnetNsgSecurityLevel": {"value":"Medium"},"routeTableName": {"value":"RouteTable-EastUS2-01"},"networkContributorsAadGroupId": {"value":"931fbead-2296-4d2b-ac29-da61f92c413b"},"networkContributorsRoleAssignmentId": {"value":["8e5b5f19-21b9-4ed9-b601-799b23a5a1a8","f4c29215-1369-42c2-8e19-055adfaa7bd4","f9370c43-cf0d-42d3-b83d-6f3412e5f5ee"]},"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubDeploySubscriptionResourceGroup": {"value":"f0bb6c48-80fd-445c-98cb-c38b5f817d52/HS-01"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"10.0.0.64/26"},"hubSubnetBastionAddressSpace": {"value":"10.0.0.128/26"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},"dcSubnetVmContAadGroupId": {"value":"83578c91-9919-4bd8-bee8-2649f6eb7c13"},"dcVmContributorsRoleAssignmentID": {"value":["184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"]},"hubSubnetVmContAadGroupId": {"value":"57f2ff92-300b-4075-a7ab-2030b46ebe2f"},"hubSubnetVmContRoleAssignmantId": {"value":["0702dcd4-0b65-4ebb-8ebd-873e2729904b","594fd8bf-f554-4272-8b19-9725c7b706b4","b3f5340d-28be-4029-bc10-56af7e20ac75","7a1689a7-66d8-4010-9213-c837316f8a30","d83bc577-1b03-4604-94a1-150ba7198ed0","6cba977a-462f-4d8c-b291-2dad991f85a0"]},"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01","Spoke-Dev-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16","10.3.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["f0bb6c48-80fd-445c-98cb-c38b5f817d52/HS-01","c64ca001-2cce-46de-837e-03f5564fc802/HS-02","16936380-29b0-4326-8f6b-db86da154736/HS-03"]},"spokeSubnetBastionAddressSpace": {"value":["10.1.0.0/26","10.2.0.0/26","10.3.0.0/26"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25","10.3.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24","10.3.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24","10.3.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24","10.3.3.0/24"]},"spokeVmContAadGroupId": {"value":["002984bd-b5ce-445d-8138-d19b514550c7"]},"spokeVmContributorsRoleAssignmentID": {"value":["5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6","b2b76710-60c9-4826-b864-272c7c115806"]}}}</v>
+        <v>{"$schema":"https://schema.management.azure.com/schemas/2019-04-01/deploymentParameters.json#","contentVersion":"1.0.0.0","parameters":{"assetLocationURI": {"value":"https://raw.githubusercontent.com/mbakunas/Azure-HubSpoke/master/"},"resourceGroupsRegion": {"value":"East US 2"},"vnetDdosProtectionLevel": {"value":"Standard - Create New"},"vnetDdosProtectionPlanName": {"value":"DDOS-Plan-01"},"vnetNsgSecurityLevel": {"value":"Medium"},"routeTableName": {"value":"RouteTable-EastUS2-01"},"networkContributorsAadGroupId": {"value":"931fbead-2296-4d2b-ac29-da61f92c413b"},"networkContributorsRoleAssignmentId": {"value":["8e5b5f19-21b9-4ed9-b601-799b23a5a1a8","f4c29215-1369-42c2-8e19-055adfaa7bd4","f9370c43-cf0d-42d3-b83d-6f3412e5f5ee","8d7739f2-1859-44c0-a184-b45e84ba363d"]},"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubDeploySubscriptionResourceGroup": {"value":"f0bb6c48-80fd-445c-98cb-c38b5f817d52/CoreNetwork-01"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"10.0.0.64/26"},"hubSubnetBastionAddressSpace": {"value":"10.0.0.128/26"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},"dcSubnetVmContAadGroupId": {"value":"83578c91-9919-4bd8-bee8-2649f6eb7c13"},"dcVmContributorsRoleAssignmentID": {"value":["184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"]},"hubSubnetVmContAadGroupId": {"value":"57f2ff92-300b-4075-a7ab-2030b46ebe2f"},"hubSubnetVmContRoleAssignmantId": {"value":["0702dcd4-0b65-4ebb-8ebd-873e2729904b","594fd8bf-f554-4272-8b19-9725c7b706b4","b3f5340d-28be-4029-bc10-56af7e20ac75","7a1689a7-66d8-4010-9213-c837316f8a30","d83bc577-1b03-4604-94a1-150ba7198ed0","6cba977a-462f-4d8c-b291-2dad991f85a0"]},"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01","Spoke-Dev-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16","10.3.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["c64ca001-2cce-46de-837e-03f5564fc802/CoreNetwork-02","fac1ea11-e5a7-4e74-8d7e-965344c54f56/CoreNetwork-03","16936380-29b0-4326-8f6b-db86da154736/CoreNetwork-04"]},"spokeSubnetBastionAddressSpace": {"value":["10.1.0.0/26","10.2.0.0/26","10.3.0.0/26"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25","10.3.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24","10.3.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24","10.3.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24","10.3.3.0/24"]},"spokeVmContAadGroupId": {"value":["002984bd-b5ce-445d-8138-d19b514550c7"]},"spokeVmContributorsRoleAssignmentID": {"value":["5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6","b2b76710-60c9-4826-b864-272c7c115806"]}}}</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B3" t="str">
         <f>_xlfn.CONCAT("{",
@@ -2220,19 +2280,19 @@
     </row>
     <row r="4" spans="1:2" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B4" s="10" t="str">
         <f>_xlfn.CONCAT(
 CHAR(34), "networkContributorsAadGroupId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), networkContributorsAadGroupId, CHAR(34), "},",
 CHAR(34), "networkContributorsRoleAssignmentId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", networkContributorsRoleAssignmentId, "]},"
 )</f>
-        <v>"networkContributorsAadGroupId": {"value":"931fbead-2296-4d2b-ac29-da61f92c413b"},"networkContributorsRoleAssignmentId": {"value":["8e5b5f19-21b9-4ed9-b601-799b23a5a1a8","f4c29215-1369-42c2-8e19-055adfaa7bd4","f9370c43-cf0d-42d3-b83d-6f3412e5f5ee"]},</v>
+        <v>"networkContributorsAadGroupId": {"value":"931fbead-2296-4d2b-ac29-da61f92c413b"},"networkContributorsRoleAssignmentId": {"value":["8e5b5f19-21b9-4ed9-b601-799b23a5a1a8","f4c29215-1369-42c2-8e19-055adfaa7bd4","f9370c43-cf0d-42d3-b83d-6f3412e5f5ee","8d7739f2-1859-44c0-a184-b45e84ba363d"]},</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" t="str">
         <f>_xlfn.CONCAT(
@@ -2255,12 +2315,12 @@
 CHAR(34), "hubSubnet4Name", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), hubSubnet4Name, CHAR(34), "},",
 CHAR(34), "hubSubnet4AddressSpace", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), calcHubSubnet4AddressSpace, CHAR(34), "},"
 )</f>
-        <v>"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubDeploySubscriptionResourceGroup": {"value":"f0bb6c48-80fd-445c-98cb-c38b5f817d52/HS-01"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"10.0.0.64/26"},"hubSubnetBastionAddressSpace": {"value":"10.0.0.128/26"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},</v>
+        <v>"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubDeploySubscriptionResourceGroup": {"value":"f0bb6c48-80fd-445c-98cb-c38b5f817d52/CoreNetwork-01"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"10.0.0.64/26"},"hubSubnetBastionAddressSpace": {"value":"10.0.0.128/26"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B6" s="8" t="str">
         <f>_xlfn.CONCAT(
@@ -2274,7 +2334,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7" t="str">
         <f>_xlfn.CONCAT(
@@ -2293,12 +2353,12 @@
 CHAR(34), "spokeVmContAadGroupId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", CHAR(34), appTeamsAadGroupObjectId, CHAR(34), "]},",
 CHAR(34), "spokeVmContributorsRoleAssignmentID", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", spokeVmContributorsRoleAssignmentID,"]}"
 )</f>
-        <v>"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01","Spoke-Dev-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16","10.3.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["f0bb6c48-80fd-445c-98cb-c38b5f817d52/HS-01","c64ca001-2cce-46de-837e-03f5564fc802/HS-02","16936380-29b0-4326-8f6b-db86da154736/HS-03"]},"spokeSubnetBastionAddressSpace": {"value":["10.1.0.0/26","10.2.0.0/26","10.3.0.0/26"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25","10.3.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24","10.3.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24","10.3.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24","10.3.3.0/24"]},"spokeVmContAadGroupId": {"value":["002984bd-b5ce-445d-8138-d19b514550c7"]},"spokeVmContributorsRoleAssignmentID": {"value":["5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6","b2b76710-60c9-4826-b864-272c7c115806"]}</v>
+        <v>"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01","Spoke-Dev-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16","10.3.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["c64ca001-2cce-46de-837e-03f5564fc802/CoreNetwork-02","fac1ea11-e5a7-4e74-8d7e-965344c54f56/CoreNetwork-03","16936380-29b0-4326-8f6b-db86da154736/CoreNetwork-04"]},"spokeSubnetBastionAddressSpace": {"value":["10.1.0.0/26","10.2.0.0/26","10.3.0.0/26"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25","10.3.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24","10.3.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24","10.3.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24","10.3.3.0/24"]},"spokeVmContAadGroupId": {"value":["002984bd-b5ce-445d-8138-d19b514550c7"]},"spokeVmContributorsRoleAssignmentID": {"value":["5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6","b2b76710-60c9-4826-b864-272c7c115806"]}</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B8" t="str">
         <f>_xlfn.CONCAT(
@@ -2309,13 +2369,13 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B11" s="12"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B12" t="str">
         <f>IF(hubSubnetFirewallDeploy = "Deploy", hubSubnetFirewallAddressSpace, "0.0.0.0/0")</f>
@@ -2324,7 +2384,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B13" t="str">
         <f>IF(hubSubnetBastionDeploy = "Deploy", hubSubnetBastionAddressSpace, "0.0.0.0/0")</f>
@@ -2333,7 +2393,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B14" t="str">
         <f>IF(hubSubnetJumpHostsDeploy = "Deploy", hubSubnetJumpHostsAddressSpace, "0.0.0.0/0")</f>
@@ -2342,7 +2402,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B15" t="str">
         <f>IF(hubSubnet1Deploy = "Deploy", hubSubnet1AddressSpace, "0.0.0.0/0")</f>
@@ -2351,7 +2411,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B16" t="str">
         <f>IF(
@@ -2363,7 +2423,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B17" t="str">
         <f>IF(
@@ -2375,7 +2435,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B18" t="str">
         <f>IF(
@@ -2387,12 +2447,12 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="21" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B21" s="7" t="str">
         <f>_xlfn.CONCAT("""", Hub!D18, """", ",", """", Hub!D19, """")</f>
@@ -2401,7 +2461,7 @@
     </row>
     <row r="22" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B22" s="7" t="str">
         <f>_xlfn.CONCAT(
@@ -2419,13 +2479,13 @@
     <row r="24" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B25" s="12"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B26" t="str">
         <f>_xlfn.CONCAT(CHAR(34), Spoke1!$B$5, CHAR(34), ",", CHAR(34), Spoke2!$B$5, CHAR(34), ",", CHAR(34), Spoke3!$B$5, CHAR(34))</f>
@@ -2434,7 +2494,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B27" t="str">
         <f>_xlfn.CONCAT(CHAR(34), Spoke1!$C$5, CHAR(34), ",", CHAR(34), Spoke2!$C$5, CHAR(34), ",", CHAR(34), Spoke3!$C$5, CHAR(34))</f>
@@ -2443,16 +2503,16 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B28" t="str">
-        <f>_xlfn.CONCAT(Spoke1!$D$2, ",", Spoke2!$D$2, ",", Spoke3!$D$2)</f>
-        <v>"f0bb6c48-80fd-445c-98cb-c38b5f817d52/HS-01","c64ca001-2cce-46de-837e-03f5564fc802/HS-02","16936380-29b0-4326-8f6b-db86da154736/HS-03"</v>
+        <f>_xlfn.CONCAT("""", Spoke1!$B$2, """", ",", """", Spoke2!$B$2, """", ",", """", Spoke3!$B$2, """")</f>
+        <v>"c64ca001-2cce-46de-837e-03f5564fc802/CoreNetwork-02","fac1ea11-e5a7-4e74-8d7e-965344c54f56/CoreNetwork-03","16936380-29b0-4326-8f6b-db86da154736/CoreNetwork-04"</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B29" t="str">
         <f>IF(
@@ -2473,7 +2533,7 @@
     </row>
     <row r="30" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B30" s="5" t="str">
         <f>IF(
@@ -2486,7 +2546,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B31" s="3" t="str">
         <f>IF(
@@ -2507,7 +2567,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B32" s="5" t="str">
         <f>IF(
@@ -2520,7 +2580,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B33" s="3" t="str">
         <f>IF(
@@ -2541,7 +2601,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B34" s="5" t="str">
         <f>IF(
@@ -2554,7 +2614,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B35" s="3" t="str">
         <f>IF(
@@ -2575,7 +2635,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B36" s="5" t="str">
         <f>IF(
@@ -2588,7 +2648,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B37" s="3" t="str">
         <f>IF(
@@ -2613,7 +2673,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B38" t="str">
         <f>_xlfn.CONCAT("""",Spoke1!D15,"""",",","""",Spoke2!D15,"""",",","""",Spoke3!D15,"""")</f>
@@ -2622,12 +2682,12 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B41" t="str">
         <f>networkAdmins</f>
@@ -2636,11 +2696,16 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B42" t="str">
-        <f>_xlfn.CONCAT("""", General!B16, """", ",", """", General!B17, """", ",", """", General!B18, """")</f>
-        <v>"8e5b5f19-21b9-4ed9-b601-799b23a5a1a8","f4c29215-1369-42c2-8e19-055adfaa7bd4","f9370c43-cf0d-42d3-b83d-6f3412e5f5ee"</v>
+        <f>_xlfn.CONCAT(
+"""", General!D18, """",
+IF(COUNTIF(deploySubscriptionResourceGroup,"*/*") &gt; 1, "," &amp; """" &amp; General!D19 &amp; """", ""),
+IF(COUNTIF(deploySubscriptionResourceGroup,"*/*") &gt; 2, "," &amp; """" &amp; General!D20 &amp; """", ""),
+IF(COUNTIF(deploySubscriptionResourceGroup,"*/*") &gt; 3, "," &amp; """" &amp; General!D21 &amp; """", "")
+)</f>
+        <v>"8e5b5f19-21b9-4ed9-b601-799b23a5a1a8","f4c29215-1369-42c2-8e19-055adfaa7bd4","f9370c43-cf0d-42d3-b83d-6f3412e5f5ee","8d7739f2-1859-44c0-a184-b45e84ba363d"</v>
       </c>
     </row>
   </sheetData>
@@ -2655,10 +2720,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CC06067-7B7A-4158-B8EE-51370472C64C}">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2668,9 +2733,10 @@
     <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="53.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -2678,248 +2744,267 @@
         <v>31</v>
       </c>
       <c r="E1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G2" t="s">
+        <v>121</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="K2" t="str">
+        <f>IF(General!B18 &lt;&gt; "", _xlfn.CONCAT(General!B18, "/", General!C18), "")</f>
+        <v>f0bb6c48-80fd-445c-98cb-c38b5f817d52/CoreNetwork-01</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" t="s">
         <v>111</v>
       </c>
-      <c r="G1" t="s">
-        <v>121</v>
-      </c>
-      <c r="I1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="G3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="K3" s="11" t="str">
+        <f>IF(General!B19 &lt;&gt; "", _xlfn.CONCAT(General!B19, "/", General!C19), "")</f>
+        <v>c64ca001-2cce-46de-837e-03f5564fc802/CoreNetwork-02</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" t="s">
         <v>108</v>
       </c>
-      <c r="E2" t="s">
-        <v>110</v>
-      </c>
-      <c r="G2" t="s">
-        <v>122</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" t="s">
-        <v>112</v>
-      </c>
-      <c r="G3" t="s">
-        <v>123</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C4" t="s">
-        <v>109</v>
-      </c>
       <c r="I4" s="9" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="K4" s="11" t="str">
+        <f>IF(General!B20 &lt;&gt; "", _xlfn.CONCAT(General!B20, "/", General!C20), "")</f>
+        <v>fac1ea11-e5a7-4e74-8d7e-965344c54f56/CoreNetwork-03</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I5" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="K5" s="11" t="str">
+        <f>IF(General!B21 &lt;&gt; "", _xlfn.CONCAT(General!B21, "/", General!C21), "")</f>
+        <v>16936380-29b0-4326-8f6b-db86da154736/CoreNetwork-04</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I6" s="9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I7" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I8" s="9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I9" s="9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I10" s="9" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I6" s="9" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I7" s="9" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I8" s="9" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I9" s="9" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I10" s="9" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I11" s="9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I12" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I13" s="9" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I14" s="9" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I12" s="9" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I13" s="9" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I14" s="9" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I15" s="9" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I16" s="9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I17" s="9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="18" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I18" s="9" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I19" s="9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I20" s="9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I21" s="9" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="22" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I22" s="9" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I23" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I24" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="25" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I25" s="9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="26" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I26" s="9" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="27" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I27" s="9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="28" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I28" s="9" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I29" s="9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="30" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I30" s="9" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I31" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="32" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I32" s="9" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="33" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I33" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="34" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I34" s="9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="35" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I35" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="36" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I36" s="9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="37" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I37" s="9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="38" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I38" s="9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I39" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="40" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I40" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="41" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I41" s="9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="42" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I42" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added optional tags to resource groups
</commit_message>
<xml_diff>
--- a/PowerShell/ParametersFileBuilder_3-Spoke.xlsx
+++ b/PowerShell/ParametersFileBuilder_3-Spoke.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mark.bakunas\Documents\GitHub\Azure-HubSpoke\PowerShell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A8C47D-EE7A-4EED-A01E-710BF43B6067}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332E0E73-F6DE-48BA-8537-36A1FCFD4D09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="630" windowWidth="21600" windowHeight="14655" xr2:uid="{74A5C2AD-3876-4989-8818-24030CBF60E7}"/>
+    <workbookView xWindow="4020" yWindow="915" windowWidth="21600" windowHeight="14655" xr2:uid="{74A5C2AD-3876-4989-8818-24030CBF60E7}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="4" r:id="rId1"/>
@@ -67,6 +67,7 @@
     <definedName name="networkContributorsRoleAssignmentId">ParametersFile!$B$42</definedName>
     <definedName name="ResourceGroups">Hub:Spoke3!$C$2</definedName>
     <definedName name="resourceGroupsRegion">General!$B$8</definedName>
+    <definedName name="resourceGroupTags">ParametersFile!$B$43</definedName>
     <definedName name="routeTableName">General!$B$7</definedName>
     <definedName name="serverTeamAadGroupObjectId">General!$B$12</definedName>
     <definedName name="spokeDeploySubscriptionResourceGroup">ParametersFile!$B$28</definedName>
@@ -107,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="217">
   <si>
     <t>Name</t>
   </si>
@@ -199,9 +200,6 @@
     <t>DDOS protection level</t>
   </si>
   <si>
-    <t>DDOS plan name</t>
-  </si>
-  <si>
     <t>NSG security level</t>
   </si>
   <si>
@@ -688,9 +686,6 @@
     <t>Resource group RBAC</t>
   </si>
   <si>
-    <t>Tags</t>
-  </si>
-  <si>
     <t>Subscription ID</t>
   </si>
   <si>
@@ -734,13 +729,43 @@
   </si>
   <si>
     <t>Resource Groups (up to 4 in any combination of subscriptions, don't enter more than are used)</t>
+  </si>
+  <si>
+    <t>"AppTaxonomy": "IT/Network","EnvironmentType": "Production"</t>
+  </si>
+  <si>
+    <t>"AppTaxonomy": "IT/Network","EnvironmentType": "Development"</t>
+  </si>
+  <si>
+    <t>"AppTaxonomy": "IT/Network","EnvironmentType": "Test"</t>
+  </si>
+  <si>
+    <t>resourceGroupTags</t>
+  </si>
+  <si>
+    <t>Blue = Data from another source (Subscription IDs, Azure AD group IDs, etc.)</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Tags (optional, leave blank for no tags)</t>
+  </si>
+  <si>
+    <t>DDOS plan name (or ID)</t>
+  </si>
+  <si>
+    <t>Green = Created items (names, address spaces, GUIDs, etc.)</t>
+  </si>
+  <si>
+    <t>Purple = Options (deploy/don't deploy, common/unique, etc.)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -754,16 +779,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -788,6 +805,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD8BEEC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -798,14 +821,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -817,18 +837,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFE2CFF1"/>
+      <color rgb="FFD8BEEC"/>
+      <color rgb="FFCDACE6"/>
       <color rgb="FFF9D7F7"/>
       <color rgb="FFF3A9EE"/>
     </mruColors>
@@ -1141,7 +1201,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27806494-5F45-4C9A-ADBE-3476E1448E75}">
-  <dimension ref="A2:D21"/>
+  <dimension ref="A2:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -1151,165 +1211,199 @@
   <cols>
     <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="78.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>214</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="13" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="1" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>127</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="10" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>125</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>183</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>193</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C17" t="s">
         <v>194</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="D17" t="s">
+      <c r="C20" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>198</v>
+      <c r="D21" s="11" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="11" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="10" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="13" t="s">
+        <v>216</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A16:D16"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
@@ -1347,22 +1441,22 @@
     <col min="4" max="5" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C1" s="12"/>
     </row>
-    <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="C2" s="13"/>
-    </row>
-    <row r="3" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="C2" s="14"/>
+    </row>
+    <row r="3" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
@@ -1375,22 +1469,22 @@
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
+    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="11" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1398,32 +1492,32 @@
       <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>109</v>
+      <c r="D8" s="13" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>109</v>
+      <c r="D9" s="13" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="11" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1431,115 +1525,115 @@
       <c r="A11" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>109</v>
+      <c r="D11" s="13" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>109</v>
+      <c r="D12" s="13" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>109</v>
+      <c r="D13" s="13" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>109</v>
+      <c r="D14" s="13" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>109</v>
+      <c r="D15" s="13" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" t="s">
         <v>43</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B18" t="s">
         <v>44</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>51</v>
       </c>
-      <c r="D17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="B18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="D18" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B19" t="s">
         <v>52</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E18" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="B19" t="s">
-        <v>53</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="14" t="s">
-        <v>50</v>
+      <c r="D19" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="E19" t="str">
         <f>IF(dcAdminsAadGroupObjectId = "", "Not needed", "Required")</f>
@@ -1547,17 +1641,17 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>130</v>
+      <c r="A20" s="5" t="s">
+        <v>129</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C20" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="14" t="s">
-        <v>54</v>
+      <c r="D20" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="E20" t="str">
         <f>IF(hubSubnetJumpHostsDeploy = "Deploy", "Required", "Not Needed")</f>
@@ -1565,37 +1659,37 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>130</v>
+      <c r="A21" s="5" t="s">
+        <v>129</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="E21" s="7" t="str">
+      <c r="D21" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="5" t="str">
         <f>IF(hubSubnet1Deploy = "Don't Deploy", "Not Needed", "Required")</f>
         <v>Required</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>130</v>
+      <c r="A22" s="5" t="s">
+        <v>129</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="E22" s="7" t="str">
+      <c r="D22" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="5" t="str">
         <f>IF(
 OR(hubSubnet1Deploy = "Don't Deploy", hubSubnet2Deploy = "Don't Deploy"),
 "Not Needed", "Required")</f>
@@ -1603,19 +1697,19 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>130</v>
+      <c r="A23" s="5" t="s">
+        <v>129</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C23" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="E23" s="7" t="str">
+      <c r="D23" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="5" t="str">
         <f>IF(
 OR(hubSubnet1Deploy = "Don't Deploy", hubSubnet2Deploy = "Don't Deploy", hubSubnet3Deploy = "Don't Deploy"),
 "Not Needed", "Required")</f>
@@ -1623,19 +1717,19 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>130</v>
+      <c r="A24" s="5" t="s">
+        <v>129</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C24" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="E24" s="7" t="str">
+      <c r="D24" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" s="5" t="str">
         <f>IF(
 OR(hubSubnet1Deploy = "Don't Deploy", hubSubnet2Deploy = "Don't Deploy", hubSubnet3Deploy = "Don't Deploy", hubSubnet4Deploy = "Don't Deploy"),
 "Not Needed", "Required")</f>
@@ -1643,20 +1737,20 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>130</v>
+      <c r="A25" s="5" t="s">
+        <v>129</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="14" t="s">
-        <v>94</v>
+      <c r="D25" s="11" t="s">
+        <v>93</v>
       </c>
       <c r="E25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1665,6 +1759,11 @@
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="D20:D24">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>IF($E20 = "Required", 1)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:D9 D11:D15" xr:uid="{D9354EF7-27D1-4C1F-B57B-07A789DEC96E}">
       <formula1>deployOptions_List</formula1>
@@ -1696,18 +1795,18 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="C2" s="13"/>
+        <v>40</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="C2" s="14"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -1721,127 +1820,127 @@
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
+    </row>
+    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>122</v>
+      <c r="C7" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>122</v>
+      <c r="C8" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>122</v>
+      <c r="C9" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>122</v>
+      <c r="C10" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>122</v>
+      <c r="C11" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
         <v>43</v>
       </c>
-      <c r="B13" t="s">
-        <v>44</v>
-      </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" s="4" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D15" s="6" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1883,18 +1982,18 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="C2" s="13"/>
+        <v>40</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="C2" s="14"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -1908,26 +2007,26 @@
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
+    </row>
+    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>111</v>
+      <c r="C7" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>110</v>
       </c>
       <c r="E7" t="str">
         <f>Spoke1!E7</f>
@@ -1936,16 +2035,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>109</v>
+      <c r="C8" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>108</v>
       </c>
       <c r="E8" t="str">
         <f>Spoke1!E8</f>
@@ -1956,11 +2055,11 @@
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>74</v>
+      <c r="C9" s="11" t="s">
+        <v>73</v>
       </c>
       <c r="E9" t="str">
         <f>Spoke1!E9</f>
@@ -1971,14 +2070,14 @@
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>109</v>
+      <c r="C10" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>108</v>
       </c>
       <c r="E10" t="str">
         <f>Spoke1!E10</f>
@@ -1989,14 +2088,14 @@
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>109</v>
+      <c r="C11" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>108</v>
       </c>
       <c r="E11" t="str">
         <f>Spoke1!E11</f>
@@ -2005,35 +2104,35 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
         <v>43</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B14" t="s">
         <v>44</v>
-      </c>
-      <c r="C13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="B14" t="s">
-        <v>45</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" s="4" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D15" s="6" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2072,18 +2171,18 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>207</v>
-      </c>
-      <c r="C2" s="13"/>
+        <v>40</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="C2" s="14"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -2097,26 +2196,26 @@
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
+    </row>
+    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>111</v>
+      <c r="C7" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>110</v>
       </c>
       <c r="E7" t="str">
         <f>Spoke1!E7</f>
@@ -2125,16 +2224,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>109</v>
+      <c r="C8" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>108</v>
       </c>
       <c r="E8" t="str">
         <f>Spoke1!E8</f>
@@ -2145,11 +2244,11 @@
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>102</v>
+      <c r="C9" s="11" t="s">
+        <v>101</v>
       </c>
       <c r="E9" t="str">
         <f>Spoke1!E9</f>
@@ -2160,14 +2259,14 @@
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>109</v>
+      <c r="C10" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>108</v>
       </c>
       <c r="E10" t="str">
         <f>Spoke1!E10</f>
@@ -2178,14 +2277,14 @@
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>109</v>
+      <c r="C11" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>108</v>
       </c>
       <c r="E11" t="str">
         <f>Spoke1!E11</f>
@@ -2194,35 +2293,35 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
         <v>43</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B14" t="s">
         <v>44</v>
-      </c>
-      <c r="C13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="B14" t="s">
-        <v>45</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" s="4" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D15" s="6" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2245,7 +2344,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E5F0421-4CC3-4847-AE8E-9E8CD1C6E8C6}">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -2259,16 +2358,16 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" s="4" t="str">
+        <v>67</v>
+      </c>
+      <c r="B1" s="2" t="str">
         <f>_xlfn.CONCAT(B3, ",", B4, B5, B6, ",", B7,  B8)</f>
-        <v>{"$schema":"https://schema.management.azure.com/schemas/2019-04-01/deploymentParameters.json#","contentVersion":"1.0.0.0","parameters":{"assetLocationURI": {"value":"https://raw.githubusercontent.com/mbakunas/Azure-HubSpoke/master/"},"resourceGroupsRegion": {"value":"East US 2"},"vnetDdosProtectionLevel": {"value":"Standard - Create New"},"vnetDdosProtectionPlanName": {"value":"DDOS-Plan-01"},"vnetNsgSecurityLevel": {"value":"Medium"},"routeTableName": {"value":"RouteTable-EastUS2-01"},"networkContributorsAadGroupId": {"value":"931fbead-2296-4d2b-ac29-da61f92c413b"},"networkContributorsRoleAssignmentId": {"value":["8e5b5f19-21b9-4ed9-b601-799b23a5a1a8","f4c29215-1369-42c2-8e19-055adfaa7bd4","f9370c43-cf0d-42d3-b83d-6f3412e5f5ee","8d7739f2-1859-44c0-a184-b45e84ba363d"]},"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubDeploySubscriptionResourceGroup": {"value":"f0bb6c48-80fd-445c-98cb-c38b5f817d52/CoreNetwork-01"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"10.0.0.64/26"},"hubSubnetBastionAddressSpace": {"value":"10.0.0.128/26"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},"dcSubnetVmContAadGroupId": {"value":"83578c91-9919-4bd8-bee8-2649f6eb7c13"},"dcVmContributorsRoleAssignmentID": {"value":["184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"]},"hubSubnetVmContAadGroupId": {"value":"57f2ff92-300b-4075-a7ab-2030b46ebe2f"},"hubSubnetVmContRoleAssignmantId": {"value":["0702dcd4-0b65-4ebb-8ebd-873e2729904b","594fd8bf-f554-4272-8b19-9725c7b706b4","b3f5340d-28be-4029-bc10-56af7e20ac75","7a1689a7-66d8-4010-9213-c837316f8a30","d83bc577-1b03-4604-94a1-150ba7198ed0","6cba977a-462f-4d8c-b291-2dad991f85a0"]},"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01","Spoke-Dev-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16","10.3.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["c64ca001-2cce-46de-837e-03f5564fc802/CoreNetwork-02","fac1ea11-e5a7-4e74-8d7e-965344c54f56/CoreNetwork-03","16936380-29b0-4326-8f6b-db86da154736/CoreNetwork-04"]},"spokeSubnetBastionAddressSpace": {"value":["10.1.0.0/26","10.2.0.0/26","10.3.0.0/26"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25","10.3.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24","10.3.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24","10.3.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24","10.3.3.0/24"]},"spokeVmContAadGroupId": {"value":["002984bd-b5ce-445d-8138-d19b514550c7"]},"spokeVmContributorsRoleAssignmentID": {"value":["5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6","b2b76710-60c9-4826-b864-272c7c115806"]}}}</v>
+        <v>{"$schema":"https://schema.management.azure.com/schemas/2019-04-01/deploymentParameters.json#","contentVersion":"1.0.0.0","parameters":{"assetLocationURI": {"value":"https://raw.githubusercontent.com/mbakunas/Azure-HubSpoke/master/"},"resourceGroupsRegion": {"value":"East US 2"},"vnetDdosProtectionLevel": {"value":"Standard - Create New"},"vnetDdosProtectionPlanName": {"value":"DDOS-Plan-01"},"vnetNsgSecurityLevel": {"value":"Medium"},"routeTableName": {"value":"RouteTable-EastUS2-01"},"networkContributorsAadGroupId": {"value":"931fbead-2296-4d2b-ac29-da61f92c413b"},"networkContributorsRoleAssignmentId": {"value":["8e5b5f19-21b9-4ed9-b601-799b23a5a1a8","f4c29215-1369-42c2-8e19-055adfaa7bd4","f9370c43-cf0d-42d3-b83d-6f3412e5f5ee","8d7739f2-1859-44c0-a184-b45e84ba363d"]},"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubDeploySubscriptionResourceGroup": {"value":"f0bb6c48-80fd-445c-98cb-c38b5f817d52/CoreNetwork-01"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"10.0.0.64/26"},"hubSubnetBastionAddressSpace": {"value":"10.0.0.128/26"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},"dcSubnetVmContAadGroupId": {"value":"83578c91-9919-4bd8-bee8-2649f6eb7c13"},"dcVmContributorsRoleAssignmentID": {"value":["184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"]},"hubSubnetVmContAadGroupId": {"value":"57f2ff92-300b-4075-a7ab-2030b46ebe2f"},"hubSubnetVmContRoleAssignmantId": {"value":["0702dcd4-0b65-4ebb-8ebd-873e2729904b","594fd8bf-f554-4272-8b19-9725c7b706b4","b3f5340d-28be-4029-bc10-56af7e20ac75","7a1689a7-66d8-4010-9213-c837316f8a30","d83bc577-1b03-4604-94a1-150ba7198ed0","6cba977a-462f-4d8c-b291-2dad991f85a0"]},"resourceGroupTags": {"value":{"CoreNetwork-01":{"AppTaxonomy": "IT/Network","EnvironmentType": "Production"},"CoreNetwork-02":{"AppTaxonomy": "IT/Network","EnvironmentType": "Production"},"CoreNetwork-03":{"AppTaxonomy": "IT/Network","EnvironmentType": "Test"},"CoreNetwork-04":{"AppTaxonomy": "IT/Network","EnvironmentType": "Development"}}},"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01","Spoke-Dev-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16","10.3.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["c64ca001-2cce-46de-837e-03f5564fc802/CoreNetwork-02","fac1ea11-e5a7-4e74-8d7e-965344c54f56/CoreNetwork-03","16936380-29b0-4326-8f6b-db86da154736/CoreNetwork-04"]},"spokeSubnetBastionAddressSpace": {"value":["10.1.0.0/26","10.2.0.0/26","10.3.0.0/26"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25","10.3.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24","10.3.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24","10.3.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24","10.3.3.0/24"]},"spokeVmContAadGroupId": {"value":["002984bd-b5ce-445d-8138-d19b514550c7"]},"spokeVmContributorsRoleAssignmentID": {"value":["5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6","b2b76710-60c9-4826-b864-272c7c115806"]}}}</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" t="str">
         <f>_xlfn.CONCAT("{",
@@ -2285,11 +2384,11 @@
         <v>{"$schema":"https://schema.management.azure.com/schemas/2019-04-01/deploymentParameters.json#","contentVersion":"1.0.0.0","parameters":{"assetLocationURI": {"value":"https://raw.githubusercontent.com/mbakunas/Azure-HubSpoke/master/"},"resourceGroupsRegion": {"value":"East US 2"},"vnetDdosProtectionLevel": {"value":"Standard - Create New"},"vnetDdosProtectionPlanName": {"value":"DDOS-Plan-01"},"vnetNsgSecurityLevel": {"value":"Medium"},"routeTableName": {"value":"RouteTable-EastUS2-01"}</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="B4" s="10" t="str">
+    <row r="4" spans="1:2" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="B4" s="8" t="str">
         <f>_xlfn.CONCAT(
 CHAR(34), "networkContributorsAadGroupId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), networkContributorsAadGroupId, CHAR(34), "},",
 CHAR(34), "networkContributorsRoleAssignmentId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", networkContributorsRoleAssignmentId, "]},"
@@ -2299,7 +2398,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" t="str">
         <f>_xlfn.CONCAT(
@@ -2325,23 +2424,24 @@
         <v>"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubDeploySubscriptionResourceGroup": {"value":"f0bb6c48-80fd-445c-98cb-c38b5f817d52/CoreNetwork-01"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"10.0.0.64/26"},"hubSubnetBastionAddressSpace": {"value":"10.0.0.128/26"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="B6" s="8" t="str">
+    <row r="6" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B6" s="6" t="str">
         <f>_xlfn.CONCAT(
 CHAR(34), "dcSubnetVmContAadGroupId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), dcAdminsAadGroupObjectId, CHAR(34), "},",
 CHAR(34), "dcVmContributorsRoleAssignmentID", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", dcVmContributorsRoleAssignmentID, "]},",
 CHAR(34), "hubSubnetVmContAadGroupId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), serverTeamAadGroupObjectId, CHAR(34), "},",
-CHAR(34), "hubSubnetVmContRoleAssignmantId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", hubSubnetVmContRoleAssignmantId, "]}"
+CHAR(34), "hubSubnetVmContRoleAssignmantId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", hubSubnetVmContRoleAssignmantId, "]},",
+CHAR(34), "resourceGroupTags", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "{", resourceGroupTags, "}}"
 )</f>
-        <v>"dcSubnetVmContAadGroupId": {"value":"83578c91-9919-4bd8-bee8-2649f6eb7c13"},"dcVmContributorsRoleAssignmentID": {"value":["184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"]},"hubSubnetVmContAadGroupId": {"value":"57f2ff92-300b-4075-a7ab-2030b46ebe2f"},"hubSubnetVmContRoleAssignmantId": {"value":["0702dcd4-0b65-4ebb-8ebd-873e2729904b","594fd8bf-f554-4272-8b19-9725c7b706b4","b3f5340d-28be-4029-bc10-56af7e20ac75","7a1689a7-66d8-4010-9213-c837316f8a30","d83bc577-1b03-4604-94a1-150ba7198ed0","6cba977a-462f-4d8c-b291-2dad991f85a0"]}</v>
+        <v>"dcSubnetVmContAadGroupId": {"value":"83578c91-9919-4bd8-bee8-2649f6eb7c13"},"dcVmContributorsRoleAssignmentID": {"value":["184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"]},"hubSubnetVmContAadGroupId": {"value":"57f2ff92-300b-4075-a7ab-2030b46ebe2f"},"hubSubnetVmContRoleAssignmantId": {"value":["0702dcd4-0b65-4ebb-8ebd-873e2729904b","594fd8bf-f554-4272-8b19-9725c7b706b4","b3f5340d-28be-4029-bc10-56af7e20ac75","7a1689a7-66d8-4010-9213-c837316f8a30","d83bc577-1b03-4604-94a1-150ba7198ed0","6cba977a-462f-4d8c-b291-2dad991f85a0"]},"resourceGroupTags": {"value":{"CoreNetwork-01":{"AppTaxonomy": "IT/Network","EnvironmentType": "Production"},"CoreNetwork-02":{"AppTaxonomy": "IT/Network","EnvironmentType": "Production"},"CoreNetwork-03":{"AppTaxonomy": "IT/Network","EnvironmentType": "Test"},"CoreNetwork-04":{"AppTaxonomy": "IT/Network","EnvironmentType": "Development"}}}</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" t="str">
         <f>_xlfn.CONCAT(
@@ -2365,7 +2465,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B8" t="str">
         <f>_xlfn.CONCAT(
@@ -2376,13 +2476,13 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B11" s="12"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B12" t="str">
         <f>IF(hubSubnetFirewallDeploy = "Deploy", hubSubnetFirewallAddressSpace, "0.0.0.0/0")</f>
@@ -2391,7 +2491,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B13" t="str">
         <f>IF(hubSubnetBastionDeploy = "Deploy", hubSubnetBastionAddressSpace, "0.0.0.0/0")</f>
@@ -2400,7 +2500,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B14" t="str">
         <f>IF(hubSubnetJumpHostsDeploy = "Deploy", hubSubnetJumpHostsAddressSpace, "0.0.0.0/0")</f>
@@ -2409,7 +2509,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B15" t="str">
         <f>IF(hubSubnet1Deploy = "Deploy", hubSubnet1AddressSpace, "0.0.0.0/0")</f>
@@ -2418,7 +2518,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B16" t="str">
         <f>IF(
@@ -2430,7 +2530,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B17" t="str">
         <f>IF(
@@ -2442,7 +2542,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B18" t="str">
         <f>IF(
@@ -2454,23 +2554,23 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B21" s="7" t="str">
+    </row>
+    <row r="21" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B21" s="5" t="str">
         <f>_xlfn.CONCAT("""", Hub!D18, """", ",", """", Hub!D19, """")</f>
         <v>"184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"</v>
       </c>
     </row>
-    <row r="22" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="B22" s="7" t="str">
+    <row r="22" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B22" s="5" t="str">
         <f>_xlfn.CONCAT(
 """", Hub!D25, """",
 IF(Hub!E20 = "Required", "," &amp; """" &amp; Hub!D20 &amp; """", ""),
@@ -2482,17 +2582,17 @@
         <v>"0702dcd4-0b65-4ebb-8ebd-873e2729904b","594fd8bf-f554-4272-8b19-9725c7b706b4","b3f5340d-28be-4029-bc10-56af7e20ac75","7a1689a7-66d8-4010-9213-c837316f8a30","d83bc577-1b03-4604-94a1-150ba7198ed0","6cba977a-462f-4d8c-b291-2dad991f85a0"</v>
       </c>
     </row>
-    <row r="23" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B25" s="12"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" t="str">
         <f>_xlfn.CONCAT(CHAR(34), Spoke1!$B$5, CHAR(34), ",", CHAR(34), Spoke2!$B$5, CHAR(34), ",", CHAR(34), Spoke3!$B$5, CHAR(34))</f>
@@ -2501,7 +2601,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B27" t="str">
         <f>_xlfn.CONCAT(CHAR(34), Spoke1!$C$5, CHAR(34), ",", CHAR(34), Spoke2!$C$5, CHAR(34), ",", CHAR(34), Spoke3!$C$5, CHAR(34))</f>
@@ -2510,7 +2610,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B28" t="str">
         <f>_xlfn.CONCAT("""", Spoke1!$B$2, """", ",", """", Spoke2!$B$2, """", ",", """", Spoke3!$B$2, """")</f>
@@ -2519,7 +2619,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B29" t="str">
         <f>IF(
@@ -2540,9 +2640,9 @@
     </row>
     <row r="30" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>83</v>
-      </c>
-      <c r="B30" s="5" t="str">
+        <v>82</v>
+      </c>
+      <c r="B30" s="3" t="str">
         <f>IF(
 Spoke1!$E$8 = "Common",
 """" &amp; Spoke1!$B$8 &amp; """",
@@ -2553,9 +2653,9 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>84</v>
-      </c>
-      <c r="B31" s="3" t="str">
+        <v>83</v>
+      </c>
+      <c r="B31" s="1" t="str">
         <f>IF(
 Spoke1!$E$8 = "Common",
 IF(Spoke1!$D$8 = "Don't Deploy", """"  &amp; "0.0.0.0/0" &amp; """", """" &amp;  Spoke1!$C$8 &amp; """" &amp; "," &amp;   """" &amp; Spoke2!$C$8  &amp; """" &amp; "," &amp;   """" &amp; Spoke3!$C$8 &amp; """"),
@@ -2574,9 +2674,9 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>87</v>
-      </c>
-      <c r="B32" s="5" t="str">
+        <v>86</v>
+      </c>
+      <c r="B32" s="3" t="str">
         <f>IF(
 Spoke1!$E$8 = "Common",
 """" &amp; Spoke1!$B$9 &amp; """",
@@ -2587,9 +2687,9 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>88</v>
-      </c>
-      <c r="B33" s="3" t="str">
+        <v>87</v>
+      </c>
+      <c r="B33" s="1" t="str">
         <f>IF(
 Spoke1!$E$9 = "Common",
 IF(Spoke1!$D$9 = "Don't Deploy", """"  &amp; "0.0.0.0/0" &amp; """", """" &amp;  Spoke1!$C$9 &amp; """" &amp; "," &amp;   """" &amp; Spoke2!$C$9  &amp; """" &amp; "," &amp;   """" &amp; Spoke3!$C$9 &amp; """"),
@@ -2608,9 +2708,9 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>89</v>
-      </c>
-      <c r="B34" s="5" t="str">
+        <v>88</v>
+      </c>
+      <c r="B34" s="3" t="str">
         <f>IF(
 Spoke1!$E$10 = "Common",
 """" &amp; Spoke1!$B$10 &amp; """",
@@ -2621,9 +2721,9 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>90</v>
-      </c>
-      <c r="B35" s="3" t="str">
+        <v>89</v>
+      </c>
+      <c r="B35" s="1" t="str">
         <f>IF(
 Spoke1!$E$10 = "Common",
 IF(Spoke1!$D$10 = "Don't Deploy", """"  &amp; "0.0.0.0/0" &amp; """", """" &amp;  Spoke1!$C$10 &amp; """" &amp; "," &amp;   """" &amp; Spoke2!$C$10  &amp; """" &amp; "," &amp;   """" &amp; Spoke3!$C$10 &amp; """"),
@@ -2642,9 +2742,9 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>91</v>
-      </c>
-      <c r="B36" s="5" t="str">
+        <v>90</v>
+      </c>
+      <c r="B36" s="3" t="str">
         <f>IF(
 Spoke1!$E$8 = "Common",
 """" &amp; Spoke1!$B$11 &amp; """",
@@ -2655,9 +2755,9 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>92</v>
-      </c>
-      <c r="B37" s="3" t="str">
+        <v>91</v>
+      </c>
+      <c r="B37" s="1" t="str">
         <f>IF(
 Spoke1!$E$11 = "Common",
 IF(OR(Spoke1!$D$11 = "Don't Deploy", Spoke1!$D$10 = "Don't Deploy"),
@@ -2680,7 +2780,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B38" t="str">
         <f>_xlfn.CONCAT("""",Spoke1!D15,"""",",","""",Spoke2!D15,"""",",","""",Spoke3!D15,"""")</f>
@@ -2689,12 +2789,12 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
         <v>190</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="10" t="s">
-        <v>191</v>
       </c>
       <c r="B41" t="str">
         <f>networkAdmins</f>
@@ -2703,16 +2803,34 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B42" t="str">
         <f>_xlfn.CONCAT(
-"""", General!D18, """",
-IF(COUNTIF(deploySubscriptionResourceGroup,"*/*") &gt; 1, "," &amp; """" &amp; General!D19 &amp; """", ""),
-IF(COUNTIF(deploySubscriptionResourceGroup,"*/*") &gt; 2, "," &amp; """" &amp; General!D20 &amp; """", ""),
-IF(COUNTIF(deploySubscriptionResourceGroup,"*/*") &gt; 3, "," &amp; """" &amp; General!D21 &amp; """", "")
+"""", General!C18, """",
+IF(COUNTIF(deploySubscriptionResourceGroup,"*/*") &gt; 1, "," &amp; """" &amp; General!C19 &amp; """", ""),
+IF(COUNTIF(deploySubscriptionResourceGroup,"*/*") &gt; 2, "," &amp; """" &amp; General!C20 &amp; """", ""),
+IF(COUNTIF(deploySubscriptionResourceGroup,"*/*") &gt; 3, "," &amp; """" &amp; General!C21 &amp; """", "")
 )</f>
         <v>"8e5b5f19-21b9-4ed9-b601-799b23a5a1a8","f4c29215-1369-42c2-8e19-055adfaa7bd4","f9370c43-cf0d-42d3-b83d-6f3412e5f5ee","8d7739f2-1859-44c0-a184-b45e84ba363d"</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>210</v>
+      </c>
+      <c r="B43" t="str">
+        <f>IF(
+AND(General!D18 &lt;&gt; "", General!D19 &lt;&gt; "", General!D20 &lt;&gt; "", General!D21 &lt;&gt; ""),
+_xlfn.CONCAT(
+"""", General!A18, """", ":{", General!D18, "},",
+"""", General!A19, """", ":{", General!D19, "},",
+"""", General!A20, """", ":{", General!D20, "},",
+"""", General!A21, """", ":{", General!D21, "}"
+),
+""
+)</f>
+        <v>"CoreNetwork-01":{"AppTaxonomy": "IT/Network","EnvironmentType": "Production"},"CoreNetwork-02":{"AppTaxonomy": "IT/Network","EnvironmentType": "Production"},"CoreNetwork-03":{"AppTaxonomy": "IT/Network","EnvironmentType": "Test"},"CoreNetwork-04":{"AppTaxonomy": "IT/Network","EnvironmentType": "Development"}</v>
       </c>
     </row>
   </sheetData>
@@ -2730,7 +2848,7 @@
   <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2748,270 +2866,270 @@
         <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G2" t="s">
-        <v>121</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>171</v>
+        <v>120</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="K2" t="str">
-        <f>IF(General!B18 &lt;&gt; "", _xlfn.CONCAT(General!B18, "/", General!C18), "")</f>
+        <f>IF(General!B18 &lt;&gt; "", _xlfn.CONCAT(General!B18, "/", General!A18), "")</f>
         <v>f0bb6c48-80fd-445c-98cb-c38b5f817d52/CoreNetwork-01</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G3" t="s">
-        <v>122</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="K3" s="11" t="str">
-        <f>IF(General!B19 &lt;&gt; "", _xlfn.CONCAT(General!B19, "/", General!C19), "")</f>
+        <v>121</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="K3" s="9" t="str">
+        <f>IF(General!B19 &lt;&gt; "", _xlfn.CONCAT(General!B19, "/", General!A19), "")</f>
         <v>c64ca001-2cce-46de-837e-03f5564fc802/CoreNetwork-02</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C4" t="s">
-        <v>108</v>
-      </c>
-      <c r="I4" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="K4" s="9" t="str">
+        <f>IF(General!B20 &lt;&gt; "", _xlfn.CONCAT(General!B20, "/", General!A20), "")</f>
+        <v>fac1ea11-e5a7-4e74-8d7e-965344c54f56/CoreNetwork-03</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I5" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="K4" s="11" t="str">
-        <f>IF(General!B20 &lt;&gt; "", _xlfn.CONCAT(General!B20, "/", General!C20), "")</f>
-        <v>fac1ea11-e5a7-4e74-8d7e-965344c54f56/CoreNetwork-03</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I5" s="9" t="s">
+      <c r="K5" s="9" t="str">
+        <f>IF(General!B21 &lt;&gt; "", _xlfn.CONCAT(General!B21, "/", General!A21), "")</f>
+        <v>16936380-29b0-4326-8f6b-db86da154736/CoreNetwork-04</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I6" s="7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I7" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I8" s="7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I9" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I10" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I11" s="7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I12" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I13" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I14" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I15" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I16" s="7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I17" s="7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="18" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I18" s="7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="19" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I19" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="20" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I20" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I21" s="7" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="22" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I22" s="7" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="23" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I23" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="24" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I24" s="7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I25" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="26" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I26" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="27" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I27" s="7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="28" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I28" s="7" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="29" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I29" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="30" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I30" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="K5" s="11" t="str">
-        <f>IF(General!B21 &lt;&gt; "", _xlfn.CONCAT(General!B21, "/", General!C21), "")</f>
-        <v>16936380-29b0-4326-8f6b-db86da154736/CoreNetwork-04</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I6" s="9" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I7" s="9" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I8" s="9" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I9" s="9" t="s">
+    </row>
+    <row r="31" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I31" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="32" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I32" s="7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I33" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="34" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I34" s="7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="35" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I35" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="36" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I36" s="7" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I10" s="9" t="s">
+    <row r="37" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I37" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="38" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I38" s="7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="39" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I39" s="7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="40" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I40" s="7" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I11" s="9" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I12" s="9" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I13" s="9" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I14" s="9" t="s">
+    <row r="41" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I41" s="7" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I15" s="9" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I16" s="9" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I17" s="9" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I18" s="9" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I19" s="9" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="20" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I20" s="9" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="21" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I21" s="9" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="22" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I22" s="9" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="23" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I23" s="9" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="24" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I24" s="9" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="25" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I25" s="9" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="26" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I26" s="9" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="27" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I27" s="9" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="28" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I28" s="9" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="29" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I29" s="9" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="30" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I30" s="9" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="31" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I31" s="9" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="32" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I32" s="9" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="33" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I33" s="9" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="34" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I34" s="9" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="35" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I35" s="9" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="36" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I36" s="9" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="37" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I37" s="9" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="38" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I38" s="9" t="s">
+    <row r="42" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I42" s="7" t="s">
         <v>165</v>
-      </c>
-    </row>
-    <row r="39" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I39" s="9" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="40" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I40" s="9" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="41" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I41" s="9" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="42" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I42" s="9" t="s">
-        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>